<commit_message>
Daily-Crawler / Changed to absolute path
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="台指期換倉成本計算" sheetId="1" state="visible" r:id="rId1"/>
@@ -400,13 +400,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="18.375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -451,7 +451,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,150 +460,199 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16919</v>
+        <v>17020</v>
       </c>
       <c r="D2" t="n">
-        <v>8144</v>
+        <v>8647</v>
       </c>
       <c r="E2" t="n">
-        <v>10016048</v>
+        <v>5905940</v>
       </c>
       <c r="F2" t="n">
-        <v>16823</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>202112</v>
+          <t>日期：2021/11/01</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>17010</v>
+        <v>17053</v>
       </c>
       <c r="D3" t="n">
-        <v>7552</v>
+        <v>8300</v>
       </c>
       <c r="E3" t="n">
-        <v>5239080</v>
+        <v>2660268</v>
       </c>
       <c r="F3" t="n">
-        <v>16816</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>17038</v>
+        <v>16919</v>
       </c>
       <c r="D4" t="n">
-        <v>7244</v>
+        <v>8144</v>
       </c>
       <c r="E4" t="n">
-        <v>3799474</v>
+        <v>10016048</v>
       </c>
       <c r="F4" t="n">
-        <v>16808</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>202112</v>
       </c>
       <c r="C5" t="n">
-        <v>17014</v>
+        <v>17010</v>
       </c>
       <c r="D5" t="n">
-        <v>7021</v>
+        <v>7552</v>
       </c>
       <c r="E5" t="n">
-        <v>4968088</v>
+        <v>5239080</v>
       </c>
       <c r="F5" t="n">
-        <v>16800</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>202112</v>
       </c>
       <c r="C6" t="n">
-        <v>16864</v>
+        <v>17038</v>
       </c>
       <c r="D6" t="n">
-        <v>6729</v>
+        <v>7244</v>
       </c>
       <c r="E6" t="n">
-        <v>4401504</v>
+        <v>3799474</v>
       </c>
       <c r="F6" t="n">
-        <v>16791</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>202112</v>
       </c>
       <c r="C7" t="n">
-        <v>16828</v>
+        <v>17014</v>
       </c>
       <c r="D7" t="n">
-        <v>6468</v>
+        <v>7021</v>
       </c>
       <c r="E7" t="n">
-        <v>3449740</v>
+        <v>4968088</v>
       </c>
       <c r="F7" t="n">
-        <v>16788</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>202112</v>
       </c>
       <c r="C8" t="n">
+        <v>16864</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6729</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4401504</v>
+      </c>
+      <c r="F8" t="n">
+        <v>16791</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>日期：2021/10/22</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C10" t="n">
         <v>16789</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D10" t="n">
         <v>6263</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E10" t="n">
         <v>105139507</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F10" t="n">
         <v>16789</v>
       </c>
     </row>
+    <row r="11"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -616,13 +665,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="19.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -643,30 +692,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B6" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -681,13 +750,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="17.125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.375" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -713,39 +782,65 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-115.21</v>
+        <v>19.71</v>
       </c>
       <c r="C2" t="n">
-        <v>60.99</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-73.59</v>
+        <v>-31.96</v>
       </c>
       <c r="C3" t="n">
-        <v>40.67</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-115.21</v>
+      </c>
+      <c r="C4" t="n">
+        <v>60.99</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C5" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B6" t="n">
         <v>24.64</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C6" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -760,13 +855,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.75" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -787,20 +882,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16983.35</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>110年11月01日</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>17080.39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B5" t="n">
         <v>17054.47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily-Crawler / Issue Fixed
週三小台週合約, 未沖銷契約量, 抓取錯誤
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="台指期換倉成本計算" sheetId="1" state="visible" r:id="rId1"/>
@@ -400,13 +400,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18.375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -676,7 +676,6 @@
         <v>16789</v>
       </c>
     </row>
-    <row r="12"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -691,11 +690,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -720,7 +719,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.74</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3">
@@ -790,7 +789,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17.125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.375" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -908,7 +907,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.75" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>

</xml_diff>

<commit_message>
2021/11/08 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -402,7 +402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,22 +462,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17046</v>
+        <v>17395</v>
       </c>
       <c r="D2" t="n">
-        <v>9084</v>
+        <v>9997</v>
       </c>
       <c r="E2" t="n">
-        <v>7057044</v>
+        <v>11741625</v>
       </c>
       <c r="F2" t="n">
-        <v>16846</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -486,22 +486,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17069</v>
+        <v>17242</v>
       </c>
       <c r="D3" t="n">
-        <v>8670</v>
+        <v>9322</v>
       </c>
       <c r="E3" t="n">
-        <v>392587</v>
+        <v>4103596</v>
       </c>
       <c r="F3" t="n">
-        <v>16836</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -510,22 +510,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17020</v>
+        <v>17046</v>
       </c>
       <c r="D4" t="n">
-        <v>8647</v>
+        <v>9084</v>
       </c>
       <c r="E4" t="n">
-        <v>5905940</v>
+        <v>7057044</v>
       </c>
       <c r="F4" t="n">
-        <v>16835</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -534,22 +534,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17053</v>
+        <v>17069</v>
       </c>
       <c r="D5" t="n">
-        <v>8300</v>
+        <v>8670</v>
       </c>
       <c r="E5" t="n">
-        <v>2660268</v>
+        <v>392587</v>
       </c>
       <c r="F5" t="n">
-        <v>16828</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -558,151 +558,199 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>16919</v>
+        <v>17020</v>
       </c>
       <c r="D6" t="n">
-        <v>8144</v>
+        <v>8647</v>
       </c>
       <c r="E6" t="n">
-        <v>10016048</v>
+        <v>5905940</v>
       </c>
       <c r="F6" t="n">
-        <v>16823</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>202112</v>
+          <t>日期：2021/11/01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>17010</v>
+        <v>17053</v>
       </c>
       <c r="D7" t="n">
-        <v>7552</v>
+        <v>8300</v>
       </c>
       <c r="E7" t="n">
-        <v>5239080</v>
+        <v>2660268</v>
       </c>
       <c r="F7" t="n">
-        <v>16816</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>17038</v>
+        <v>16919</v>
       </c>
       <c r="D8" t="n">
-        <v>7244</v>
+        <v>8144</v>
       </c>
       <c r="E8" t="n">
-        <v>3799474</v>
+        <v>10016048</v>
       </c>
       <c r="F8" t="n">
-        <v>16808</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>202112</v>
       </c>
       <c r="C9" t="n">
-        <v>17014</v>
+        <v>17010</v>
       </c>
       <c r="D9" t="n">
-        <v>7021</v>
+        <v>7552</v>
       </c>
       <c r="E9" t="n">
-        <v>4968088</v>
+        <v>5239080</v>
       </c>
       <c r="F9" t="n">
-        <v>16800</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>202112</v>
       </c>
       <c r="C10" t="n">
-        <v>16864</v>
+        <v>17038</v>
       </c>
       <c r="D10" t="n">
-        <v>6729</v>
+        <v>7244</v>
       </c>
       <c r="E10" t="n">
-        <v>4401504</v>
+        <v>3799474</v>
       </c>
       <c r="F10" t="n">
-        <v>16791</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>202112</v>
       </c>
       <c r="C11" t="n">
-        <v>16828</v>
+        <v>17014</v>
       </c>
       <c r="D11" t="n">
-        <v>6468</v>
+        <v>7021</v>
       </c>
       <c r="E11" t="n">
-        <v>3449740</v>
+        <v>4968088</v>
       </c>
       <c r="F11" t="n">
-        <v>16788</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>202112</v>
       </c>
       <c r="C12" t="n">
+        <v>16864</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6729</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4401504</v>
+      </c>
+      <c r="F12" t="n">
+        <v>16791</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>日期：2021/10/22</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C13" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C14" t="n">
         <v>16789</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D14" t="n">
         <v>6263</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E14" t="n">
         <v>105139507</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F14" t="n">
         <v>16789</v>
       </c>
     </row>
-    <row r="13"/>
+    <row r="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -715,7 +763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -742,70 +790,90 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B10" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -820,7 +888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -852,91 +920,117 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-74.23999999999999</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>30.94</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>38.92</v>
+        <v>265.52</v>
       </c>
       <c r="C3" t="n">
-        <v>17.27</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.71</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>-21.98</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-31.96</v>
+        <v>38.92</v>
       </c>
       <c r="C5" t="n">
-        <v>112.79</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-115.21</v>
+        <v>19.71</v>
       </c>
       <c r="C6" t="n">
-        <v>60.99</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-73.59</v>
+        <v>-31.96</v>
       </c>
       <c r="C7" t="n">
-        <v>40.67</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-115.21</v>
+      </c>
+      <c r="C8" t="n">
+        <v>60.99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C9" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B10" t="n">
         <v>24.64</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C10" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -951,7 +1045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
@@ -978,60 +1072,80 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17156.65</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17116.74</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17133.93</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17080.39</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16983.35</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>110年11月01日</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>17080.39</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B9" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1047,7 +1161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -1118,156 +1232,200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46531</v>
+        <v>47070</v>
       </c>
       <c r="C2" t="n">
-        <v>50459</v>
+        <v>48979</v>
       </c>
       <c r="D2" t="n">
-        <v>1264</v>
+        <v>1594</v>
       </c>
       <c r="E2" t="n">
-        <v>-3179</v>
+        <v>-3421</v>
       </c>
       <c r="J2" t="n">
-        <v>-23097</v>
+        <v>-17455</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2021/11/05</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="C3" t="n">
+        <v>50491</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1055</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-4983</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-21396</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C4" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-23097</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B5" t="n">
         <v>45267</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C5" t="n">
         <v>49710</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D5" t="n">
         <v>-1089</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E5" t="n">
         <v>-6796</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J5" t="n">
         <v>-21534</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>2021/11/02</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B6" t="n">
         <v>46356</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C6" t="n">
         <v>52063</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <f>B2-B3</f>
         <v/>
       </c>
-      <c r="E4">
+      <c r="E6">
         <f>C2-C3</f>
         <v/>
       </c>
-      <c r="F4" t="n">
+      <c r="F6" t="n">
         <v>21541</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G6" t="n">
         <v>43984</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J6" t="n">
         <v>-22443</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>2021/11/01</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B7" t="n">
         <v>43954</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C7" t="n">
         <v>51270</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <f>B3-B4</f>
         <v/>
       </c>
-      <c r="E5">
+      <c r="E7">
         <f>C3-C4</f>
         <v/>
       </c>
-      <c r="F5" t="n">
+      <c r="F7" t="n">
         <v>20227</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G7" t="n">
         <v>42311</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J7" t="n">
         <v>-22084</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>2021/10/29</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B8" t="n">
         <v>44430</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C8" t="n">
         <v>51627</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <f>B4-B5</f>
         <v/>
       </c>
-      <c r="E6">
+      <c r="E8">
         <f>C4-C5</f>
         <v/>
       </c>
-      <c r="F6" t="n">
+      <c r="F8" t="n">
         <v>19062</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G8" t="n">
         <v>42904</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J8" t="n">
         <v>-23842</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B9" t="n">
         <v>42514</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C9" t="n">
         <v>51801</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F9" t="n">
         <v>19933</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G9" t="n">
         <v>42347</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J9" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/010 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -13,7 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="期貨大額交易人未沖銷部位" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -56,9 +56,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -402,13 +405,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18.375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -453,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17395</v>
+        <v>17524</v>
       </c>
       <c r="D2" t="n">
-        <v>9997</v>
+        <v>10976</v>
       </c>
       <c r="E2" t="n">
-        <v>11741625</v>
+        <v>911248</v>
       </c>
       <c r="F2" t="n">
-        <v>16892</v>
+        <v>16948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -486,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17242</v>
+        <v>17521</v>
       </c>
       <c r="D3" t="n">
-        <v>9322</v>
+        <v>10924</v>
       </c>
       <c r="E3" t="n">
-        <v>4103596</v>
+        <v>16241967</v>
       </c>
       <c r="F3" t="n">
-        <v>16856</v>
+        <v>16945</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -510,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17046</v>
+        <v>17395</v>
       </c>
       <c r="D4" t="n">
-        <v>9084</v>
+        <v>9997</v>
       </c>
       <c r="E4" t="n">
-        <v>7057044</v>
+        <v>11741625</v>
       </c>
       <c r="F4" t="n">
-        <v>16846</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -534,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17069</v>
+        <v>17242</v>
       </c>
       <c r="D5" t="n">
-        <v>8670</v>
+        <v>9322</v>
       </c>
       <c r="E5" t="n">
-        <v>392587</v>
+        <v>4103596</v>
       </c>
       <c r="F5" t="n">
-        <v>16836</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -558,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17020</v>
+        <v>17046</v>
       </c>
       <c r="D6" t="n">
-        <v>8647</v>
+        <v>9084</v>
       </c>
       <c r="E6" t="n">
-        <v>5905940</v>
+        <v>7057044</v>
       </c>
       <c r="F6" t="n">
-        <v>16835</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -582,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17053</v>
+        <v>17069</v>
       </c>
       <c r="D7" t="n">
-        <v>8300</v>
+        <v>8670</v>
       </c>
       <c r="E7" t="n">
-        <v>2660268</v>
+        <v>392587</v>
       </c>
       <c r="F7" t="n">
-        <v>16828</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -606,151 +609,198 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>16919</v>
+        <v>17020</v>
       </c>
       <c r="D8" t="n">
-        <v>8144</v>
+        <v>8647</v>
       </c>
       <c r="E8" t="n">
-        <v>10016048</v>
+        <v>5905940</v>
       </c>
       <c r="F8" t="n">
-        <v>16823</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>202112</v>
+          <t>日期：2021/11/01</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C9" t="n">
-        <v>17010</v>
+        <v>17053</v>
       </c>
       <c r="D9" t="n">
-        <v>7552</v>
+        <v>8300</v>
       </c>
       <c r="E9" t="n">
-        <v>5239080</v>
+        <v>2660268</v>
       </c>
       <c r="F9" t="n">
-        <v>16816</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C10" t="n">
-        <v>17038</v>
+        <v>16919</v>
       </c>
       <c r="D10" t="n">
-        <v>7244</v>
+        <v>8144</v>
       </c>
       <c r="E10" t="n">
-        <v>3799474</v>
+        <v>10016048</v>
       </c>
       <c r="F10" t="n">
-        <v>16808</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>202112</v>
       </c>
       <c r="C11" t="n">
-        <v>17014</v>
+        <v>17010</v>
       </c>
       <c r="D11" t="n">
-        <v>7021</v>
+        <v>7552</v>
       </c>
       <c r="E11" t="n">
-        <v>4968088</v>
+        <v>5239080</v>
       </c>
       <c r="F11" t="n">
-        <v>16800</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>202112</v>
       </c>
       <c r="C12" t="n">
-        <v>16864</v>
+        <v>17038</v>
       </c>
       <c r="D12" t="n">
-        <v>6729</v>
+        <v>7244</v>
       </c>
       <c r="E12" t="n">
-        <v>4401504</v>
+        <v>3799474</v>
       </c>
       <c r="F12" t="n">
-        <v>16791</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>202112</v>
       </c>
       <c r="C13" t="n">
-        <v>16828</v>
+        <v>17014</v>
       </c>
       <c r="D13" t="n">
-        <v>6468</v>
+        <v>7021</v>
       </c>
       <c r="E13" t="n">
-        <v>3449740</v>
+        <v>4968088</v>
       </c>
       <c r="F13" t="n">
-        <v>16788</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>202112</v>
       </c>
       <c r="C14" t="n">
+        <v>16864</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6729</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4401504</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16791</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>日期：2021/10/22</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C15" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F15" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C16" t="n">
         <v>16789</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D16" t="n">
         <v>6263</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E16" t="n">
         <v>105139507</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F16" t="n">
         <v>16789</v>
       </c>
     </row>
-    <row r="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -763,13 +813,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -790,90 +840,110 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.11</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.06</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B12" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -888,13 +958,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17.125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.375" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -920,117 +990,143 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67.51000000000001</v>
+        <v>0.29</v>
       </c>
       <c r="C2" t="n">
-        <v>50.89</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>265.52</v>
+        <v>196.05</v>
       </c>
       <c r="C3" t="n">
-        <v>-47.48</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-74.23999999999999</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>30.94</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38.92</v>
+        <v>265.52</v>
       </c>
       <c r="C5" t="n">
-        <v>17.27</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>19.71</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>-21.98</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-31.96</v>
+        <v>38.92</v>
       </c>
       <c r="C7" t="n">
-        <v>112.79</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-115.21</v>
+        <v>19.71</v>
       </c>
       <c r="C8" t="n">
-        <v>60.99</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-73.59</v>
+        <v>-31.96</v>
       </c>
       <c r="C9" t="n">
-        <v>40.67</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-115.21</v>
+      </c>
+      <c r="C10" t="n">
+        <v>60.99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C11" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B12" t="n">
         <v>24.64</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C12" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1045,13 +1141,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.75" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -1072,80 +1168,100 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17348.15</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17202.29</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17156.65</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17116.74</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17133.93</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17080.39</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>16983.35</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>110年11月01日</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>17080.39</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B11" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1161,13 +1277,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.25" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -1175,6 +1291,9 @@
     <col width="11.25" bestFit="1" customWidth="1" min="6" max="7"/>
     <col width="16.5" bestFit="1" customWidth="1" min="8" max="9"/>
     <col width="16.5" customWidth="1" min="10" max="10"/>
+    <col width="20.5" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="15.5" bestFit="1" customWidth="1" min="12" max="13"/>
+    <col width="20.5" bestFit="1" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1228,204 +1347,460 @@
           <t>外資多空淨額</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>外資多空淨額增減</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>九大多方增減</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>九大空方增減</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>九大多空淨額增減</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47070</v>
+        <v>48858</v>
       </c>
       <c r="C2" t="n">
-        <v>48979</v>
+        <v>47770</v>
       </c>
       <c r="D2" t="n">
-        <v>1594</v>
+        <v>474</v>
       </c>
       <c r="E2" t="n">
-        <v>-3421</v>
+        <v>351</v>
+      </c>
+      <c r="F2" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G2" t="n">
+        <v>40270</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2027</v>
+      </c>
+      <c r="I2" t="n">
+        <v>904</v>
       </c>
       <c r="J2" t="n">
-        <v>-17455</v>
+        <v>-16513</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-2931</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2501</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-553</v>
+      </c>
+      <c r="N2" t="n">
+        <v>3054</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45476</v>
+        <v>48384</v>
       </c>
       <c r="C3" t="n">
-        <v>50491</v>
+        <v>48507</v>
       </c>
       <c r="D3" t="n">
-        <v>-1055</v>
+        <v>1314</v>
       </c>
       <c r="E3" t="n">
-        <v>-4983</v>
+        <v>-595</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>25784</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>39366</v>
+      </c>
+      <c r="H3" t="n">
+        <v>896</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-2977</v>
       </c>
       <c r="J3" t="n">
-        <v>-21396</v>
+        <v>-13582</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3873</v>
+      </c>
+      <c r="L3" t="n">
+        <v>418</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2382</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1964</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46531</v>
+        <v>47070</v>
       </c>
       <c r="C4" t="n">
-        <v>50459</v>
+        <v>48979</v>
       </c>
       <c r="D4" t="n">
-        <v>1264</v>
+        <v>1594</v>
       </c>
       <c r="E4" t="n">
-        <v>-3179</v>
+        <v>-3421</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>24888</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>42343</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2148</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1793</v>
       </c>
       <c r="J4" t="n">
-        <v>-23097</v>
+        <v>-17455</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3941</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-554</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1628</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1074</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>2021/11/05</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>45476</v>
+      </c>
+      <c r="C5" t="n">
+        <v>50491</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1055</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-4983</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>22740</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>44136</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1964</v>
+      </c>
+      <c r="I5" t="n">
+        <v>263</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-21396</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1701</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-3019</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-5246</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C6" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-4728</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B7" t="n">
         <v>45267</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C7" t="n">
         <v>49710</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D7" t="n">
         <v>-1089</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E7" t="n">
         <v>-6796</v>
       </c>
-      <c r="J5" t="n">
+      <c r="F7" s="2" t="n">
+        <v>20790</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>42324</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-751</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1660</v>
+      </c>
+      <c r="J7" t="n">
         <v>-21534</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C6" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D6">
-        <f>B2-B3</f>
-        <v/>
-      </c>
-      <c r="E6">
-        <f>C2-C3</f>
-        <v/>
-      </c>
-      <c r="F6" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G6" t="n">
-        <v>43984</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-22443</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/01</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>43954</v>
-      </c>
-      <c r="C7" t="n">
-        <v>51270</v>
-      </c>
-      <c r="D7">
-        <f>B3-B4</f>
-        <v/>
-      </c>
-      <c r="E7">
-        <f>C3-C4</f>
-        <v/>
-      </c>
-      <c r="F7" t="n">
-        <v>20227</v>
-      </c>
-      <c r="G7" t="n">
-        <v>42311</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-22084</v>
+      <c r="K7" t="n">
+        <v>909</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-338</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-5136</v>
+      </c>
+      <c r="N7" t="n">
+        <v>4798</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>44430</v>
+        <v>46356</v>
       </c>
       <c r="C8" t="n">
-        <v>51627</v>
-      </c>
-      <c r="D8">
-        <f>B4-B5</f>
-        <v/>
-      </c>
-      <c r="E8">
-        <f>C4-C5</f>
-        <v/>
-      </c>
-      <c r="F8" t="n">
-        <v>19062</v>
-      </c>
-      <c r="G8" t="n">
-        <v>42904</v>
+        <v>52063</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2402</v>
+      </c>
+      <c r="E8" t="n">
+        <v>793</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>21541</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>43984</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1314</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1673</v>
       </c>
       <c r="J8" t="n">
-        <v>-23842</v>
+        <v>-22443</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-359</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1088</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-880</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1968</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>2021/11/01</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>43954</v>
+      </c>
+      <c r="C9" t="n">
+        <v>51270</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-476</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-357</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>20227</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>42311</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1165</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-593</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-22084</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1758</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-1641</v>
+      </c>
+      <c r="M9" t="n">
+        <v>236</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-1877</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C10" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I10" t="n">
+        <v>557</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N10" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B11" t="n">
         <v>42514</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C11" t="n">
         <v>51801</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F11" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G11" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J11" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/11 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,13 +405,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="18.375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17524</v>
+        <v>17445</v>
       </c>
       <c r="D2" t="n">
-        <v>10976</v>
+        <v>12028</v>
       </c>
       <c r="E2" t="n">
-        <v>911248</v>
+        <v>18352140</v>
       </c>
       <c r="F2" t="n">
-        <v>16948</v>
+        <v>16992</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17521</v>
+        <v>17524</v>
       </c>
       <c r="D3" t="n">
-        <v>10924</v>
+        <v>10976</v>
       </c>
       <c r="E3" t="n">
-        <v>16241967</v>
+        <v>911248</v>
       </c>
       <c r="F3" t="n">
-        <v>16945</v>
+        <v>16948</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17395</v>
+        <v>17521</v>
       </c>
       <c r="D4" t="n">
-        <v>9997</v>
+        <v>10924</v>
       </c>
       <c r="E4" t="n">
-        <v>11741625</v>
+        <v>16241967</v>
       </c>
       <c r="F4" t="n">
-        <v>16892</v>
+        <v>16945</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17242</v>
+        <v>17395</v>
       </c>
       <c r="D5" t="n">
-        <v>9322</v>
+        <v>9997</v>
       </c>
       <c r="E5" t="n">
-        <v>4103596</v>
+        <v>11741625</v>
       </c>
       <c r="F5" t="n">
-        <v>16856</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17046</v>
+        <v>17242</v>
       </c>
       <c r="D6" t="n">
-        <v>9084</v>
+        <v>9322</v>
       </c>
       <c r="E6" t="n">
-        <v>7057044</v>
+        <v>4103596</v>
       </c>
       <c r="F6" t="n">
-        <v>16846</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17069</v>
+        <v>17046</v>
       </c>
       <c r="D7" t="n">
-        <v>8670</v>
+        <v>9084</v>
       </c>
       <c r="E7" t="n">
-        <v>392587</v>
+        <v>7057044</v>
       </c>
       <c r="F7" t="n">
-        <v>16836</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17020</v>
+        <v>17069</v>
       </c>
       <c r="D8" t="n">
-        <v>8647</v>
+        <v>8670</v>
       </c>
       <c r="E8" t="n">
-        <v>5905940</v>
+        <v>392587</v>
       </c>
       <c r="F8" t="n">
-        <v>16835</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17053</v>
+        <v>17020</v>
       </c>
       <c r="D9" t="n">
-        <v>8300</v>
+        <v>8647</v>
       </c>
       <c r="E9" t="n">
-        <v>2660268</v>
+        <v>5905940</v>
       </c>
       <c r="F9" t="n">
-        <v>16828</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,150 +657,175 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>16919</v>
+        <v>17053</v>
       </c>
       <c r="D10" t="n">
-        <v>8144</v>
+        <v>8300</v>
       </c>
       <c r="E10" t="n">
-        <v>10016048</v>
+        <v>2660268</v>
       </c>
       <c r="F10" t="n">
-        <v>16823</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>17010</v>
+        <v>16919</v>
       </c>
       <c r="D11" t="n">
-        <v>7552</v>
+        <v>8144</v>
       </c>
       <c r="E11" t="n">
-        <v>5239080</v>
+        <v>10016048</v>
       </c>
       <c r="F11" t="n">
-        <v>16816</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>202112</v>
       </c>
       <c r="C12" t="n">
-        <v>17038</v>
+        <v>17010</v>
       </c>
       <c r="D12" t="n">
-        <v>7244</v>
+        <v>7552</v>
       </c>
       <c r="E12" t="n">
-        <v>3799474</v>
+        <v>5239080</v>
       </c>
       <c r="F12" t="n">
-        <v>16808</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>202112</v>
       </c>
       <c r="C13" t="n">
-        <v>17014</v>
+        <v>17038</v>
       </c>
       <c r="D13" t="n">
-        <v>7021</v>
+        <v>7244</v>
       </c>
       <c r="E13" t="n">
-        <v>4968088</v>
+        <v>3799474</v>
       </c>
       <c r="F13" t="n">
-        <v>16800</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>202112</v>
       </c>
       <c r="C14" t="n">
-        <v>16864</v>
+        <v>17014</v>
       </c>
       <c r="D14" t="n">
-        <v>6729</v>
+        <v>7021</v>
       </c>
       <c r="E14" t="n">
-        <v>4401504</v>
+        <v>4968088</v>
       </c>
       <c r="F14" t="n">
-        <v>16791</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>202112</v>
       </c>
       <c r="C15" t="n">
-        <v>16828</v>
+        <v>16864</v>
       </c>
       <c r="D15" t="n">
-        <v>6468</v>
+        <v>6729</v>
       </c>
       <c r="E15" t="n">
-        <v>3449740</v>
+        <v>4401504</v>
       </c>
       <c r="F15" t="n">
-        <v>16788</v>
+        <v>16791</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/22</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>202112</v>
       </c>
       <c r="C16" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F16" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C17" t="n">
         <v>16789</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D17" t="n">
         <v>6263</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E17" t="n">
         <v>105139507</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F17" t="n">
         <v>16789</v>
       </c>
     </row>
+    <row r="18"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -813,13 +838,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="19.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -840,110 +865,120 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -958,13 +993,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="17.125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.375" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -990,143 +1025,156 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C3" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C4" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C6" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C8" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C9" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C10" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C11" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C12" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" t="n">
         <v>24.64</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1141,13 +1189,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.75" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -1168,100 +1216,110 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B12" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1277,13 +1335,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.25" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -1371,436 +1429,482 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C2" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D2" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E2" t="n">
-        <v>351</v>
+        <v>-7</v>
       </c>
       <c r="F2" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G2" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H2" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I2" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J2" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K2" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L2" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M2" t="n">
-        <v>-553</v>
+        <v>-1075</v>
       </c>
       <c r="N2" t="n">
-        <v>3054</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C3" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D3" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E3" t="n">
-        <v>-595</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>39366</v>
+        <v>351</v>
+      </c>
+      <c r="F3" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G3" t="n">
+        <v>40270</v>
       </c>
       <c r="H3" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I3" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J3" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K3" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L3" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M3" t="n">
-        <v>2382</v>
+        <v>-553</v>
       </c>
       <c r="N3" t="n">
-        <v>-1964</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C4" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D4" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E4" t="n">
-        <v>-3421</v>
+        <v>-595</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H4" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I4" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J4" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K4" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L4" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M4" t="n">
-        <v>-1628</v>
+        <v>2382</v>
       </c>
       <c r="N4" t="n">
-        <v>1074</v>
+        <v>-1964</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C5" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D5" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E5" t="n">
-        <v>-4983</v>
+        <v>-3421</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H5" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I5" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J5" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K5" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L5" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M5" t="n">
-        <v>-5246</v>
+        <v>-1628</v>
       </c>
       <c r="N5" t="n">
-        <v>2227</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C6" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D6" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E6" t="n">
-        <v>-3179</v>
+        <v>-4983</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H6" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I6" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J6" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K6" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L6" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M6" t="n">
-        <v>-4728</v>
+        <v>-5246</v>
       </c>
       <c r="N6" t="n">
-        <v>6006</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-4728</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" t="n">
         <v>45267</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C8" t="n">
         <v>49710</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>-1089</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E8" t="n">
         <v>-6796</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F8" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G8" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H8" t="n">
         <v>-751</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I8" t="n">
         <v>-1660</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J8" t="n">
         <v>-21534</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K8" t="n">
         <v>909</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L8" t="n">
         <v>-338</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M8" t="n">
         <v>-5136</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N8" t="n">
         <v>4798</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C8" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E8" t="n">
-        <v>793</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N8" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C9" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D9" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E9" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H9" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I9" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J9" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K9" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L9" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M9" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N9" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C10" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D10" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E10" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H10" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I10" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J10" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K10" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L10" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M10" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N10" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C11" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I11" t="n">
+        <v>557</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N11" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B12" t="n">
         <v>42514</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C12" t="n">
         <v>51801</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F12" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G12" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J12" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/12 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17445</v>
+        <v>17524</v>
       </c>
       <c r="D2" t="n">
-        <v>12028</v>
+        <v>14458</v>
       </c>
       <c r="E2" t="n">
-        <v>18352140</v>
+        <v>42583320</v>
       </c>
       <c r="F2" t="n">
-        <v>16992</v>
+        <v>17081</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17524</v>
+        <v>17445</v>
       </c>
       <c r="D3" t="n">
-        <v>10976</v>
+        <v>12028</v>
       </c>
       <c r="E3" t="n">
-        <v>911248</v>
+        <v>18352140</v>
       </c>
       <c r="F3" t="n">
-        <v>16948</v>
+        <v>16992</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17521</v>
+        <v>17524</v>
       </c>
       <c r="D4" t="n">
-        <v>10924</v>
+        <v>10976</v>
       </c>
       <c r="E4" t="n">
-        <v>16241967</v>
+        <v>911248</v>
       </c>
       <c r="F4" t="n">
-        <v>16945</v>
+        <v>16948</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17395</v>
+        <v>17521</v>
       </c>
       <c r="D5" t="n">
-        <v>9997</v>
+        <v>10924</v>
       </c>
       <c r="E5" t="n">
-        <v>11741625</v>
+        <v>16241967</v>
       </c>
       <c r="F5" t="n">
-        <v>16892</v>
+        <v>16945</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17242</v>
+        <v>17395</v>
       </c>
       <c r="D6" t="n">
-        <v>9322</v>
+        <v>9997</v>
       </c>
       <c r="E6" t="n">
-        <v>4103596</v>
+        <v>11741625</v>
       </c>
       <c r="F6" t="n">
-        <v>16856</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17046</v>
+        <v>17242</v>
       </c>
       <c r="D7" t="n">
-        <v>9084</v>
+        <v>9322</v>
       </c>
       <c r="E7" t="n">
-        <v>7057044</v>
+        <v>4103596</v>
       </c>
       <c r="F7" t="n">
-        <v>16846</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17069</v>
+        <v>17046</v>
       </c>
       <c r="D8" t="n">
-        <v>8670</v>
+        <v>9084</v>
       </c>
       <c r="E8" t="n">
-        <v>392587</v>
+        <v>7057044</v>
       </c>
       <c r="F8" t="n">
-        <v>16836</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17020</v>
+        <v>17069</v>
       </c>
       <c r="D9" t="n">
-        <v>8647</v>
+        <v>8670</v>
       </c>
       <c r="E9" t="n">
-        <v>5905940</v>
+        <v>392587</v>
       </c>
       <c r="F9" t="n">
-        <v>16835</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17053</v>
+        <v>17020</v>
       </c>
       <c r="D10" t="n">
-        <v>8300</v>
+        <v>8647</v>
       </c>
       <c r="E10" t="n">
-        <v>2660268</v>
+        <v>5905940</v>
       </c>
       <c r="F10" t="n">
-        <v>16828</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,151 +681,175 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>16919</v>
+        <v>17053</v>
       </c>
       <c r="D11" t="n">
-        <v>8144</v>
+        <v>8300</v>
       </c>
       <c r="E11" t="n">
-        <v>10016048</v>
+        <v>2660268</v>
       </c>
       <c r="F11" t="n">
-        <v>16823</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C12" t="n">
-        <v>17010</v>
+        <v>16919</v>
       </c>
       <c r="D12" t="n">
-        <v>7552</v>
+        <v>8144</v>
       </c>
       <c r="E12" t="n">
-        <v>5239080</v>
+        <v>10016048</v>
       </c>
       <c r="F12" t="n">
-        <v>16816</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>202112</v>
       </c>
       <c r="C13" t="n">
-        <v>17038</v>
+        <v>17010</v>
       </c>
       <c r="D13" t="n">
-        <v>7244</v>
+        <v>7552</v>
       </c>
       <c r="E13" t="n">
-        <v>3799474</v>
+        <v>5239080</v>
       </c>
       <c r="F13" t="n">
-        <v>16808</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>202112</v>
       </c>
       <c r="C14" t="n">
-        <v>17014</v>
+        <v>17038</v>
       </c>
       <c r="D14" t="n">
-        <v>7021</v>
+        <v>7244</v>
       </c>
       <c r="E14" t="n">
-        <v>4968088</v>
+        <v>3799474</v>
       </c>
       <c r="F14" t="n">
-        <v>16800</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>202112</v>
       </c>
       <c r="C15" t="n">
-        <v>16864</v>
+        <v>17014</v>
       </c>
       <c r="D15" t="n">
-        <v>6729</v>
+        <v>7021</v>
       </c>
       <c r="E15" t="n">
-        <v>4401504</v>
+        <v>4968088</v>
       </c>
       <c r="F15" t="n">
-        <v>16791</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>202112</v>
       </c>
       <c r="C16" t="n">
-        <v>16828</v>
+        <v>16864</v>
       </c>
       <c r="D16" t="n">
-        <v>6468</v>
+        <v>6729</v>
       </c>
       <c r="E16" t="n">
-        <v>3449740</v>
+        <v>4401504</v>
       </c>
       <c r="F16" t="n">
-        <v>16788</v>
+        <v>16791</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/22</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>202112</v>
       </c>
       <c r="C17" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F17" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C18" t="n">
         <v>16789</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>6263</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>105139507</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F18" t="n">
         <v>16789</v>
       </c>
     </row>
-    <row r="18"/>
+    <row r="19"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -838,7 +862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -865,120 +889,130 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B14" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -993,7 +1027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -1025,156 +1059,169 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C4" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C5" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C6" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C7" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C9" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C10" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C11" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C12" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C13" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B14" t="n">
         <v>24.64</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C14" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1189,7 +1236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
@@ -1216,110 +1263,120 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1335,7 +1392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1429,482 +1486,528 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C2" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D2" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E2" t="n">
-        <v>-7</v>
+        <v>400</v>
       </c>
       <c r="F2" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G2" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H2" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I2" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J2" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K2" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L2" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M2" t="n">
-        <v>-1075</v>
+        <v>-932</v>
       </c>
       <c r="N2" t="n">
-        <v>389</v>
+        <v>-1147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C3" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D3" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E3" t="n">
-        <v>351</v>
+        <v>-7</v>
       </c>
       <c r="F3" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G3" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H3" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I3" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J3" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K3" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L3" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M3" t="n">
-        <v>-553</v>
+        <v>-1075</v>
       </c>
       <c r="N3" t="n">
-        <v>3054</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C4" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D4" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E4" t="n">
-        <v>-595</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>39366</v>
+        <v>351</v>
+      </c>
+      <c r="F4" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G4" t="n">
+        <v>40270</v>
       </c>
       <c r="H4" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I4" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J4" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K4" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L4" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M4" t="n">
-        <v>2382</v>
+        <v>-553</v>
       </c>
       <c r="N4" t="n">
-        <v>-1964</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C5" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D5" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E5" t="n">
-        <v>-3421</v>
+        <v>-595</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H5" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I5" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J5" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K5" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L5" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M5" t="n">
-        <v>-1628</v>
+        <v>2382</v>
       </c>
       <c r="N5" t="n">
-        <v>1074</v>
+        <v>-1964</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C6" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D6" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E6" t="n">
-        <v>-4983</v>
+        <v>-3421</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H6" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I6" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J6" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K6" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L6" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M6" t="n">
-        <v>-5246</v>
+        <v>-1628</v>
       </c>
       <c r="N6" t="n">
-        <v>2227</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C7" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D7" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E7" t="n">
-        <v>-3179</v>
+        <v>-4983</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H7" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I7" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J7" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K7" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L7" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M7" t="n">
-        <v>-4728</v>
+        <v>-5246</v>
       </c>
       <c r="N7" t="n">
-        <v>6006</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C8" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-4728</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B9" t="n">
         <v>45267</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C9" t="n">
         <v>49710</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>-1089</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" t="n">
         <v>-6796</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F9" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G9" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H9" t="n">
         <v>-751</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I9" t="n">
         <v>-1660</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J9" t="n">
         <v>-21534</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K9" t="n">
         <v>909</v>
       </c>
-      <c r="L8" t="n">
+      <c r="L9" t="n">
         <v>-338</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M9" t="n">
         <v>-5136</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N9" t="n">
         <v>4798</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C9" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E9" t="n">
-        <v>793</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J9" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C10" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D10" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E10" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H10" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I10" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J10" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K10" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L10" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M10" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N10" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C11" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D11" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E11" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H11" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I11" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J11" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K11" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L11" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M11" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N11" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C12" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I12" t="n">
+        <v>557</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N12" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" t="n">
         <v>42514</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>51801</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F13" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G13" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J13" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/15 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17524</v>
+        <v>17647</v>
       </c>
       <c r="D2" t="n">
-        <v>14458</v>
+        <v>35126</v>
       </c>
       <c r="E2" t="n">
-        <v>42583320</v>
+        <v>364728196</v>
       </c>
       <c r="F2" t="n">
-        <v>17081</v>
+        <v>17414</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17445</v>
+        <v>17524</v>
       </c>
       <c r="D3" t="n">
-        <v>12028</v>
+        <v>14458</v>
       </c>
       <c r="E3" t="n">
-        <v>18352140</v>
+        <v>42583320</v>
       </c>
       <c r="F3" t="n">
-        <v>16992</v>
+        <v>17081</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17524</v>
+        <v>17445</v>
       </c>
       <c r="D4" t="n">
-        <v>10976</v>
+        <v>12028</v>
       </c>
       <c r="E4" t="n">
-        <v>911248</v>
+        <v>18352140</v>
       </c>
       <c r="F4" t="n">
-        <v>16948</v>
+        <v>16992</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17521</v>
+        <v>17524</v>
       </c>
       <c r="D5" t="n">
-        <v>10924</v>
+        <v>10976</v>
       </c>
       <c r="E5" t="n">
-        <v>16241967</v>
+        <v>911248</v>
       </c>
       <c r="F5" t="n">
-        <v>16945</v>
+        <v>16948</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17395</v>
+        <v>17521</v>
       </c>
       <c r="D6" t="n">
-        <v>9997</v>
+        <v>10924</v>
       </c>
       <c r="E6" t="n">
-        <v>11741625</v>
+        <v>16241967</v>
       </c>
       <c r="F6" t="n">
-        <v>16892</v>
+        <v>16945</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17242</v>
+        <v>17395</v>
       </c>
       <c r="D7" t="n">
-        <v>9322</v>
+        <v>9997</v>
       </c>
       <c r="E7" t="n">
-        <v>4103596</v>
+        <v>11741625</v>
       </c>
       <c r="F7" t="n">
-        <v>16856</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17046</v>
+        <v>17242</v>
       </c>
       <c r="D8" t="n">
-        <v>9084</v>
+        <v>9322</v>
       </c>
       <c r="E8" t="n">
-        <v>7057044</v>
+        <v>4103596</v>
       </c>
       <c r="F8" t="n">
-        <v>16846</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17069</v>
+        <v>17046</v>
       </c>
       <c r="D9" t="n">
-        <v>8670</v>
+        <v>9084</v>
       </c>
       <c r="E9" t="n">
-        <v>392587</v>
+        <v>7057044</v>
       </c>
       <c r="F9" t="n">
-        <v>16836</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17020</v>
+        <v>17069</v>
       </c>
       <c r="D10" t="n">
-        <v>8647</v>
+        <v>8670</v>
       </c>
       <c r="E10" t="n">
-        <v>5905940</v>
+        <v>392587</v>
       </c>
       <c r="F10" t="n">
-        <v>16835</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17053</v>
+        <v>17020</v>
       </c>
       <c r="D11" t="n">
-        <v>8300</v>
+        <v>8647</v>
       </c>
       <c r="E11" t="n">
-        <v>2660268</v>
+        <v>5905940</v>
       </c>
       <c r="F11" t="n">
-        <v>16828</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,151 +705,175 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>16919</v>
+        <v>17053</v>
       </c>
       <c r="D12" t="n">
-        <v>8144</v>
+        <v>8300</v>
       </c>
       <c r="E12" t="n">
-        <v>10016048</v>
+        <v>2660268</v>
       </c>
       <c r="F12" t="n">
-        <v>16823</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>17010</v>
+        <v>16919</v>
       </c>
       <c r="D13" t="n">
-        <v>7552</v>
+        <v>8144</v>
       </c>
       <c r="E13" t="n">
-        <v>5239080</v>
+        <v>10016048</v>
       </c>
       <c r="F13" t="n">
-        <v>16816</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>202112</v>
       </c>
       <c r="C14" t="n">
-        <v>17038</v>
+        <v>17010</v>
       </c>
       <c r="D14" t="n">
-        <v>7244</v>
+        <v>7552</v>
       </c>
       <c r="E14" t="n">
-        <v>3799474</v>
+        <v>5239080</v>
       </c>
       <c r="F14" t="n">
-        <v>16808</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>202112</v>
       </c>
       <c r="C15" t="n">
-        <v>17014</v>
+        <v>17038</v>
       </c>
       <c r="D15" t="n">
-        <v>7021</v>
+        <v>7244</v>
       </c>
       <c r="E15" t="n">
-        <v>4968088</v>
+        <v>3799474</v>
       </c>
       <c r="F15" t="n">
-        <v>16800</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>202112</v>
       </c>
       <c r="C16" t="n">
-        <v>16864</v>
+        <v>17014</v>
       </c>
       <c r="D16" t="n">
-        <v>6729</v>
+        <v>7021</v>
       </c>
       <c r="E16" t="n">
-        <v>4401504</v>
+        <v>4968088</v>
       </c>
       <c r="F16" t="n">
-        <v>16791</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>202112</v>
       </c>
       <c r="C17" t="n">
-        <v>16828</v>
+        <v>16864</v>
       </c>
       <c r="D17" t="n">
-        <v>6468</v>
+        <v>6729</v>
       </c>
       <c r="E17" t="n">
-        <v>3449740</v>
+        <v>4401504</v>
       </c>
       <c r="F17" t="n">
-        <v>16788</v>
+        <v>16791</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/22</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>202112</v>
       </c>
       <c r="C18" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F18" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C19" t="n">
         <v>16789</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>6263</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E19" t="n">
         <v>105139507</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F19" t="n">
         <v>16789</v>
       </c>
     </row>
-    <row r="19"/>
+    <row r="20"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -862,7 +886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -889,130 +913,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1027,7 +1061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -1059,169 +1093,182 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C2" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C5" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C6" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C7" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C8" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C10" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C11" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C12" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C13" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C14" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>24.64</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1236,7 +1283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
@@ -1263,120 +1310,130 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B14" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1392,7 +1449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1486,528 +1543,574 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C2" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D2" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E2" t="n">
-        <v>400</v>
+        <v>279</v>
       </c>
       <c r="F2" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G2" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H2" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I2" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J2" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K2" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L2" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M2" t="n">
-        <v>-932</v>
+        <v>-2084</v>
       </c>
       <c r="N2" t="n">
-        <v>-1147</v>
+        <v>-466</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C3" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D3" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E3" t="n">
-        <v>-7</v>
+        <v>400</v>
       </c>
       <c r="F3" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G3" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H3" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I3" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J3" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K3" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L3" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M3" t="n">
-        <v>-1075</v>
+        <v>-932</v>
       </c>
       <c r="N3" t="n">
-        <v>389</v>
+        <v>-1147</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C4" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D4" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E4" t="n">
-        <v>351</v>
+        <v>-7</v>
       </c>
       <c r="F4" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G4" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H4" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I4" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J4" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K4" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L4" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M4" t="n">
-        <v>-553</v>
+        <v>-1075</v>
       </c>
       <c r="N4" t="n">
-        <v>3054</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C5" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D5" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E5" t="n">
-        <v>-595</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>39366</v>
+        <v>351</v>
+      </c>
+      <c r="F5" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G5" t="n">
+        <v>40270</v>
       </c>
       <c r="H5" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I5" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J5" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K5" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L5" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M5" t="n">
-        <v>2382</v>
+        <v>-553</v>
       </c>
       <c r="N5" t="n">
-        <v>-1964</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C6" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D6" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E6" t="n">
-        <v>-3421</v>
+        <v>-595</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H6" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I6" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J6" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K6" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L6" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M6" t="n">
-        <v>-1628</v>
+        <v>2382</v>
       </c>
       <c r="N6" t="n">
-        <v>1074</v>
+        <v>-1964</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C7" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D7" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E7" t="n">
-        <v>-4983</v>
+        <v>-3421</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H7" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I7" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J7" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K7" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L7" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M7" t="n">
-        <v>-5246</v>
+        <v>-1628</v>
       </c>
       <c r="N7" t="n">
-        <v>2227</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C8" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D8" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E8" t="n">
-        <v>-3179</v>
+        <v>-4983</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H8" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I8" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J8" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K8" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L8" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M8" t="n">
-        <v>-4728</v>
+        <v>-5246</v>
       </c>
       <c r="N8" t="n">
-        <v>6006</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-4728</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>45267</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>49710</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>-1089</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>-6796</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F10" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G10" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
         <v>-751</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I10" t="n">
         <v>-1660</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J10" t="n">
         <v>-21534</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K10" t="n">
         <v>909</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L10" t="n">
         <v>-338</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M10" t="n">
         <v>-5136</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N10" t="n">
         <v>4798</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C10" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E10" t="n">
-        <v>793</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J10" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K10" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M10" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N10" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C11" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D11" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E11" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H11" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I11" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J11" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K11" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L11" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M11" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N11" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C12" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D12" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E12" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H12" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I12" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J12" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K12" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L12" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M12" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N12" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C13" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I13" t="n">
+        <v>557</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N13" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B14" t="n">
         <v>42514</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C14" t="n">
         <v>51801</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F14" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G14" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J14" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/16 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17647</v>
+        <v>17680</v>
       </c>
       <c r="D2" t="n">
-        <v>35126</v>
+        <v>55055</v>
       </c>
       <c r="E2" t="n">
-        <v>364728196</v>
+        <v>352344720</v>
       </c>
       <c r="F2" t="n">
-        <v>17414</v>
+        <v>17510</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17524</v>
+        <v>17647</v>
       </c>
       <c r="D3" t="n">
-        <v>14458</v>
+        <v>35126</v>
       </c>
       <c r="E3" t="n">
-        <v>42583320</v>
+        <v>364728196</v>
       </c>
       <c r="F3" t="n">
-        <v>17081</v>
+        <v>17414</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17445</v>
+        <v>17524</v>
       </c>
       <c r="D4" t="n">
-        <v>12028</v>
+        <v>14458</v>
       </c>
       <c r="E4" t="n">
-        <v>18352140</v>
+        <v>42583320</v>
       </c>
       <c r="F4" t="n">
-        <v>16992</v>
+        <v>17081</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17524</v>
+        <v>17445</v>
       </c>
       <c r="D5" t="n">
-        <v>10976</v>
+        <v>12028</v>
       </c>
       <c r="E5" t="n">
-        <v>911248</v>
+        <v>18352140</v>
       </c>
       <c r="F5" t="n">
-        <v>16948</v>
+        <v>16992</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17521</v>
+        <v>17524</v>
       </c>
       <c r="D6" t="n">
-        <v>10924</v>
+        <v>10976</v>
       </c>
       <c r="E6" t="n">
-        <v>16241967</v>
+        <v>911248</v>
       </c>
       <c r="F6" t="n">
-        <v>16945</v>
+        <v>16948</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17395</v>
+        <v>17521</v>
       </c>
       <c r="D7" t="n">
-        <v>9997</v>
+        <v>10924</v>
       </c>
       <c r="E7" t="n">
-        <v>11741625</v>
+        <v>16241967</v>
       </c>
       <c r="F7" t="n">
-        <v>16892</v>
+        <v>16945</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17242</v>
+        <v>17395</v>
       </c>
       <c r="D8" t="n">
-        <v>9322</v>
+        <v>9997</v>
       </c>
       <c r="E8" t="n">
-        <v>4103596</v>
+        <v>11741625</v>
       </c>
       <c r="F8" t="n">
-        <v>16856</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17046</v>
+        <v>17242</v>
       </c>
       <c r="D9" t="n">
-        <v>9084</v>
+        <v>9322</v>
       </c>
       <c r="E9" t="n">
-        <v>7057044</v>
+        <v>4103596</v>
       </c>
       <c r="F9" t="n">
-        <v>16846</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17069</v>
+        <v>17046</v>
       </c>
       <c r="D10" t="n">
-        <v>8670</v>
+        <v>9084</v>
       </c>
       <c r="E10" t="n">
-        <v>392587</v>
+        <v>7057044</v>
       </c>
       <c r="F10" t="n">
-        <v>16836</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17020</v>
+        <v>17069</v>
       </c>
       <c r="D11" t="n">
-        <v>8647</v>
+        <v>8670</v>
       </c>
       <c r="E11" t="n">
-        <v>5905940</v>
+        <v>392587</v>
       </c>
       <c r="F11" t="n">
-        <v>16835</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17053</v>
+        <v>17020</v>
       </c>
       <c r="D12" t="n">
-        <v>8300</v>
+        <v>8647</v>
       </c>
       <c r="E12" t="n">
-        <v>2660268</v>
+        <v>5905940</v>
       </c>
       <c r="F12" t="n">
-        <v>16828</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,151 +729,175 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>16919</v>
+        <v>17053</v>
       </c>
       <c r="D13" t="n">
-        <v>8144</v>
+        <v>8300</v>
       </c>
       <c r="E13" t="n">
-        <v>10016048</v>
+        <v>2660268</v>
       </c>
       <c r="F13" t="n">
-        <v>16823</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C14" t="n">
-        <v>17010</v>
+        <v>16919</v>
       </c>
       <c r="D14" t="n">
-        <v>7552</v>
+        <v>8144</v>
       </c>
       <c r="E14" t="n">
-        <v>5239080</v>
+        <v>10016048</v>
       </c>
       <c r="F14" t="n">
-        <v>16816</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>202112</v>
       </c>
       <c r="C15" t="n">
-        <v>17038</v>
+        <v>17010</v>
       </c>
       <c r="D15" t="n">
-        <v>7244</v>
+        <v>7552</v>
       </c>
       <c r="E15" t="n">
-        <v>3799474</v>
+        <v>5239080</v>
       </c>
       <c r="F15" t="n">
-        <v>16808</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>202112</v>
       </c>
       <c r="C16" t="n">
-        <v>17014</v>
+        <v>17038</v>
       </c>
       <c r="D16" t="n">
-        <v>7021</v>
+        <v>7244</v>
       </c>
       <c r="E16" t="n">
-        <v>4968088</v>
+        <v>3799474</v>
       </c>
       <c r="F16" t="n">
-        <v>16800</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>202112</v>
       </c>
       <c r="C17" t="n">
-        <v>16864</v>
+        <v>17014</v>
       </c>
       <c r="D17" t="n">
-        <v>6729</v>
+        <v>7021</v>
       </c>
       <c r="E17" t="n">
-        <v>4401504</v>
+        <v>4968088</v>
       </c>
       <c r="F17" t="n">
-        <v>16791</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>202112</v>
       </c>
       <c r="C18" t="n">
-        <v>16828</v>
+        <v>16864</v>
       </c>
       <c r="D18" t="n">
-        <v>6468</v>
+        <v>6729</v>
       </c>
       <c r="E18" t="n">
-        <v>3449740</v>
+        <v>4401504</v>
       </c>
       <c r="F18" t="n">
-        <v>16788</v>
+        <v>16791</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/22</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>202112</v>
       </c>
       <c r="C19" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F19" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C20" t="n">
         <v>16789</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D20" t="n">
         <v>6263</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E20" t="n">
         <v>105139507</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F20" t="n">
         <v>16789</v>
       </c>
     </row>
-    <row r="20"/>
+    <row r="21"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -886,7 +910,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -913,140 +937,150 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1061,7 +1095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -1093,182 +1127,195 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C2" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C3" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C6" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C7" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C9" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C11" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C12" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C13" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C14" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C15" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>24.64</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1283,7 +1330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
@@ -1310,130 +1357,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1449,7 +1506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1543,574 +1600,620 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C2" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D2" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E2" t="n">
-        <v>279</v>
+        <v>81</v>
       </c>
       <c r="F2" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G2" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H2" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I2" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J2" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K2" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L2" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M2" t="n">
-        <v>-2084</v>
+        <v>375</v>
       </c>
       <c r="N2" t="n">
-        <v>-466</v>
+        <v>-301</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C3" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D3" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E3" t="n">
-        <v>400</v>
+        <v>279</v>
       </c>
       <c r="F3" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G3" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H3" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I3" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J3" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K3" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L3" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M3" t="n">
-        <v>-932</v>
+        <v>-2084</v>
       </c>
       <c r="N3" t="n">
-        <v>-1147</v>
+        <v>-466</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C4" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D4" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E4" t="n">
-        <v>-7</v>
+        <v>400</v>
       </c>
       <c r="F4" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G4" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H4" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I4" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J4" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K4" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L4" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M4" t="n">
-        <v>-1075</v>
+        <v>-932</v>
       </c>
       <c r="N4" t="n">
-        <v>389</v>
+        <v>-1147</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C5" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D5" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E5" t="n">
-        <v>351</v>
+        <v>-7</v>
       </c>
       <c r="F5" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G5" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H5" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I5" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J5" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K5" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L5" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M5" t="n">
-        <v>-553</v>
+        <v>-1075</v>
       </c>
       <c r="N5" t="n">
-        <v>3054</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C6" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D6" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E6" t="n">
-        <v>-595</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>39366</v>
+        <v>351</v>
+      </c>
+      <c r="F6" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G6" t="n">
+        <v>40270</v>
       </c>
       <c r="H6" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I6" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J6" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K6" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L6" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M6" t="n">
-        <v>2382</v>
+        <v>-553</v>
       </c>
       <c r="N6" t="n">
-        <v>-1964</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C7" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D7" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E7" t="n">
-        <v>-3421</v>
+        <v>-595</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H7" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I7" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J7" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K7" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L7" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M7" t="n">
-        <v>-1628</v>
+        <v>2382</v>
       </c>
       <c r="N7" t="n">
-        <v>1074</v>
+        <v>-1964</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C8" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D8" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E8" t="n">
-        <v>-4983</v>
+        <v>-3421</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H8" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I8" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J8" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K8" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L8" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M8" t="n">
-        <v>-5246</v>
+        <v>-1628</v>
       </c>
       <c r="N8" t="n">
-        <v>2227</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C9" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D9" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E9" t="n">
-        <v>-3179</v>
+        <v>-4983</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H9" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I9" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J9" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K9" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L9" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M9" t="n">
-        <v>-4728</v>
+        <v>-5246</v>
       </c>
       <c r="N9" t="n">
-        <v>6006</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C10" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-4728</v>
+      </c>
+      <c r="N10" t="n">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B11" t="n">
         <v>45267</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C11" t="n">
         <v>49710</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>-1089</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E11" t="n">
         <v>-6796</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F11" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G11" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H11" t="n">
         <v>-751</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I11" t="n">
         <v>-1660</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J11" t="n">
         <v>-21534</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K11" t="n">
         <v>909</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L11" t="n">
         <v>-338</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M11" t="n">
         <v>-5136</v>
       </c>
-      <c r="N10" t="n">
+      <c r="N11" t="n">
         <v>4798</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C11" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D11" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E11" t="n">
-        <v>793</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J11" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N11" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C12" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D12" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E12" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H12" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I12" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J12" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K12" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L12" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M12" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N12" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C13" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D13" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E13" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H13" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I13" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J13" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K13" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L13" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M13" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N13" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C14" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I14" t="n">
+        <v>557</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N14" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>42514</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>51801</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F15" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G15" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J15" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/17 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17680</v>
+        <v>17764</v>
       </c>
       <c r="D2" t="n">
-        <v>55055</v>
+        <v>67327</v>
       </c>
       <c r="E2" t="n">
-        <v>352344720</v>
+        <v>217999808</v>
       </c>
       <c r="F2" t="n">
-        <v>17510</v>
+        <v>17556</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17647</v>
+        <v>17680</v>
       </c>
       <c r="D3" t="n">
-        <v>35126</v>
+        <v>55055</v>
       </c>
       <c r="E3" t="n">
-        <v>364728196</v>
+        <v>352344720</v>
       </c>
       <c r="F3" t="n">
-        <v>17414</v>
+        <v>17510</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17524</v>
+        <v>17647</v>
       </c>
       <c r="D4" t="n">
-        <v>14458</v>
+        <v>35126</v>
       </c>
       <c r="E4" t="n">
-        <v>42583320</v>
+        <v>364728196</v>
       </c>
       <c r="F4" t="n">
-        <v>17081</v>
+        <v>17414</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17445</v>
+        <v>17524</v>
       </c>
       <c r="D5" t="n">
-        <v>12028</v>
+        <v>14458</v>
       </c>
       <c r="E5" t="n">
-        <v>18352140</v>
+        <v>42583320</v>
       </c>
       <c r="F5" t="n">
-        <v>16992</v>
+        <v>17081</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17524</v>
+        <v>17445</v>
       </c>
       <c r="D6" t="n">
-        <v>10976</v>
+        <v>12028</v>
       </c>
       <c r="E6" t="n">
-        <v>911248</v>
+        <v>18352140</v>
       </c>
       <c r="F6" t="n">
-        <v>16948</v>
+        <v>16992</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17521</v>
+        <v>17524</v>
       </c>
       <c r="D7" t="n">
-        <v>10924</v>
+        <v>10976</v>
       </c>
       <c r="E7" t="n">
-        <v>16241967</v>
+        <v>911248</v>
       </c>
       <c r="F7" t="n">
-        <v>16945</v>
+        <v>16948</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17395</v>
+        <v>17521</v>
       </c>
       <c r="D8" t="n">
-        <v>9997</v>
+        <v>10924</v>
       </c>
       <c r="E8" t="n">
-        <v>11741625</v>
+        <v>16241967</v>
       </c>
       <c r="F8" t="n">
-        <v>16892</v>
+        <v>16945</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17242</v>
+        <v>17395</v>
       </c>
       <c r="D9" t="n">
-        <v>9322</v>
+        <v>9997</v>
       </c>
       <c r="E9" t="n">
-        <v>4103596</v>
+        <v>11741625</v>
       </c>
       <c r="F9" t="n">
-        <v>16856</v>
+        <v>16892</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17046</v>
+        <v>17242</v>
       </c>
       <c r="D10" t="n">
-        <v>9084</v>
+        <v>9322</v>
       </c>
       <c r="E10" t="n">
-        <v>7057044</v>
+        <v>4103596</v>
       </c>
       <c r="F10" t="n">
-        <v>16846</v>
+        <v>16856</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17069</v>
+        <v>17046</v>
       </c>
       <c r="D11" t="n">
-        <v>8670</v>
+        <v>9084</v>
       </c>
       <c r="E11" t="n">
-        <v>392587</v>
+        <v>7057044</v>
       </c>
       <c r="F11" t="n">
-        <v>16836</v>
+        <v>16846</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17020</v>
+        <v>17069</v>
       </c>
       <c r="D12" t="n">
-        <v>8647</v>
+        <v>8670</v>
       </c>
       <c r="E12" t="n">
-        <v>5905940</v>
+        <v>392587</v>
       </c>
       <c r="F12" t="n">
-        <v>16835</v>
+        <v>16836</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17053</v>
+        <v>17020</v>
       </c>
       <c r="D13" t="n">
-        <v>8300</v>
+        <v>8647</v>
       </c>
       <c r="E13" t="n">
-        <v>2660268</v>
+        <v>5905940</v>
       </c>
       <c r="F13" t="n">
-        <v>16828</v>
+        <v>16835</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,151 +753,175 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>16919</v>
+        <v>17053</v>
       </c>
       <c r="D14" t="n">
-        <v>8144</v>
+        <v>8300</v>
       </c>
       <c r="E14" t="n">
-        <v>10016048</v>
+        <v>2660268</v>
       </c>
       <c r="F14" t="n">
-        <v>16823</v>
+        <v>16828</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>202112</v>
+          <t>日期：2021/10/29</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>202112</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>17010</v>
+        <v>16919</v>
       </c>
       <c r="D15" t="n">
-        <v>7552</v>
+        <v>8144</v>
       </c>
       <c r="E15" t="n">
-        <v>5239080</v>
+        <v>10016048</v>
       </c>
       <c r="F15" t="n">
-        <v>16816</v>
+        <v>16823</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/10/27</t>
+          <t>日期：2021/10/28</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>202112</v>
       </c>
       <c r="C16" t="n">
-        <v>17038</v>
+        <v>17010</v>
       </c>
       <c r="D16" t="n">
-        <v>7244</v>
+        <v>7552</v>
       </c>
       <c r="E16" t="n">
-        <v>3799474</v>
+        <v>5239080</v>
       </c>
       <c r="F16" t="n">
-        <v>16808</v>
+        <v>16816</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/10/26</t>
+          <t>日期：2021/10/27</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>202112</v>
       </c>
       <c r="C17" t="n">
-        <v>17014</v>
+        <v>17038</v>
       </c>
       <c r="D17" t="n">
-        <v>7021</v>
+        <v>7244</v>
       </c>
       <c r="E17" t="n">
-        <v>4968088</v>
+        <v>3799474</v>
       </c>
       <c r="F17" t="n">
-        <v>16800</v>
+        <v>16808</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/10/25</t>
+          <t>日期：2021/10/26</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>202112</v>
       </c>
       <c r="C18" t="n">
-        <v>16864</v>
+        <v>17014</v>
       </c>
       <c r="D18" t="n">
-        <v>6729</v>
+        <v>7021</v>
       </c>
       <c r="E18" t="n">
-        <v>4401504</v>
+        <v>4968088</v>
       </c>
       <c r="F18" t="n">
-        <v>16791</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/10/22</t>
+          <t>日期：2021/10/25</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>202112</v>
       </c>
       <c r="C19" t="n">
-        <v>16828</v>
+        <v>16864</v>
       </c>
       <c r="D19" t="n">
-        <v>6468</v>
+        <v>6729</v>
       </c>
       <c r="E19" t="n">
-        <v>3449740</v>
+        <v>4401504</v>
       </c>
       <c r="F19" t="n">
-        <v>16788</v>
+        <v>16791</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/10/21</t>
+          <t>日期：2021/10/22</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>202112</v>
       </c>
       <c r="C20" t="n">
+        <v>16828</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6468</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3449740</v>
+      </c>
+      <c r="F20" t="n">
+        <v>16788</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>日期：2021/10/21</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C21" t="n">
         <v>16789</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>6263</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E21" t="n">
         <v>105139507</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F21" t="n">
         <v>16789</v>
       </c>
     </row>
-    <row r="21"/>
+    <row r="22"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -910,7 +934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -937,150 +961,160 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B17" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1095,7 +1129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -1127,195 +1161,208 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C2" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C3" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C4" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C6" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C7" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C8" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C10" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C12" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C13" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C14" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C15" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C16" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B17" t="n">
         <v>24.64</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C17" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1330,7 +1377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
@@ -1357,140 +1404,150 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1506,7 +1563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1600,620 +1657,666 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C2" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D2" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E2" t="n">
-        <v>81</v>
+        <v>-3921</v>
       </c>
       <c r="F2" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G2" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H2" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I2" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J2" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K2" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L2" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M2" t="n">
-        <v>375</v>
+        <v>2338</v>
       </c>
       <c r="N2" t="n">
-        <v>-301</v>
+        <v>-494</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C3" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D3" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E3" t="n">
-        <v>279</v>
+        <v>81</v>
       </c>
       <c r="F3" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G3" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H3" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I3" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J3" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K3" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L3" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M3" t="n">
-        <v>-2084</v>
+        <v>375</v>
       </c>
       <c r="N3" t="n">
-        <v>-466</v>
+        <v>-301</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C4" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D4" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E4" t="n">
-        <v>400</v>
+        <v>279</v>
       </c>
       <c r="F4" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G4" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H4" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I4" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J4" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K4" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L4" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M4" t="n">
-        <v>-932</v>
+        <v>-2084</v>
       </c>
       <c r="N4" t="n">
-        <v>-1147</v>
+        <v>-466</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C5" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D5" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E5" t="n">
-        <v>-7</v>
+        <v>400</v>
       </c>
       <c r="F5" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G5" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H5" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I5" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J5" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K5" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L5" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M5" t="n">
-        <v>-1075</v>
+        <v>-932</v>
       </c>
       <c r="N5" t="n">
-        <v>389</v>
+        <v>-1147</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C6" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D6" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E6" t="n">
-        <v>351</v>
+        <v>-7</v>
       </c>
       <c r="F6" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G6" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H6" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I6" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J6" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K6" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L6" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M6" t="n">
-        <v>-553</v>
+        <v>-1075</v>
       </c>
       <c r="N6" t="n">
-        <v>3054</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C7" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D7" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E7" t="n">
-        <v>-595</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>39366</v>
+        <v>351</v>
+      </c>
+      <c r="F7" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G7" t="n">
+        <v>40270</v>
       </c>
       <c r="H7" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I7" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J7" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K7" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L7" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M7" t="n">
-        <v>2382</v>
+        <v>-553</v>
       </c>
       <c r="N7" t="n">
-        <v>-1964</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C8" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D8" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E8" t="n">
-        <v>-3421</v>
+        <v>-595</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H8" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I8" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J8" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K8" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L8" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M8" t="n">
-        <v>-1628</v>
+        <v>2382</v>
       </c>
       <c r="N8" t="n">
-        <v>1074</v>
+        <v>-1964</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C9" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D9" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E9" t="n">
-        <v>-4983</v>
+        <v>-3421</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H9" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I9" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J9" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K9" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L9" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M9" t="n">
-        <v>-5246</v>
+        <v>-1628</v>
       </c>
       <c r="N9" t="n">
-        <v>2227</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C10" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D10" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E10" t="n">
-        <v>-3179</v>
+        <v>-4983</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H10" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I10" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J10" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K10" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L10" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M10" t="n">
-        <v>-4728</v>
+        <v>-5246</v>
       </c>
       <c r="N10" t="n">
-        <v>6006</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-3179</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-4728</v>
+      </c>
+      <c r="N11" t="n">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B12" t="n">
         <v>45267</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C12" t="n">
         <v>49710</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>-1089</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E12" t="n">
         <v>-6796</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F12" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G12" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H12" t="n">
         <v>-751</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I12" t="n">
         <v>-1660</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J12" t="n">
         <v>-21534</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K12" t="n">
         <v>909</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L12" t="n">
         <v>-338</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M12" t="n">
         <v>-5136</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N12" t="n">
         <v>4798</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C12" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E12" t="n">
-        <v>793</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J12" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M12" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N12" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C13" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D13" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E13" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H13" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I13" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J13" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K13" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L13" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M13" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N13" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C14" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D14" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E14" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H14" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I14" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J14" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K14" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L14" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M14" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N14" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C15" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I15" t="n">
+        <v>557</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M15" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N15" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>42514</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>51801</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F16" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G16" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J16" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/22 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,13 +405,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="18.375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,42 +465,67 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D2" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E2" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F2" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F3" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>17813</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>2560</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E4" t="n">
         <v>45601280</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F4" t="n">
         <v>17813</v>
       </c>
     </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -513,13 +538,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="19.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -540,180 +565,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B20" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -728,13 +763,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="17.125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.375" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -760,234 +795,247 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C4" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C5" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C6" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C7" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C10" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C11" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C13" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C15" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C16" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C17" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C18" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C19" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B20" t="n">
         <v>24.64</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C20" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1002,13 +1050,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.75" customWidth="1" min="1" max="1"/>
     <col width="16.5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -1029,170 +1077,180 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B19" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1208,13 +1266,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.25" bestFit="1" customWidth="1" min="2" max="3"/>
@@ -1302,758 +1360,804 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C2" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D2" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E2" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F2" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G2" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H2" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I2" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J2" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K2" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L2" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M2" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N2" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C3" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D3" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E3" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F3" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G3" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H3" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I3" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J3" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K3" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L3" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M3" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N3" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C4" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D4" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E4" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F4" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G4" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H4" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I4" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J4" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K4" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L4" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M4" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N4" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C5" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D5" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E5" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F5" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G5" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H5" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I5" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J5" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K5" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L5" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M5" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N5" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C6" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D6" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E6" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F6" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G6" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H6" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I6" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J6" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K6" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L6" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M6" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N6" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C7" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D7" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E7" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F7" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G7" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H7" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I7" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J7" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K7" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L7" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M7" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N7" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C8" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D8" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E8" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F8" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G8" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H8" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I8" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J8" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K8" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L8" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M8" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N8" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C9" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D9" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E9" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F9" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G9" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H9" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I9" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J9" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K9" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L9" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M9" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N9" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C10" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D10" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E10" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F10" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G10" t="n">
+        <v>40270</v>
       </c>
       <c r="H10" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I10" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J10" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K10" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L10" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M10" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N10" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C11" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D11" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E11" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H11" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I11" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J11" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K11" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L11" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M11" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N11" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C12" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D12" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E12" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H12" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I12" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J12" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K12" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L12" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M12" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N12" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C13" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D13" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E13" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H13" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I13" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J13" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K13" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L13" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M13" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N13" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C14" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E14" t="n">
+        <v>749</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>45267</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>49710</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>-1089</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>-2353</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F15" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G15" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H15" t="n">
         <v>-751</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I15" t="n">
         <v>-1660</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J15" t="n">
         <v>-21534</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K15" t="n">
         <v>909</v>
       </c>
-      <c r="L14" t="n">
+      <c r="L15" t="n">
         <v>-338</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M15" t="n">
         <v>-693</v>
       </c>
-      <c r="N14" t="n">
+      <c r="N15" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C15" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E15" t="n">
-        <v>793</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J15" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K15" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M15" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N15" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C16" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D16" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E16" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H16" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I16" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J16" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K16" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L16" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M16" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N16" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C17" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D17" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E17" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H17" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I17" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J17" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K17" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L17" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M17" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N17" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C18" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I18" t="n">
+        <v>557</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N18" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B19" t="n">
         <v>42514</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C19" t="n">
         <v>51801</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F19" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G19" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J19" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/23 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D2" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E2" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F2" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,43 +489,67 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D3" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E3" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F3" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F4" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>17813</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>2560</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E5" t="n">
         <v>45601280</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="5"/>
+    <row r="6"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -538,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -565,190 +589,200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B21" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -763,7 +797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -795,247 +829,260 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C2" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C5" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C6" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C7" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C8" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C11" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C12" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C14" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C16" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C17" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C18" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C19" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C20" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B21" t="n">
         <v>24.64</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C21" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1050,7 +1097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1077,180 +1124,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B20" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1266,7 +1323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1360,804 +1417,850 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C2" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D2" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E2" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F2" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G2" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H2" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I2" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J2" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K2" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L2" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N2" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C3" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D3" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E3" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F3" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G3" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H3" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I3" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J3" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K3" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L3" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M3" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N3" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C4" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D4" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E4" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F4" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G4" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H4" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I4" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J4" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K4" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L4" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M4" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N4" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C5" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D5" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E5" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F5" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G5" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H5" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I5" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J5" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K5" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L5" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M5" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N5" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C6" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D6" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E6" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F6" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G6" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H6" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I6" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J6" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K6" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L6" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M6" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N6" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C7" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D7" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E7" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F7" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G7" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H7" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I7" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J7" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K7" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L7" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M7" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N7" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C8" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D8" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E8" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F8" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G8" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H8" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I8" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J8" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K8" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L8" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M8" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N8" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C9" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D9" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E9" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F9" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G9" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H9" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I9" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J9" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K9" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L9" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M9" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N9" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C10" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D10" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E10" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F10" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G10" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H10" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I10" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J10" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K10" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L10" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M10" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N10" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C11" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D11" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E11" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F11" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G11" t="n">
+        <v>40270</v>
       </c>
       <c r="H11" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I11" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J11" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K11" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L11" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M11" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N11" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C12" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D12" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E12" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H12" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I12" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J12" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K12" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L12" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M12" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N12" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C13" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D13" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E13" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H13" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I13" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J13" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K13" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L13" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M13" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N13" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C14" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D14" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E14" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H14" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I14" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J14" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K14" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L14" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M14" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N14" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C15" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E15" t="n">
+        <v>749</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M15" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>45267</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>49710</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" t="n">
         <v>-1089</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E16" t="n">
         <v>-2353</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F16" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G16" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H16" t="n">
         <v>-751</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I16" t="n">
         <v>-1660</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J16" t="n">
         <v>-21534</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K16" t="n">
         <v>909</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L16" t="n">
         <v>-338</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M16" t="n">
         <v>-693</v>
       </c>
-      <c r="N15" t="n">
+      <c r="N16" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C16" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E16" t="n">
-        <v>793</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H16" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J16" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K16" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M16" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N16" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C17" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D17" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E17" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H17" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I17" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J17" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K17" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L17" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M17" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N17" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C18" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D18" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E18" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H18" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I18" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J18" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K18" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L18" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M18" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N18" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C19" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I19" t="n">
+        <v>557</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N19" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B20" t="n">
         <v>42514</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C20" t="n">
         <v>51801</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F20" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G20" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J20" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/24 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D2" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E2" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F2" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D3" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E3" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F3" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,43 +513,67 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D4" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E4" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F4" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F5" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>17813</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>2560</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>45601280</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F6" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="6"/>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -562,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -589,200 +613,210 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B22" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -797,7 +831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -829,260 +863,273 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C2" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C3" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C6" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C7" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C8" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C9" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C12" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C13" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C15" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C17" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C18" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C19" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C20" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C21" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B22" t="n">
         <v>24.64</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C22" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1097,7 +1144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1124,190 +1171,200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B21" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1323,7 +1380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1417,850 +1474,896 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C2" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D2" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E2" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F2" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G2" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H2" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I2" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J2" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K2" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L2" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M2" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N2" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C3" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D3" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E3" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F3" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G3" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H3" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I3" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J3" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K3" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L3" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M3" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N3" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C4" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D4" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E4" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F4" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G4" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H4" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I4" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J4" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K4" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L4" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M4" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N4" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C5" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D5" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E5" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F5" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G5" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H5" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I5" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J5" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K5" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L5" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M5" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N5" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C6" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D6" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E6" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F6" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G6" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H6" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I6" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J6" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K6" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L6" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M6" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N6" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C7" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D7" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E7" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F7" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G7" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H7" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I7" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J7" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K7" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L7" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M7" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N7" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C8" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D8" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E8" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F8" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G8" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H8" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I8" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J8" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K8" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L8" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M8" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N8" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C9" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D9" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E9" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F9" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G9" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H9" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I9" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J9" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K9" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L9" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M9" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N9" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C10" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D10" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E10" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F10" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G10" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H10" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I10" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J10" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K10" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L10" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M10" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N10" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C11" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D11" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E11" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F11" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G11" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H11" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I11" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J11" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K11" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L11" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M11" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N11" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C12" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D12" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E12" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F12" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G12" t="n">
+        <v>40270</v>
       </c>
       <c r="H12" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I12" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J12" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K12" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L12" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M12" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N12" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C13" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D13" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E13" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H13" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I13" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J13" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K13" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L13" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M13" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N13" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C14" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D14" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E14" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H14" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I14" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J14" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K14" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L14" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M14" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N14" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C15" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D15" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E15" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H15" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I15" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J15" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K15" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L15" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M15" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N15" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C16" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E16" t="n">
+        <v>749</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B17" t="n">
         <v>45267</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C17" t="n">
         <v>49710</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D17" t="n">
         <v>-1089</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E17" t="n">
         <v>-2353</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F17" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G17" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H17" t="n">
         <v>-751</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I17" t="n">
         <v>-1660</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J17" t="n">
         <v>-21534</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K17" t="n">
         <v>909</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L17" t="n">
         <v>-338</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M17" t="n">
         <v>-693</v>
       </c>
-      <c r="N16" t="n">
+      <c r="N17" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C17" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E17" t="n">
-        <v>793</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I17" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J17" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K17" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M17" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C18" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D18" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E18" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H18" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I18" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J18" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K18" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L18" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M18" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N18" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C19" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D19" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E19" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H19" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I19" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J19" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K19" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L19" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M19" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N19" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C20" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I20" t="n">
+        <v>557</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N20" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B21" t="n">
         <v>42514</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C21" t="n">
         <v>51801</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F21" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G21" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J21" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/25 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D2" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E2" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F2" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D3" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E3" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F3" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D4" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E4" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F4" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,43 +537,67 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D5" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E5" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F5" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F6" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C7" t="n">
         <v>17813</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>2560</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E7" t="n">
         <v>45601280</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F7" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="7"/>
+    <row r="8"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -586,7 +610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -613,210 +637,220 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -831,7 +865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -863,273 +897,286 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C2" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C3" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C4" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C7" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C8" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C9" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C10" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C13" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C14" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C16" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C18" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C19" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C20" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C21" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C22" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>24.64</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C23" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1144,7 +1191,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1171,200 +1218,210 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B22" t="n">
         <v>17054.47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/26 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D2" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E2" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F2" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D3" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E3" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F3" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D4" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E4" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F4" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D5" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E5" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F5" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,43 +561,67 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D6" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E6" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F6" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F7" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C8" t="n">
         <v>17813</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>2560</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E8" t="n">
         <v>45601280</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F8" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="8"/>
+    <row r="9"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -610,7 +634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -637,220 +661,230 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -865,7 +899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -897,286 +931,299 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C2" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C3" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C5" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C8" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C9" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C10" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C11" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C13" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C14" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C15" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C16" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C17" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C19" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C20" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C21" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C22" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C23" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>24.64</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C24" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1191,7 +1238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1218,210 +1265,220 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1437,7 +1494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1531,896 +1588,942 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C2" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D2" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E2" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F2" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G2" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H2" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I2" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J2" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K2" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L2" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M2" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N2" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C3" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D3" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E3" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F3" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G3" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H3" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I3" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J3" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K3" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L3" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M3" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N3" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C4" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D4" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E4" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F4" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G4" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H4" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I4" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J4" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K4" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L4" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M4" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N4" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C5" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D5" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E5" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F5" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G5" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H5" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I5" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J5" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K5" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L5" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M5" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N5" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C6" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D6" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E6" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F6" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G6" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H6" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I6" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J6" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K6" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L6" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M6" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N6" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C7" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D7" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E7" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F7" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G7" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H7" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I7" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J7" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K7" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L7" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M7" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N7" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C8" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D8" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E8" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F8" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G8" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H8" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I8" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J8" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K8" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L8" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M8" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N8" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C9" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D9" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E9" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F9" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G9" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H9" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I9" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J9" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K9" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L9" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M9" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N9" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C10" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D10" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E10" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F10" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G10" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H10" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I10" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J10" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K10" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L10" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M10" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N10" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C11" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D11" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E11" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F11" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G11" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H11" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I11" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J11" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K11" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L11" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M11" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N11" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C12" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D12" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E12" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F12" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G12" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H12" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I12" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J12" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K12" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L12" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M12" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N12" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C13" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D13" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E13" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F13" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G13" t="n">
+        <v>40270</v>
       </c>
       <c r="H13" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I13" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J13" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K13" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L13" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M13" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N13" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C14" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D14" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E14" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H14" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I14" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J14" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K14" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L14" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M14" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N14" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C15" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D15" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E15" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H15" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I15" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J15" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K15" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L15" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M15" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N15" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C16" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D16" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E16" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H16" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I16" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J16" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K16" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L16" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M16" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N16" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C17" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E17" t="n">
+        <v>749</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M17" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B18" t="n">
         <v>45267</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C18" t="n">
         <v>49710</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>-1089</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>-2353</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F18" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G18" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H18" t="n">
         <v>-751</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I18" t="n">
         <v>-1660</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J18" t="n">
         <v>-21534</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K18" t="n">
         <v>909</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L18" t="n">
         <v>-338</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M18" t="n">
         <v>-693</v>
       </c>
-      <c r="N17" t="n">
+      <c r="N18" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C18" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D18" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E18" t="n">
-        <v>793</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H18" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J18" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K18" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M18" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N18" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C19" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D19" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E19" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H19" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I19" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J19" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K19" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L19" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M19" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N19" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C20" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D20" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E20" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H20" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I20" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J20" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K20" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L20" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M20" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N20" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C21" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I21" t="n">
+        <v>557</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L21" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N21" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B22" t="n">
         <v>42514</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C22" t="n">
         <v>51801</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F22" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G22" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J22" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/29 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D2" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E2" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F2" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D3" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E3" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F3" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D4" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E4" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F4" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D5" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E5" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F5" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D6" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E6" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F6" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,43 +585,67 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D7" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E7" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F7" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F8" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C9" t="n">
         <v>17813</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>2560</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" t="n">
         <v>45601280</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F9" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="9"/>
+    <row r="10"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -634,7 +658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -661,230 +685,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B25" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -899,7 +933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -931,299 +965,312 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C2" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C3" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C4" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C5" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C6" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C9" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C10" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C11" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C12" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C14" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C15" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C16" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C17" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C18" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C20" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C21" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C22" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C23" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C24" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B25" t="n">
         <v>24.64</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C25" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1238,7 +1285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1265,220 +1312,230 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1494,7 +1551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1588,942 +1645,988 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C2" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D2" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E2" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F2" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G2" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H2" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I2" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J2" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K2" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L2" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M2" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N2" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C3" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D3" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E3" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F3" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G3" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H3" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I3" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J3" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K3" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L3" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M3" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N3" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C4" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D4" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E4" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F4" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G4" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H4" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I4" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J4" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K4" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L4" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M4" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N4" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C5" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D5" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E5" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F5" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G5" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H5" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I5" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J5" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K5" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L5" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M5" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N5" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C6" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D6" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E6" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F6" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G6" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H6" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I6" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J6" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K6" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L6" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M6" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N6" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C7" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D7" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E7" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F7" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G7" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H7" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I7" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J7" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K7" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L7" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M7" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N7" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C8" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D8" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E8" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F8" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G8" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H8" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I8" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J8" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K8" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L8" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M8" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N8" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C9" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D9" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E9" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F9" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G9" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H9" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I9" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J9" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K9" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L9" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M9" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N9" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C10" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D10" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E10" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F10" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G10" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H10" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I10" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J10" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K10" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L10" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M10" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N10" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C11" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D11" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E11" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F11" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G11" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H11" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I11" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J11" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K11" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L11" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M11" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N11" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C12" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D12" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E12" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F12" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G12" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H12" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I12" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J12" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K12" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L12" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M12" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N12" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C13" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D13" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E13" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F13" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G13" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H13" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I13" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J13" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K13" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L13" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M13" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N13" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C14" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D14" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E14" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F14" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G14" t="n">
+        <v>40270</v>
       </c>
       <c r="H14" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I14" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J14" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K14" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L14" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M14" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N14" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C15" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D15" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E15" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H15" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I15" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J15" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K15" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L15" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M15" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N15" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C16" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D16" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E16" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H16" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I16" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J16" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K16" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L16" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M16" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N16" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C17" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D17" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E17" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H17" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I17" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J17" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K17" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L17" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M17" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N17" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C18" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E18" t="n">
+        <v>749</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B19" t="n">
         <v>45267</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C19" t="n">
         <v>49710</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>-1089</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E19" t="n">
         <v>-2353</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F19" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G19" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H19" t="n">
         <v>-751</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I19" t="n">
         <v>-1660</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J19" t="n">
         <v>-21534</v>
       </c>
-      <c r="K18" t="n">
+      <c r="K19" t="n">
         <v>909</v>
       </c>
-      <c r="L18" t="n">
+      <c r="L19" t="n">
         <v>-338</v>
       </c>
-      <c r="M18" t="n">
+      <c r="M19" t="n">
         <v>-693</v>
       </c>
-      <c r="N18" t="n">
+      <c r="N19" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C19" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E19" t="n">
-        <v>793</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I19" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J19" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K19" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M19" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N19" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C20" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D20" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E20" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H20" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I20" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J20" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K20" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L20" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M20" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N20" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C21" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D21" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E21" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H21" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I21" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J21" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K21" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L21" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M21" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N21" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C22" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I22" t="n">
+        <v>557</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L22" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N22" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>42514</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C23" t="n">
         <v>51801</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F23" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G23" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J23" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/11/30 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D2" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E2" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F2" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D3" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E3" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F3" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D4" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E4" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F4" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D5" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E5" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F5" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D6" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E6" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F6" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D7" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E7" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F7" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,43 +609,67 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D8" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E8" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F8" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F9" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>17813</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>2560</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>45601280</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="10"/>
+    <row r="11"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -658,7 +682,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -685,240 +709,250 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B26" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -933,7 +967,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -965,312 +999,325 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C2" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C3" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C4" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C5" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C6" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C7" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C10" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C11" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C12" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C13" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C15" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C16" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C17" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C18" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C19" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C21" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C22" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C23" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C24" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C25" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B26" t="n">
         <v>24.64</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C26" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1285,7 +1332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1312,230 +1359,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B25" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1551,7 +1608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1645,988 +1702,1034 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C2" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D2" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E2" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F2" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G2" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H2" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I2" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J2" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K2" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L2" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M2" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N2" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C3" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D3" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E3" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F3" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G3" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H3" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I3" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J3" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K3" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L3" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M3" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N3" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C4" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D4" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E4" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F4" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G4" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H4" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I4" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J4" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K4" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L4" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M4" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N4" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C5" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D5" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E5" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F5" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G5" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H5" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I5" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J5" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K5" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L5" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M5" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N5" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C6" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D6" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E6" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F6" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G6" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H6" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I6" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J6" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K6" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L6" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M6" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N6" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C7" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D7" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E7" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F7" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G7" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H7" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I7" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J7" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K7" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L7" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M7" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N7" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C8" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D8" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E8" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F8" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G8" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H8" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I8" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J8" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K8" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L8" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M8" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N8" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C9" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D9" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E9" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F9" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G9" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H9" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I9" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J9" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K9" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L9" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M9" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N9" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C10" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D10" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E10" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F10" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G10" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H10" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I10" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J10" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K10" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L10" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M10" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N10" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C11" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D11" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E11" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F11" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G11" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H11" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I11" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J11" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K11" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L11" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M11" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N11" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C12" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D12" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E12" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F12" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G12" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H12" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I12" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J12" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K12" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L12" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M12" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N12" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C13" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D13" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E13" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F13" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G13" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H13" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I13" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J13" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K13" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L13" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M13" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N13" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C14" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D14" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E14" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F14" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G14" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H14" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I14" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J14" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K14" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L14" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M14" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N14" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C15" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D15" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E15" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F15" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G15" t="n">
+        <v>40270</v>
       </c>
       <c r="H15" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I15" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J15" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K15" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L15" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M15" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N15" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C16" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D16" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E16" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H16" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I16" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J16" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K16" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L16" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M16" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N16" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C17" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D17" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E17" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H17" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I17" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J17" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K17" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L17" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M17" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N17" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C18" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D18" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E18" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H18" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I18" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J18" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K18" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L18" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M18" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N18" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C19" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E19" t="n">
+        <v>749</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B20" t="n">
         <v>45267</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C20" t="n">
         <v>49710</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D20" t="n">
         <v>-1089</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E20" t="n">
         <v>-2353</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F20" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G20" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H20" t="n">
         <v>-751</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I20" t="n">
         <v>-1660</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J20" t="n">
         <v>-21534</v>
       </c>
-      <c r="K19" t="n">
+      <c r="K20" t="n">
         <v>909</v>
       </c>
-      <c r="L19" t="n">
+      <c r="L20" t="n">
         <v>-338</v>
       </c>
-      <c r="M19" t="n">
+      <c r="M20" t="n">
         <v>-693</v>
       </c>
-      <c r="N19" t="n">
+      <c r="N20" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C20" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E20" t="n">
-        <v>793</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H20" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I20" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J20" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K20" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M20" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N20" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C21" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D21" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E21" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H21" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I21" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J21" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K21" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L21" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M21" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N21" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C22" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D22" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E22" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H22" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I22" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J22" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K22" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L22" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M22" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N22" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C23" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I23" t="n">
+        <v>557</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L23" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M23" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N23" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>42514</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C24" t="n">
         <v>51801</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F24" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G24" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J24" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/01 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D2" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E2" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F2" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D3" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E3" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F3" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D4" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E4" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F4" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D5" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E5" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F5" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D6" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E6" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F6" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D7" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E7" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F7" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D8" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E8" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F8" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,43 +633,67 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D9" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E9" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F9" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C11" t="n">
         <v>17813</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>2560</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E11" t="n">
         <v>45601280</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F11" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -682,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -709,250 +733,260 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B27" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -967,7 +1001,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -999,325 +1033,338 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C2" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C3" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C4" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C5" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C6" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C7" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C8" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C11" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C12" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C13" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C14" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C17" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C18" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C20" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C22" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C23" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C24" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C25" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C26" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B27" t="n">
         <v>24.64</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C27" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1332,7 +1379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1359,240 +1406,250 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B26" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1608,7 +1665,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1702,1034 +1759,1080 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C2" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D2" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E2" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F2" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G2" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H2" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I2" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J2" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K2" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L2" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M2" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N2" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C3" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D3" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E3" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F3" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G3" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H3" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I3" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J3" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K3" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L3" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M3" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N3" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C4" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D4" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E4" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F4" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G4" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H4" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I4" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J4" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K4" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L4" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M4" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N4" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C5" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D5" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E5" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F5" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G5" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H5" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I5" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J5" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K5" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L5" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M5" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N5" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C6" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D6" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E6" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F6" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G6" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H6" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I6" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J6" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K6" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L6" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M6" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N6" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C7" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D7" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E7" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F7" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G7" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H7" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I7" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J7" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K7" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L7" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M7" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N7" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C8" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D8" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E8" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F8" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G8" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H8" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I8" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J8" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K8" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L8" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M8" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N8" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C9" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D9" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E9" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F9" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G9" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H9" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I9" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J9" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K9" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L9" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M9" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N9" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C10" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D10" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E10" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F10" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G10" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H10" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I10" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J10" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K10" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L10" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M10" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N10" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C11" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D11" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E11" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F11" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G11" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H11" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I11" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J11" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K11" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L11" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M11" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N11" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C12" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D12" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E12" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F12" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G12" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H12" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I12" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J12" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K12" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L12" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M12" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N12" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C13" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D13" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E13" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F13" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G13" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H13" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I13" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J13" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K13" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L13" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M13" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N13" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C14" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D14" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E14" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F14" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G14" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H14" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I14" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J14" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K14" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L14" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M14" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N14" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C15" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D15" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E15" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F15" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G15" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H15" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I15" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J15" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K15" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L15" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M15" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N15" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C16" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D16" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E16" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F16" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G16" t="n">
+        <v>40270</v>
       </c>
       <c r="H16" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I16" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J16" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K16" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L16" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M16" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N16" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C17" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D17" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E17" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H17" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I17" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J17" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K17" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L17" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M17" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N17" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C18" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D18" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E18" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H18" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I18" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J18" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K18" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L18" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M18" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N18" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C19" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D19" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E19" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H19" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I19" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J19" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K19" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L19" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M19" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N19" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C20" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E20" t="n">
+        <v>749</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N20" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B21" t="n">
         <v>45267</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C21" t="n">
         <v>49710</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>-1089</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E21" t="n">
         <v>-2353</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F21" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G21" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H21" t="n">
         <v>-751</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I21" t="n">
         <v>-1660</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J21" t="n">
         <v>-21534</v>
       </c>
-      <c r="K20" t="n">
+      <c r="K21" t="n">
         <v>909</v>
       </c>
-      <c r="L20" t="n">
+      <c r="L21" t="n">
         <v>-338</v>
       </c>
-      <c r="M20" t="n">
+      <c r="M21" t="n">
         <v>-693</v>
       </c>
-      <c r="N20" t="n">
+      <c r="N21" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C21" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D21" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E21" t="n">
-        <v>793</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H21" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I21" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J21" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K21" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M21" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N21" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C22" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D22" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E22" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H22" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I22" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J22" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K22" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L22" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M22" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N22" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C23" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D23" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E23" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H23" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I23" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J23" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K23" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L23" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M23" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N23" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C24" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I24" t="n">
+        <v>557</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L24" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N24" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B25" t="n">
         <v>42514</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C25" t="n">
         <v>51801</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F25" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G25" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J25" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/02 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D2" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E2" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F2" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D3" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E3" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F3" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D4" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E4" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F4" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D5" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E5" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F5" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D6" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E6" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F6" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D7" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E7" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F7" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D8" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E8" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F8" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D9" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E9" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F9" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,43 +657,67 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D10" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E10" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F10" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F11" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C12" t="n">
         <v>17813</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>2560</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E12" t="n">
         <v>45601280</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F12" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="12"/>
+    <row r="13"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -706,7 +730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -733,7 +757,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -743,250 +767,260 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B28" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1001,7 +1035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1033,338 +1067,351 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C2" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C3" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C4" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C5" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C6" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C7" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C8" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C9" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C12" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C13" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C14" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C15" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C18" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C19" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C20" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C21" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C22" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C23" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C24" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C25" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C26" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C27" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B28" t="n">
         <v>24.64</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C28" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1379,7 +1426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1406,250 +1453,260 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B27" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1665,7 +1722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1759,1080 +1816,1126 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C2" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D2" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E2" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F2" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G2" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H2" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I2" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J2" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K2" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L2" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M2" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N2" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C3" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D3" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E3" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F3" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G3" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H3" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I3" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J3" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K3" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L3" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M3" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N3" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C4" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D4" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E4" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F4" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G4" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H4" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I4" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J4" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K4" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L4" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M4" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N4" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C5" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D5" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E5" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F5" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G5" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H5" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I5" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J5" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K5" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L5" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M5" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N5" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C6" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D6" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E6" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F6" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G6" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H6" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I6" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J6" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K6" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L6" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M6" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N6" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C7" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D7" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E7" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F7" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G7" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H7" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I7" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J7" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K7" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L7" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M7" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N7" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C8" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D8" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E8" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F8" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G8" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H8" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I8" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J8" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K8" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L8" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M8" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N8" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C9" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D9" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E9" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F9" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G9" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H9" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I9" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J9" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K9" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L9" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M9" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N9" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C10" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D10" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E10" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F10" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G10" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H10" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I10" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J10" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K10" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L10" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M10" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N10" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C11" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D11" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E11" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F11" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G11" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H11" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I11" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J11" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K11" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L11" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M11" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N11" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C12" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D12" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E12" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F12" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G12" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H12" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I12" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J12" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K12" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L12" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M12" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N12" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C13" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D13" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E13" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F13" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G13" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H13" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I13" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J13" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K13" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L13" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M13" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N13" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C14" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D14" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E14" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F14" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G14" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H14" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I14" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J14" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K14" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L14" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M14" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N14" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C15" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D15" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E15" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F15" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G15" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H15" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I15" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J15" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K15" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L15" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M15" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N15" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C16" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D16" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E16" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F16" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G16" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H16" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I16" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J16" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K16" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L16" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M16" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N16" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C17" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D17" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E17" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F17" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G17" t="n">
+        <v>40270</v>
       </c>
       <c r="H17" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I17" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J17" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K17" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L17" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M17" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N17" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C18" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D18" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E18" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H18" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I18" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J18" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K18" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L18" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M18" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N18" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C19" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D19" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E19" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H19" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I19" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J19" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K19" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L19" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M19" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N19" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C20" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D20" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E20" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H20" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I20" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J20" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K20" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L20" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M20" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N20" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C21" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E21" t="n">
+        <v>749</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B22" t="n">
         <v>45267</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C22" t="n">
         <v>49710</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D22" t="n">
         <v>-1089</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E22" t="n">
         <v>-2353</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F22" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G22" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H22" t="n">
         <v>-751</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I22" t="n">
         <v>-1660</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J22" t="n">
         <v>-21534</v>
       </c>
-      <c r="K21" t="n">
+      <c r="K22" t="n">
         <v>909</v>
       </c>
-      <c r="L21" t="n">
+      <c r="L22" t="n">
         <v>-338</v>
       </c>
-      <c r="M21" t="n">
+      <c r="M22" t="n">
         <v>-693</v>
       </c>
-      <c r="N21" t="n">
+      <c r="N22" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C22" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D22" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E22" t="n">
-        <v>793</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I22" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J22" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K22" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L22" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M22" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N22" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C23" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D23" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E23" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H23" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I23" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J23" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K23" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L23" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M23" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N23" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C24" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D24" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E24" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H24" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I24" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J24" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K24" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L24" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M24" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N24" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C25" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I25" t="n">
+        <v>557</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L25" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M25" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N25" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B26" t="n">
         <v>42514</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C26" t="n">
         <v>51801</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F26" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G26" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J26" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/03 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D2" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E2" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F2" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D3" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E3" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F3" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D4" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E4" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F4" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D5" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E5" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F5" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D6" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E6" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F6" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D7" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E7" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F7" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D8" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E8" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F8" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D9" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E9" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F9" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D10" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E10" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F10" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,43 +681,67 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D11" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E11" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F11" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>17813</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>2560</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E13" t="n">
         <v>45601280</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F13" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="13"/>
+    <row r="14"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -730,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -757,17 +781,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -777,250 +801,260 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B29" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1035,7 +1069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1067,351 +1101,364 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C2" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C3" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C4" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C5" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C6" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C7" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C8" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C9" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C10" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C13" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C14" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C15" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C16" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C18" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C19" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C20" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C21" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C22" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C24" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C25" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C26" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C27" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C28" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B29" t="n">
         <v>24.64</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C29" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1426,7 +1473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1453,260 +1500,270 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B28" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1722,7 +1779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1816,1126 +1873,1172 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C2" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D2" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E2" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F2" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G2" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H2" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I2" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J2" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K2" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L2" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M2" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N2" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C3" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D3" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E3" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F3" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G3" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H3" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I3" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J3" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K3" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L3" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M3" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N3" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C4" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D4" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E4" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F4" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G4" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H4" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I4" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J4" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K4" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L4" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M4" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N4" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C5" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D5" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E5" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F5" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G5" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H5" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I5" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J5" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K5" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L5" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M5" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N5" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C6" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D6" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E6" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F6" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G6" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H6" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I6" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J6" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K6" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L6" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M6" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N6" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C7" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D7" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E7" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F7" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G7" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H7" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I7" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J7" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K7" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L7" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M7" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N7" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C8" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D8" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E8" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F8" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G8" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H8" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I8" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J8" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K8" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L8" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M8" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N8" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C9" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D9" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E9" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F9" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G9" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H9" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I9" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J9" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K9" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L9" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M9" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N9" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C10" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D10" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E10" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F10" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G10" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H10" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I10" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J10" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K10" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L10" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M10" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N10" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C11" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D11" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E11" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F11" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G11" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H11" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I11" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J11" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K11" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L11" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M11" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N11" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C12" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D12" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E12" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F12" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G12" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H12" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I12" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J12" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K12" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L12" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M12" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N12" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C13" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D13" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E13" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F13" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G13" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H13" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I13" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J13" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K13" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L13" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M13" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N13" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C14" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D14" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E14" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F14" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G14" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H14" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I14" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J14" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K14" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L14" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M14" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N14" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C15" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D15" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E15" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F15" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G15" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H15" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I15" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J15" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K15" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L15" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M15" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N15" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C16" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D16" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E16" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F16" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G16" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H16" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I16" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J16" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K16" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L16" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M16" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N16" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C17" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D17" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E17" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F17" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G17" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H17" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I17" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J17" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K17" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L17" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M17" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N17" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C18" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D18" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E18" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F18" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G18" t="n">
+        <v>40270</v>
       </c>
       <c r="H18" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I18" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J18" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K18" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L18" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M18" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N18" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C19" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D19" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E19" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H19" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I19" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J19" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K19" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L19" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M19" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N19" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C20" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D20" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E20" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H20" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I20" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J20" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K20" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L20" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M20" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N20" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C21" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D21" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E21" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H21" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I21" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J21" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K21" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L21" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M21" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N21" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C22" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E22" t="n">
+        <v>749</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N22" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>45267</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C23" t="n">
         <v>49710</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D23" t="n">
         <v>-1089</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E23" t="n">
         <v>-2353</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F23" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G23" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H23" t="n">
         <v>-751</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I23" t="n">
         <v>-1660</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J23" t="n">
         <v>-21534</v>
       </c>
-      <c r="K22" t="n">
+      <c r="K23" t="n">
         <v>909</v>
       </c>
-      <c r="L22" t="n">
+      <c r="L23" t="n">
         <v>-338</v>
       </c>
-      <c r="M22" t="n">
+      <c r="M23" t="n">
         <v>-693</v>
       </c>
-      <c r="N22" t="n">
+      <c r="N23" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C23" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D23" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E23" t="n">
-        <v>793</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H23" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J23" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K23" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M23" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N23" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C24" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D24" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E24" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H24" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I24" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J24" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K24" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L24" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M24" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N24" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C25" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D25" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E25" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H25" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I25" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J25" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K25" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L25" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M25" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N25" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C26" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I26" t="n">
+        <v>557</v>
+      </c>
+      <c r="J26" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L26" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N26" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B27" t="n">
         <v>42514</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C27" t="n">
         <v>51801</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F27" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G27" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J27" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/06 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D2" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E2" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F2" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D3" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E3" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F3" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D4" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E4" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F4" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D5" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E5" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F5" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D6" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E6" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F6" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D7" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E7" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F7" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D8" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E8" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F8" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D9" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E9" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F9" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D10" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E10" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F10" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D11" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E11" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F11" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,43 +705,67 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D12" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E12" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F12" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F13" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C14" t="n">
         <v>17813</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" t="n">
         <v>2560</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E14" t="n">
         <v>45601280</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F14" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="14"/>
+    <row r="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -754,7 +778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -781,27 +805,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -811,250 +835,260 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B30" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1069,7 +1103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1101,364 +1135,377 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C3" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C4" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C5" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C6" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C7" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C8" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C9" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C10" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C11" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C14" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C15" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C16" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C17" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C19" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C20" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C21" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C22" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C23" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C24" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C25" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C26" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C27" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C28" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C29" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B30" t="n">
         <v>24.64</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C30" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1473,7 +1520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1500,270 +1547,280 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B29" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1779,7 +1836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1873,1172 +1930,1218 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C2" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D2" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E2" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F2" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G2" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H2" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I2" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J2" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K2" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L2" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M2" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N2" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C3" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D3" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E3" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F3" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G3" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H3" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I3" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J3" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K3" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L3" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M3" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N3" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C4" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D4" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E4" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F4" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G4" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H4" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I4" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J4" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K4" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L4" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M4" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N4" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C5" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D5" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E5" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F5" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G5" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H5" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I5" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J5" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K5" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L5" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M5" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N5" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C6" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D6" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E6" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F6" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G6" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H6" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I6" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J6" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K6" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L6" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M6" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N6" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C7" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D7" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E7" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F7" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G7" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H7" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I7" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J7" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K7" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L7" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M7" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N7" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C8" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D8" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E8" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F8" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G8" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H8" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I8" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J8" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K8" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L8" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M8" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N8" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C9" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D9" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E9" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F9" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G9" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H9" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I9" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J9" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K9" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L9" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M9" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N9" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C10" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D10" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E10" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F10" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G10" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H10" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I10" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J10" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K10" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L10" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M10" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N10" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C11" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D11" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E11" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F11" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G11" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H11" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I11" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J11" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K11" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L11" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M11" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N11" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C12" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D12" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E12" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F12" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G12" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H12" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I12" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J12" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K12" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L12" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M12" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N12" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C13" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D13" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E13" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F13" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G13" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H13" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I13" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J13" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K13" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L13" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M13" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N13" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C14" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D14" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E14" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F14" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G14" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H14" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I14" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J14" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K14" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L14" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M14" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N14" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C15" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D15" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E15" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F15" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G15" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H15" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I15" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J15" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K15" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L15" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M15" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N15" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C16" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D16" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E16" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F16" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G16" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H16" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I16" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J16" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K16" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L16" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M16" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N16" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C17" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D17" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E17" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F17" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G17" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H17" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I17" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J17" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K17" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L17" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M17" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N17" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C18" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D18" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E18" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F18" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G18" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H18" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I18" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J18" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K18" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L18" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M18" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N18" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C19" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D19" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E19" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F19" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G19" t="n">
+        <v>40270</v>
       </c>
       <c r="H19" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I19" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J19" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K19" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L19" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M19" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N19" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C20" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D20" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E20" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H20" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I20" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J20" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K20" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L20" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M20" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N20" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C21" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D21" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E21" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H21" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I21" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J21" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K21" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L21" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M21" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N21" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C22" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D22" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E22" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H22" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I22" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J22" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K22" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L22" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M22" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N22" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C23" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E23" t="n">
+        <v>749</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M23" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N23" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>45267</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C24" t="n">
         <v>49710</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D24" t="n">
         <v>-1089</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E24" t="n">
         <v>-2353</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F24" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G24" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H24" t="n">
         <v>-751</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I24" t="n">
         <v>-1660</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J24" t="n">
         <v>-21534</v>
       </c>
-      <c r="K23" t="n">
+      <c r="K24" t="n">
         <v>909</v>
       </c>
-      <c r="L23" t="n">
+      <c r="L24" t="n">
         <v>-338</v>
       </c>
-      <c r="M23" t="n">
+      <c r="M24" t="n">
         <v>-693</v>
       </c>
-      <c r="N23" t="n">
+      <c r="N24" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C24" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D24" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E24" t="n">
-        <v>793</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H24" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J24" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K24" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L24" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M24" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N24" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C25" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D25" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E25" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H25" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I25" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J25" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K25" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L25" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M25" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N25" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C26" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D26" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E26" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H26" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I26" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J26" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K26" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L26" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M26" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N26" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C27" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I27" t="n">
+        <v>557</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L27" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M27" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N27" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B28" t="n">
         <v>42514</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C28" t="n">
         <v>51801</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F28" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G28" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J28" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/07 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D2" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E2" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F2" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D3" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E3" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F3" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D4" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E4" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F4" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D5" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E5" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F5" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D6" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E6" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F6" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D7" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E7" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F7" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D8" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E8" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F8" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D9" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E9" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F9" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D10" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E10" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F10" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D11" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E11" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F11" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D12" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E12" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F12" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,43 +729,67 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D13" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E13" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F13" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F14" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>17813</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>2560</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>45601280</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F15" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="15"/>
+    <row r="16"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -778,7 +802,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -805,37 +829,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -845,250 +869,260 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B31" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1103,7 +1137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1135,377 +1169,390 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C2" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C4" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C5" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C6" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C7" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C8" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C9" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C10" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C11" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C12" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C15" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C16" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C17" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C18" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C21" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C22" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C23" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C24" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C26" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C27" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C28" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C29" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C30" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B31" t="n">
         <v>24.64</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C31" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1520,7 +1567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1547,280 +1594,290 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B30" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1836,7 +1893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1930,1218 +1987,1264 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C2" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D2" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E2" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F2" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G2" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H2" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I2" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J2" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K2" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L2" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M2" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N2" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C3" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D3" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E3" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F3" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G3" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H3" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I3" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J3" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K3" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L3" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M3" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N3" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C4" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D4" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E4" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F4" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G4" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H4" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I4" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J4" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K4" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L4" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M4" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N4" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C5" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D5" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E5" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F5" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G5" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H5" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I5" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J5" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K5" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L5" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M5" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N5" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C6" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D6" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E6" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F6" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G6" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H6" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I6" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J6" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K6" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L6" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M6" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N6" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C7" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D7" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E7" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F7" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G7" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H7" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I7" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J7" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K7" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L7" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M7" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N7" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C8" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D8" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E8" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F8" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G8" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H8" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I8" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J8" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K8" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L8" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M8" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N8" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C9" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D9" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E9" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F9" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G9" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H9" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I9" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J9" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K9" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L9" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M9" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N9" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C10" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D10" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E10" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F10" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G10" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H10" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I10" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J10" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K10" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L10" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M10" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N10" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C11" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D11" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E11" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F11" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G11" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H11" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I11" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J11" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K11" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L11" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M11" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N11" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C12" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D12" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E12" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F12" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G12" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H12" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I12" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J12" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K12" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L12" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M12" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N12" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C13" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D13" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E13" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F13" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G13" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H13" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I13" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J13" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K13" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L13" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M13" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N13" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C14" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D14" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E14" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F14" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G14" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H14" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I14" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J14" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K14" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L14" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M14" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N14" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C15" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D15" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E15" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F15" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G15" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H15" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I15" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J15" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K15" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L15" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M15" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N15" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C16" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D16" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E16" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F16" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G16" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H16" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I16" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J16" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K16" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L16" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M16" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N16" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C17" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D17" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E17" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F17" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G17" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H17" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I17" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J17" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K17" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L17" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M17" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N17" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C18" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D18" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E18" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F18" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G18" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H18" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I18" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J18" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K18" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L18" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M18" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N18" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C19" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D19" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E19" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F19" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G19" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H19" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I19" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J19" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K19" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L19" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M19" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N19" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C20" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D20" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E20" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F20" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G20" t="n">
+        <v>40270</v>
       </c>
       <c r="H20" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I20" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J20" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K20" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L20" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M20" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N20" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C21" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D21" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E21" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H21" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I21" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J21" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K21" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L21" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M21" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N21" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C22" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D22" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E22" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H22" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I22" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J22" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K22" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L22" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M22" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N22" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C23" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D23" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E23" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H23" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I23" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J23" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K23" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L23" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M23" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N23" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C24" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E24" t="n">
+        <v>749</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N24" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B25" t="n">
         <v>45267</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C25" t="n">
         <v>49710</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D25" t="n">
         <v>-1089</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E25" t="n">
         <v>-2353</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F25" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G25" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H25" t="n">
         <v>-751</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I25" t="n">
         <v>-1660</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J25" t="n">
         <v>-21534</v>
       </c>
-      <c r="K24" t="n">
+      <c r="K25" t="n">
         <v>909</v>
       </c>
-      <c r="L24" t="n">
+      <c r="L25" t="n">
         <v>-338</v>
       </c>
-      <c r="M24" t="n">
+      <c r="M25" t="n">
         <v>-693</v>
       </c>
-      <c r="N24" t="n">
+      <c r="N25" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C25" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D25" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E25" t="n">
-        <v>793</v>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G25" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H25" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J25" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K25" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L25" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M25" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C26" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D26" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E26" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H26" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I26" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J26" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K26" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L26" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M26" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N26" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C27" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D27" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E27" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H27" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I27" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J27" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K27" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L27" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M27" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N27" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C28" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I28" t="n">
+        <v>557</v>
+      </c>
+      <c r="J28" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L28" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N28" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B29" t="n">
         <v>42514</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C29" t="n">
         <v>51801</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F29" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G29" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J28" t="n">
+      <c r="J29" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/08 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17740</v>
+        <v>17793</v>
       </c>
       <c r="D2" t="n">
-        <v>10960</v>
+        <v>11174</v>
       </c>
       <c r="E2" t="n">
-        <v>18556040</v>
+        <v>3807702</v>
       </c>
       <c r="F2" t="n">
-        <v>17644</v>
+        <v>17647</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D3" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E3" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F3" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D4" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E4" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F4" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D5" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E5" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F5" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D6" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E6" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F6" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D7" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E7" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F7" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D8" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E8" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F8" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D9" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E9" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F9" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D10" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E10" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F10" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D11" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E11" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F11" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D12" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E12" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F12" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D13" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E13" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F13" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,43 +753,67 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D14" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E14" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F14" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>17813</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" t="n">
         <v>2560</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E16" t="n">
         <v>45601280</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F16" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="16"/>
+    <row r="17"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -802,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -829,47 +853,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -879,250 +903,260 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B32" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1137,7 +1171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1169,390 +1203,403 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C2" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C3" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C5" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C6" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C7" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C8" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C9" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C10" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C11" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C12" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C13" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C16" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C17" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C18" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C19" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C21" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C22" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C23" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C25" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C26" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C27" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C28" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C29" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C30" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C31" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B32" t="n">
         <v>24.64</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C32" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1567,7 +1614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1594,290 +1641,300 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B31" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1893,7 +1950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1987,1264 +2044,1310 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C2" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D2" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E2" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F2" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G2" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H2" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I2" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J2" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K2" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L2" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M2" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N2" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C3" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D3" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E3" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F3" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G3" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H3" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I3" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J3" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K3" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L3" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M3" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N3" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C4" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D4" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E4" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F4" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G4" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H4" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I4" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J4" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K4" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L4" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M4" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N4" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C5" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D5" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E5" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F5" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G5" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H5" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I5" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J5" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K5" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L5" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M5" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N5" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C6" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D6" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E6" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F6" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G6" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H6" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I6" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J6" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K6" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L6" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M6" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N6" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C7" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D7" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E7" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F7" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G7" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H7" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I7" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J7" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K7" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L7" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M7" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N7" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C8" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D8" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E8" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F8" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G8" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H8" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I8" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J8" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K8" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L8" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M8" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N8" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C9" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D9" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E9" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F9" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G9" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H9" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I9" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J9" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K9" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L9" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M9" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N9" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C10" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D10" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E10" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F10" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G10" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H10" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I10" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J10" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K10" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L10" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M10" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N10" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C11" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D11" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E11" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F11" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G11" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H11" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I11" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J11" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K11" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L11" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M11" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N11" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C12" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D12" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E12" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F12" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G12" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H12" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I12" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J12" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K12" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L12" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M12" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N12" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C13" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D13" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E13" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F13" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G13" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H13" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I13" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J13" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K13" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L13" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M13" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N13" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C14" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D14" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E14" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F14" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G14" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H14" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I14" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J14" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K14" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L14" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M14" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N14" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C15" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D15" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E15" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F15" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G15" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H15" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I15" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J15" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K15" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L15" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M15" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N15" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C16" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D16" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E16" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F16" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G16" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H16" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I16" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J16" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K16" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L16" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M16" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N16" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C17" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D17" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E17" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F17" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G17" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H17" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I17" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J17" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K17" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L17" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M17" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N17" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C18" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D18" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E18" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F18" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G18" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H18" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I18" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J18" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K18" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L18" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M18" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N18" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C19" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D19" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E19" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F19" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G19" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H19" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I19" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J19" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K19" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L19" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M19" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N19" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C20" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D20" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E20" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F20" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G20" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H20" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I20" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J20" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K20" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L20" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M20" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N20" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C21" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D21" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E21" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F21" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G21" t="n">
+        <v>40270</v>
       </c>
       <c r="H21" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I21" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J21" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K21" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L21" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M21" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N21" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C22" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D22" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E22" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H22" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I22" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J22" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K22" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L22" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M22" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N22" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C23" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D23" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E23" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H23" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I23" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J23" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K23" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L23" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M23" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N23" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C24" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D24" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E24" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H24" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I24" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J24" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K24" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L24" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M24" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N24" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C25" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E25" t="n">
+        <v>749</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M25" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B26" t="n">
         <v>45267</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C26" t="n">
         <v>49710</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D26" t="n">
         <v>-1089</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E26" t="n">
         <v>-2353</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F26" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G26" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H26" t="n">
         <v>-751</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I26" t="n">
         <v>-1660</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J26" t="n">
         <v>-21534</v>
       </c>
-      <c r="K25" t="n">
+      <c r="K26" t="n">
         <v>909</v>
       </c>
-      <c r="L25" t="n">
+      <c r="L26" t="n">
         <v>-338</v>
       </c>
-      <c r="M25" t="n">
+      <c r="M26" t="n">
         <v>-693</v>
       </c>
-      <c r="N25" t="n">
+      <c r="N26" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C26" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D26" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E26" t="n">
-        <v>793</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H26" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I26" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J26" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K26" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L26" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M26" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N26" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C27" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D27" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E27" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H27" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I27" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J27" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K27" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L27" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M27" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N27" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C28" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D28" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E28" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H28" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I28" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J28" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K28" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L28" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M28" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N28" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C29" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I29" t="n">
+        <v>557</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N29" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B30" t="n">
         <v>42514</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C30" t="n">
         <v>51801</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F30" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G30" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J30" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/09 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17793</v>
+        <v>17852</v>
       </c>
       <c r="D2" t="n">
-        <v>11174</v>
+        <v>12187</v>
       </c>
       <c r="E2" t="n">
-        <v>3807702</v>
+        <v>18084076</v>
       </c>
       <c r="F2" t="n">
-        <v>17647</v>
+        <v>17664</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17740</v>
+        <v>17793</v>
       </c>
       <c r="D3" t="n">
-        <v>10960</v>
+        <v>11174</v>
       </c>
       <c r="E3" t="n">
-        <v>18556040</v>
+        <v>3807702</v>
       </c>
       <c r="F3" t="n">
-        <v>17644</v>
+        <v>17647</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D4" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E4" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F4" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D5" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E5" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F5" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D6" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E6" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F6" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D7" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E7" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F7" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D8" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E8" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F8" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D9" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E9" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F9" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D10" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E10" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F10" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D11" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E11" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F11" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D12" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E12" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F12" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D13" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E13" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F13" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,22 +753,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D14" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E14" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F14" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -777,43 +777,67 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D15" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E15" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F15" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F16" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C17" t="n">
         <v>17813</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D17" t="n">
         <v>2560</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E17" t="n">
         <v>45601280</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F17" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="17"/>
+    <row r="18"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -826,7 +850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -853,7 +877,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -863,47 +887,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -913,250 +937,260 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B33" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1171,7 +1205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1203,403 +1237,416 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C2" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C3" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C4" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C6" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C7" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C8" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C9" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C10" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C11" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C12" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C13" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C14" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C17" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C18" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C19" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C20" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C22" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C23" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C24" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C26" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C28" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C29" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C30" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C31" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C32" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B33" t="n">
         <v>24.64</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C33" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1614,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1641,300 +1688,310 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B32" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1950,7 +2007,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2044,1310 +2101,1356 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C2" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D2" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E2" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F2" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G2" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H2" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I2" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J2" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K2" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L2" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M2" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N2" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C3" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D3" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E3" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F3" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G3" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H3" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I3" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J3" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K3" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L3" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M3" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N3" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C4" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D4" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E4" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F4" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G4" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H4" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I4" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J4" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K4" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L4" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M4" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N4" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C5" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D5" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E5" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F5" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G5" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H5" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I5" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J5" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K5" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L5" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M5" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N5" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C6" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D6" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E6" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F6" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G6" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H6" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I6" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J6" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K6" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L6" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M6" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N6" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C7" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D7" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E7" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F7" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G7" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H7" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I7" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J7" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K7" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L7" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M7" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N7" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C8" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D8" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E8" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F8" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G8" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H8" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I8" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J8" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K8" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L8" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M8" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N8" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C9" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D9" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E9" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F9" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G9" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H9" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I9" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J9" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K9" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L9" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M9" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N9" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C10" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D10" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E10" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F10" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G10" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H10" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I10" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J10" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K10" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L10" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M10" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N10" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C11" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D11" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E11" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F11" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G11" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H11" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I11" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J11" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K11" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L11" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M11" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N11" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C12" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D12" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E12" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F12" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G12" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H12" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I12" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J12" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K12" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L12" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M12" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N12" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C13" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D13" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E13" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F13" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G13" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H13" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I13" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J13" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K13" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L13" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M13" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N13" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C14" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D14" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E14" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F14" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G14" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H14" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I14" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J14" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K14" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L14" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M14" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N14" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C15" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D15" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E15" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F15" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G15" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H15" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I15" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J15" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K15" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L15" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M15" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N15" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C16" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D16" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E16" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F16" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G16" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H16" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I16" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J16" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K16" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L16" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M16" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N16" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C17" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D17" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E17" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F17" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G17" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H17" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I17" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J17" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K17" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L17" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M17" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N17" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C18" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D18" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E18" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F18" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G18" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H18" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I18" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J18" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K18" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L18" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M18" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N18" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C19" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D19" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E19" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F19" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G19" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H19" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I19" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J19" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K19" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L19" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M19" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N19" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C20" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D20" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E20" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F20" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G20" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H20" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I20" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J20" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K20" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L20" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M20" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N20" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C21" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D21" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E21" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F21" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G21" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H21" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I21" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J21" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K21" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L21" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M21" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N21" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C22" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D22" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E22" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F22" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G22" t="n">
+        <v>40270</v>
       </c>
       <c r="H22" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I22" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J22" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K22" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L22" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M22" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N22" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C23" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D23" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E23" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H23" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I23" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J23" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K23" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L23" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M23" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N23" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C24" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D24" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E24" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H24" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I24" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J24" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K24" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L24" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M24" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N24" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C25" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D25" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E25" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H25" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I25" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J25" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K25" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L25" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M25" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N25" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C26" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E26" t="n">
+        <v>749</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J26" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N26" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B27" t="n">
         <v>45267</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C27" t="n">
         <v>49710</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D27" t="n">
         <v>-1089</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E27" t="n">
         <v>-2353</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F27" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G27" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H27" t="n">
         <v>-751</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I27" t="n">
         <v>-1660</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J27" t="n">
         <v>-21534</v>
       </c>
-      <c r="K26" t="n">
+      <c r="K27" t="n">
         <v>909</v>
       </c>
-      <c r="L26" t="n">
+      <c r="L27" t="n">
         <v>-338</v>
       </c>
-      <c r="M26" t="n">
+      <c r="M27" t="n">
         <v>-693</v>
       </c>
-      <c r="N26" t="n">
+      <c r="N27" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C27" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D27" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E27" t="n">
-        <v>793</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G27" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H27" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I27" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J27" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K27" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L27" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M27" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N27" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C28" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D28" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E28" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H28" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I28" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J28" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K28" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L28" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M28" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N28" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C29" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D29" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E29" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H29" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I29" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J29" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K29" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L29" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M29" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N29" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C30" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I30" t="n">
+        <v>557</v>
+      </c>
+      <c r="J30" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M30" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N30" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B31" t="n">
         <v>42514</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C31" t="n">
         <v>51801</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F31" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G31" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J31" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/10 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17852</v>
+        <v>17763</v>
       </c>
       <c r="D2" t="n">
-        <v>12187</v>
+        <v>13989</v>
       </c>
       <c r="E2" t="n">
-        <v>18084076</v>
+        <v>32008926</v>
       </c>
       <c r="F2" t="n">
-        <v>17664</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17793</v>
+        <v>17852</v>
       </c>
       <c r="D3" t="n">
-        <v>11174</v>
+        <v>12187</v>
       </c>
       <c r="E3" t="n">
-        <v>3807702</v>
+        <v>18084076</v>
       </c>
       <c r="F3" t="n">
-        <v>17647</v>
+        <v>17664</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17740</v>
+        <v>17793</v>
       </c>
       <c r="D4" t="n">
-        <v>10960</v>
+        <v>11174</v>
       </c>
       <c r="E4" t="n">
-        <v>18556040</v>
+        <v>3807702</v>
       </c>
       <c r="F4" t="n">
-        <v>17644</v>
+        <v>17647</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D5" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E5" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F5" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D6" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E6" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F6" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D7" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E7" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F7" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D8" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E8" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F8" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D9" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E9" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F9" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D10" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E10" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F10" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D11" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E11" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F11" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D12" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E12" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F12" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D13" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E13" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F13" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,22 +753,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D14" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E14" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F14" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -777,22 +777,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D15" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E15" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F15" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -801,43 +801,67 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D16" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E16" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F16" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C18" t="n">
         <v>17813</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>2560</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>45601280</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F18" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="18"/>
+    <row r="19"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -850,7 +874,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -877,17 +901,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -897,47 +921,47 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -947,250 +971,260 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1205,7 +1239,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1237,416 +1271,429 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C2" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C3" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C4" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C5" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C6" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C7" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C8" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C9" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C10" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C11" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C12" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C13" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C14" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C15" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C18" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C19" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C20" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C21" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C22" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C23" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C24" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C25" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C26" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C27" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C29" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C30" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C31" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C32" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C33" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
         <v>24.64</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C34" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1661,7 +1708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1688,310 +1735,320 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B33" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2007,7 +2064,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2101,1356 +2158,1402 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C2" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D2" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E2" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F2" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G2" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H2" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I2" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J2" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K2" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L2" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M2" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N2" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C3" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D3" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E3" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F3" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G3" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H3" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I3" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J3" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K3" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L3" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M3" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N3" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C4" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D4" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E4" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F4" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G4" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H4" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I4" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J4" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K4" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L4" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M4" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N4" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C5" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D5" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E5" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F5" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G5" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H5" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I5" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J5" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K5" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L5" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M5" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N5" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C6" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D6" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E6" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F6" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G6" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H6" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I6" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J6" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K6" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L6" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M6" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N6" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C7" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D7" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E7" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F7" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G7" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H7" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I7" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J7" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K7" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L7" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M7" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N7" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C8" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D8" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E8" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F8" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G8" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H8" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I8" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J8" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K8" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L8" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M8" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N8" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C9" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D9" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E9" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F9" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G9" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H9" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I9" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J9" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K9" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L9" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M9" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N9" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C10" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D10" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E10" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F10" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G10" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H10" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I10" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J10" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K10" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L10" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M10" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N10" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C11" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D11" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E11" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F11" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G11" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H11" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I11" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J11" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K11" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L11" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M11" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N11" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C12" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D12" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E12" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F12" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G12" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H12" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I12" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J12" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K12" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L12" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M12" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N12" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C13" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D13" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E13" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F13" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G13" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H13" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I13" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J13" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K13" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L13" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M13" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N13" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C14" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D14" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E14" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F14" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G14" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H14" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I14" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J14" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K14" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L14" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M14" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N14" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C15" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D15" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E15" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F15" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G15" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H15" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I15" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J15" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K15" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L15" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M15" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N15" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C16" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D16" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E16" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F16" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G16" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H16" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I16" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J16" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K16" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L16" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M16" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N16" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C17" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D17" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E17" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F17" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G17" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H17" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I17" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J17" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K17" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L17" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M17" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N17" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C18" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D18" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E18" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F18" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G18" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H18" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I18" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J18" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K18" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L18" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M18" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N18" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C19" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D19" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E19" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F19" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G19" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H19" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I19" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J19" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K19" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L19" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M19" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N19" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C20" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D20" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E20" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F20" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G20" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H20" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I20" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J20" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K20" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L20" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M20" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N20" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C21" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D21" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E21" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F21" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G21" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H21" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I21" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J21" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K21" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L21" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M21" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N21" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C22" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D22" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E22" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F22" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G22" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H22" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I22" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J22" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K22" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L22" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M22" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N22" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C23" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D23" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E23" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F23" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G23" t="n">
+        <v>40270</v>
       </c>
       <c r="H23" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I23" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J23" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K23" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L23" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M23" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N23" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C24" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D24" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E24" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H24" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I24" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J24" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K24" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L24" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M24" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N24" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C25" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D25" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E25" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H25" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I25" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J25" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K25" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L25" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M25" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N25" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C26" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D26" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E26" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H26" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I26" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J26" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K26" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L26" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M26" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N26" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C27" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E27" t="n">
+        <v>749</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M27" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N27" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B28" t="n">
         <v>45267</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C28" t="n">
         <v>49710</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D28" t="n">
         <v>-1089</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E28" t="n">
         <v>-2353</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F28" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G28" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H28" t="n">
         <v>-751</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I28" t="n">
         <v>-1660</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J28" t="n">
         <v>-21534</v>
       </c>
-      <c r="K27" t="n">
+      <c r="K28" t="n">
         <v>909</v>
       </c>
-      <c r="L27" t="n">
+      <c r="L28" t="n">
         <v>-338</v>
       </c>
-      <c r="M27" t="n">
+      <c r="M28" t="n">
         <v>-693</v>
       </c>
-      <c r="N27" t="n">
+      <c r="N28" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C28" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D28" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E28" t="n">
-        <v>793</v>
-      </c>
-      <c r="F28" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G28" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H28" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I28" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J28" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K28" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L28" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M28" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N28" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C29" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D29" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E29" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H29" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I29" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J29" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K29" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L29" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M29" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N29" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C30" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D30" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E30" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H30" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I30" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J30" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K30" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L30" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M30" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N30" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C31" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I31" t="n">
+        <v>557</v>
+      </c>
+      <c r="J31" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M31" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N31" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B32" t="n">
         <v>42514</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C32" t="n">
         <v>51801</v>
       </c>
-      <c r="F31" s="2" t="n">
+      <c r="F32" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G31" s="2" t="n">
+      <c r="G32" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J31" t="n">
+      <c r="J32" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/13 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17763</v>
+        <v>17691</v>
       </c>
       <c r="D2" t="n">
-        <v>13989</v>
+        <v>38344</v>
       </c>
       <c r="E2" t="n">
-        <v>32008926</v>
+        <v>430864305</v>
       </c>
       <c r="F2" t="n">
-        <v>17676</v>
+        <v>17685</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17852</v>
+        <v>17763</v>
       </c>
       <c r="D3" t="n">
-        <v>12187</v>
+        <v>13989</v>
       </c>
       <c r="E3" t="n">
-        <v>18084076</v>
+        <v>32008926</v>
       </c>
       <c r="F3" t="n">
-        <v>17664</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17793</v>
+        <v>17852</v>
       </c>
       <c r="D4" t="n">
-        <v>11174</v>
+        <v>12187</v>
       </c>
       <c r="E4" t="n">
-        <v>3807702</v>
+        <v>18084076</v>
       </c>
       <c r="F4" t="n">
-        <v>17647</v>
+        <v>17664</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17740</v>
+        <v>17793</v>
       </c>
       <c r="D5" t="n">
-        <v>10960</v>
+        <v>11174</v>
       </c>
       <c r="E5" t="n">
-        <v>18556040</v>
+        <v>3807702</v>
       </c>
       <c r="F5" t="n">
-        <v>17644</v>
+        <v>17647</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D6" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E6" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F6" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D7" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E7" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F7" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D8" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E8" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F8" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D9" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E9" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F9" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D10" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E10" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F10" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D11" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E11" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F11" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D12" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E12" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F12" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D13" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E13" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F13" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,22 +753,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D14" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E14" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F14" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -777,22 +777,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D15" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E15" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F15" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -801,22 +801,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D16" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E16" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F16" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -825,43 +825,67 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D17" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E17" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F17" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F18" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C19" t="n">
         <v>17813</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>2560</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E19" t="n">
         <v>45601280</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F19" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="19"/>
+    <row r="20"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -874,7 +898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -901,7 +925,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -911,17 +935,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -931,47 +955,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -981,250 +1005,260 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B35" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1239,7 +1273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1271,429 +1305,442 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C2" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C3" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C4" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C5" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C6" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C7" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C8" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C9" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C10" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C11" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C12" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C13" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C14" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C15" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C16" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C19" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C20" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C21" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C22" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C24" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C25" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C26" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C27" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C28" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C30" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C31" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C32" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C33" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C34" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B35" t="n">
         <v>24.64</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C35" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1708,7 +1755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1735,320 +1782,330 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2064,7 +2121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2158,1402 +2215,1448 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C2" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D2" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E2" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F2" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G2" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H2" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I2" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J2" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K2" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L2" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M2" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N2" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C3" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D3" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E3" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F3" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G3" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H3" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I3" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J3" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K3" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L3" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M3" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N3" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C4" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D4" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E4" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F4" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G4" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H4" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I4" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J4" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K4" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L4" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M4" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N4" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C5" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D5" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E5" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F5" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G5" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H5" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I5" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J5" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K5" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L5" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M5" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N5" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C6" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D6" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E6" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F6" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G6" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H6" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I6" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J6" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K6" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L6" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M6" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N6" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C7" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D7" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E7" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F7" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G7" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H7" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I7" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J7" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K7" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L7" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M7" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N7" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C8" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D8" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E8" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F8" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G8" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H8" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I8" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J8" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K8" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L8" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M8" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N8" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C9" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D9" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E9" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F9" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G9" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H9" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I9" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J9" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K9" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L9" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M9" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N9" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C10" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D10" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E10" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F10" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G10" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H10" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I10" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J10" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K10" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L10" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M10" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N10" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C11" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D11" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E11" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F11" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G11" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H11" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I11" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J11" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K11" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L11" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M11" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N11" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C12" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D12" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E12" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F12" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G12" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H12" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I12" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J12" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K12" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L12" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M12" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N12" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C13" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D13" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E13" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F13" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G13" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H13" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I13" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J13" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K13" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L13" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M13" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N13" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C14" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D14" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E14" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F14" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G14" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H14" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I14" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J14" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K14" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L14" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M14" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N14" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C15" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D15" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E15" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F15" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G15" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H15" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I15" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J15" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K15" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L15" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M15" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N15" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C16" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D16" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E16" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F16" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G16" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H16" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I16" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J16" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K16" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L16" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M16" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N16" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C17" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D17" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E17" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F17" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G17" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H17" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I17" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J17" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K17" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L17" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M17" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N17" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C18" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D18" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E18" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F18" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G18" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H18" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I18" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J18" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K18" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L18" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M18" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N18" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C19" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D19" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E19" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F19" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G19" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H19" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I19" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J19" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K19" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L19" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M19" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N19" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C20" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D20" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E20" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F20" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G20" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H20" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I20" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J20" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K20" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L20" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M20" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N20" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C21" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D21" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E21" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F21" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G21" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H21" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I21" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J21" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K21" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L21" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M21" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N21" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C22" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D22" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E22" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F22" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G22" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H22" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I22" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J22" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K22" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L22" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M22" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N22" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C23" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D23" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E23" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F23" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G23" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H23" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I23" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J23" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K23" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L23" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M23" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N23" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C24" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D24" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E24" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F24" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G24" t="n">
+        <v>40270</v>
       </c>
       <c r="H24" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I24" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J24" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K24" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L24" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M24" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N24" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C25" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D25" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E25" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H25" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I25" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J25" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K25" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L25" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M25" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N25" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C26" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D26" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E26" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H26" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I26" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J26" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K26" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L26" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M26" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N26" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C27" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D27" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E27" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H27" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I27" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J27" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K27" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L27" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M27" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N27" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C28" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E28" t="n">
+        <v>749</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J28" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N28" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B29" t="n">
         <v>45267</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C29" t="n">
         <v>49710</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D29" t="n">
         <v>-1089</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E29" t="n">
         <v>-2353</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F29" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G29" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H29" t="n">
         <v>-751</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I29" t="n">
         <v>-1660</v>
       </c>
-      <c r="J28" t="n">
+      <c r="J29" t="n">
         <v>-21534</v>
       </c>
-      <c r="K28" t="n">
+      <c r="K29" t="n">
         <v>909</v>
       </c>
-      <c r="L28" t="n">
+      <c r="L29" t="n">
         <v>-338</v>
       </c>
-      <c r="M28" t="n">
+      <c r="M29" t="n">
         <v>-693</v>
       </c>
-      <c r="N28" t="n">
+      <c r="N29" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C29" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D29" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E29" t="n">
-        <v>793</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G29" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H29" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J29" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K29" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L29" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M29" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N29" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C30" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D30" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E30" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H30" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I30" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J30" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K30" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L30" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M30" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N30" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C31" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D31" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E31" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H31" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I31" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J31" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K31" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L31" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M31" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N31" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C32" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I32" t="n">
+        <v>557</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L32" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M32" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N32" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B33" t="n">
         <v>42514</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C33" t="n">
         <v>51801</v>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F33" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G33" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J33" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/14 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17691</v>
+        <v>17543</v>
       </c>
       <c r="D2" t="n">
-        <v>38344</v>
+        <v>59283</v>
       </c>
       <c r="E2" t="n">
-        <v>430864305</v>
+        <v>367332877</v>
       </c>
       <c r="F2" t="n">
-        <v>17685</v>
+        <v>17635</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17763</v>
+        <v>17691</v>
       </c>
       <c r="D3" t="n">
-        <v>13989</v>
+        <v>38344</v>
       </c>
       <c r="E3" t="n">
-        <v>32008926</v>
+        <v>430864305</v>
       </c>
       <c r="F3" t="n">
-        <v>17676</v>
+        <v>17685</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17852</v>
+        <v>17763</v>
       </c>
       <c r="D4" t="n">
-        <v>12187</v>
+        <v>13989</v>
       </c>
       <c r="E4" t="n">
-        <v>18084076</v>
+        <v>32008926</v>
       </c>
       <c r="F4" t="n">
-        <v>17664</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17793</v>
+        <v>17852</v>
       </c>
       <c r="D5" t="n">
-        <v>11174</v>
+        <v>12187</v>
       </c>
       <c r="E5" t="n">
-        <v>3807702</v>
+        <v>18084076</v>
       </c>
       <c r="F5" t="n">
-        <v>17647</v>
+        <v>17664</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17740</v>
+        <v>17793</v>
       </c>
       <c r="D6" t="n">
-        <v>10960</v>
+        <v>11174</v>
       </c>
       <c r="E6" t="n">
-        <v>18556040</v>
+        <v>3807702</v>
       </c>
       <c r="F6" t="n">
-        <v>17644</v>
+        <v>17647</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D7" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E7" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F7" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D8" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E8" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F8" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D9" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E9" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F9" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D10" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E10" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F10" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D11" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E11" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F11" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D12" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E12" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F12" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D13" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E13" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F13" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,22 +753,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D14" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E14" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F14" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -777,22 +777,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D15" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E15" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F15" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -801,22 +801,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D16" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E16" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F16" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -825,22 +825,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D17" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E17" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F17" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -849,43 +849,67 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D18" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E18" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F18" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E19" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F19" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C20" t="n">
         <v>17813</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D20" t="n">
         <v>2560</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E20" t="n">
         <v>45601280</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F20" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="20"/>
+    <row r="21"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -898,7 +922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -925,7 +949,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -935,7 +959,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -945,17 +969,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -965,47 +989,47 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1015,250 +1039,260 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B36" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1273,7 +1307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1305,442 +1339,455 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C2" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C3" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C4" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C5" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C6" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C7" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C9" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C10" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C11" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C12" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C13" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C14" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C15" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C16" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C17" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C20" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C21" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C22" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C23" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C24" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C25" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C26" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C27" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C28" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C29" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C30" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C31" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C32" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C33" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C34" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C35" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B36" t="n">
         <v>24.64</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C36" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1755,7 +1802,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1782,330 +1829,340 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B35" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2121,7 +2178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2215,1448 +2272,1494 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C2" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D2" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E2" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F2" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G2" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H2" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I2" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J2" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K2" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L2" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M2" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N2" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C3" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D3" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E3" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F3" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G3" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H3" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I3" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J3" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K3" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L3" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M3" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N3" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C4" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D4" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E4" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F4" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G4" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H4" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I4" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J4" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K4" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L4" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M4" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N4" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C5" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D5" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E5" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F5" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G5" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H5" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I5" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J5" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K5" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L5" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M5" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N5" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C6" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D6" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E6" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F6" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G6" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H6" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I6" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J6" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K6" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L6" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M6" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N6" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C7" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D7" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E7" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F7" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G7" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H7" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I7" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J7" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K7" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L7" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M7" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N7" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C8" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D8" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E8" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F8" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G8" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H8" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I8" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J8" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K8" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L8" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M8" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N8" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C9" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D9" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E9" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F9" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G9" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H9" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I9" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J9" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K9" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L9" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M9" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N9" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C10" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D10" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E10" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F10" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G10" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H10" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I10" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J10" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K10" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L10" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M10" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N10" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C11" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D11" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E11" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F11" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G11" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H11" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I11" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J11" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K11" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L11" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M11" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N11" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C12" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D12" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E12" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F12" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G12" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H12" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I12" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J12" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K12" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L12" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M12" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N12" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C13" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D13" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E13" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F13" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G13" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H13" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I13" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J13" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K13" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L13" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M13" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N13" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C14" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D14" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E14" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F14" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G14" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H14" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I14" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J14" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K14" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L14" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M14" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N14" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C15" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D15" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E15" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F15" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G15" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H15" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I15" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J15" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K15" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L15" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M15" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N15" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C16" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D16" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E16" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F16" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G16" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H16" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I16" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J16" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K16" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L16" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M16" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N16" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C17" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D17" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E17" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F17" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G17" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H17" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I17" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J17" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K17" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L17" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M17" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N17" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C18" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D18" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E18" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F18" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G18" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H18" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I18" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J18" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K18" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L18" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M18" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N18" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C19" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D19" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E19" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F19" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G19" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H19" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I19" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J19" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K19" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L19" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M19" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N19" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C20" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D20" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E20" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F20" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G20" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H20" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I20" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J20" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K20" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L20" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M20" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N20" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C21" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D21" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E21" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F21" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G21" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H21" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I21" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J21" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K21" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L21" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M21" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N21" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C22" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D22" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E22" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F22" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G22" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H22" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I22" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J22" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K22" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L22" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M22" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N22" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C23" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D23" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E23" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F23" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G23" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H23" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I23" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J23" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K23" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L23" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M23" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N23" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C24" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D24" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E24" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F24" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G24" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H24" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I24" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J24" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K24" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L24" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M24" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N24" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C25" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D25" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E25" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G25" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F25" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G25" t="n">
+        <v>40270</v>
       </c>
       <c r="H25" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I25" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J25" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K25" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L25" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M25" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N25" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C26" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D26" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E26" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H26" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I26" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J26" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K26" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L26" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M26" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N26" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C27" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D27" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E27" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H27" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I27" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J27" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K27" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L27" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M27" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N27" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C28" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D28" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E28" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H28" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I28" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J28" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K28" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L28" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M28" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N28" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C29" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E29" t="n">
+        <v>749</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N29" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B30" t="n">
         <v>45267</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C30" t="n">
         <v>49710</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>-1089</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E30" t="n">
         <v>-2353</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F30" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G30" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H30" t="n">
         <v>-751</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I30" t="n">
         <v>-1660</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J30" t="n">
         <v>-21534</v>
       </c>
-      <c r="K29" t="n">
+      <c r="K30" t="n">
         <v>909</v>
       </c>
-      <c r="L29" t="n">
+      <c r="L30" t="n">
         <v>-338</v>
       </c>
-      <c r="M29" t="n">
+      <c r="M30" t="n">
         <v>-693</v>
       </c>
-      <c r="N29" t="n">
+      <c r="N30" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C30" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E30" t="n">
-        <v>793</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H30" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J30" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K30" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L30" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M30" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N30" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C31" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D31" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E31" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H31" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I31" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J31" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K31" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L31" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M31" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N31" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C32" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D32" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E32" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H32" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I32" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J32" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K32" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L32" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M32" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N32" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C33" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I33" t="n">
+        <v>557</v>
+      </c>
+      <c r="J33" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L33" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M33" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N33" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
         <v>42514</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C34" t="n">
         <v>51801</v>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F34" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G33" s="2" t="n">
+      <c r="G34" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J33" t="n">
+      <c r="J34" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/15 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17543</v>
+        <v>17597</v>
       </c>
       <c r="D2" t="n">
-        <v>59283</v>
+        <v>70527</v>
       </c>
       <c r="E2" t="n">
-        <v>367332877</v>
+        <v>197860668</v>
       </c>
       <c r="F2" t="n">
-        <v>17635</v>
+        <v>17629</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17691</v>
+        <v>17543</v>
       </c>
       <c r="D3" t="n">
-        <v>38344</v>
+        <v>59283</v>
       </c>
       <c r="E3" t="n">
-        <v>430864305</v>
+        <v>367332877</v>
       </c>
       <c r="F3" t="n">
-        <v>17685</v>
+        <v>17635</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17763</v>
+        <v>17691</v>
       </c>
       <c r="D4" t="n">
-        <v>13989</v>
+        <v>38344</v>
       </c>
       <c r="E4" t="n">
-        <v>32008926</v>
+        <v>430864305</v>
       </c>
       <c r="F4" t="n">
-        <v>17676</v>
+        <v>17685</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17852</v>
+        <v>17763</v>
       </c>
       <c r="D5" t="n">
-        <v>12187</v>
+        <v>13989</v>
       </c>
       <c r="E5" t="n">
-        <v>18084076</v>
+        <v>32008926</v>
       </c>
       <c r="F5" t="n">
-        <v>17664</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17793</v>
+        <v>17852</v>
       </c>
       <c r="D6" t="n">
-        <v>11174</v>
+        <v>12187</v>
       </c>
       <c r="E6" t="n">
-        <v>3807702</v>
+        <v>18084076</v>
       </c>
       <c r="F6" t="n">
-        <v>17647</v>
+        <v>17664</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17740</v>
+        <v>17793</v>
       </c>
       <c r="D7" t="n">
-        <v>10960</v>
+        <v>11174</v>
       </c>
       <c r="E7" t="n">
-        <v>18556040</v>
+        <v>3807702</v>
       </c>
       <c r="F7" t="n">
-        <v>17644</v>
+        <v>17647</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17638</v>
+        <v>17740</v>
       </c>
       <c r="D8" t="n">
-        <v>9914</v>
+        <v>10960</v>
       </c>
       <c r="E8" t="n">
-        <v>14004572</v>
+        <v>18556040</v>
       </c>
       <c r="F8" t="n">
-        <v>17634</v>
+        <v>17644</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17650</v>
+        <v>17638</v>
       </c>
       <c r="D9" t="n">
-        <v>9120</v>
+        <v>9914</v>
       </c>
       <c r="E9" t="n">
-        <v>9478050</v>
+        <v>14004572</v>
       </c>
       <c r="F9" t="n">
-        <v>17633</v>
+        <v>17634</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17649</v>
+        <v>17650</v>
       </c>
       <c r="D10" t="n">
-        <v>8583</v>
+        <v>9120</v>
       </c>
       <c r="E10" t="n">
-        <v>19484496</v>
+        <v>9478050</v>
       </c>
       <c r="F10" t="n">
-        <v>17632</v>
+        <v>17633</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -681,22 +681,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17536</v>
+        <v>17649</v>
       </c>
       <c r="D11" t="n">
-        <v>7479</v>
+        <v>8583</v>
       </c>
       <c r="E11" t="n">
-        <v>8592640</v>
+        <v>19484496</v>
       </c>
       <c r="F11" t="n">
-        <v>17630</v>
+        <v>17632</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -705,22 +705,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17280</v>
+        <v>17536</v>
       </c>
       <c r="D12" t="n">
-        <v>6989</v>
+        <v>7479</v>
       </c>
       <c r="E12" t="n">
-        <v>10229760</v>
+        <v>8592640</v>
       </c>
       <c r="F12" t="n">
-        <v>17636</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17261</v>
+        <v>17280</v>
       </c>
       <c r="D13" t="n">
-        <v>6397</v>
+        <v>6989</v>
       </c>
       <c r="E13" t="n">
-        <v>1622534</v>
+        <v>10229760</v>
       </c>
       <c r="F13" t="n">
-        <v>17669</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,22 +753,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17296</v>
+        <v>17261</v>
       </c>
       <c r="D14" t="n">
-        <v>6303</v>
+        <v>6397</v>
       </c>
       <c r="E14" t="n">
-        <v>16915488</v>
+        <v>1622534</v>
       </c>
       <c r="F14" t="n">
-        <v>17676</v>
+        <v>17669</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -777,22 +777,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17627</v>
+        <v>17296</v>
       </c>
       <c r="D15" t="n">
-        <v>5325</v>
+        <v>6303</v>
       </c>
       <c r="E15" t="n">
-        <v>3930821</v>
+        <v>16915488</v>
       </c>
       <c r="F15" t="n">
-        <v>17745</v>
+        <v>17676</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -801,22 +801,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17634</v>
+        <v>17627</v>
       </c>
       <c r="D16" t="n">
-        <v>5102</v>
+        <v>5325</v>
       </c>
       <c r="E16" t="n">
-        <v>12996258</v>
+        <v>3930821</v>
       </c>
       <c r="F16" t="n">
-        <v>17751</v>
+        <v>17745</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -825,22 +825,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17610</v>
+        <v>17634</v>
       </c>
       <c r="D17" t="n">
-        <v>4365</v>
+        <v>5102</v>
       </c>
       <c r="E17" t="n">
-        <v>14774790</v>
+        <v>12996258</v>
       </c>
       <c r="F17" t="n">
-        <v>17770</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -849,22 +849,22 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>17790</v>
+        <v>17610</v>
       </c>
       <c r="D18" t="n">
-        <v>3526</v>
+        <v>4365</v>
       </c>
       <c r="E18" t="n">
-        <v>6849150</v>
+        <v>14774790</v>
       </c>
       <c r="F18" t="n">
-        <v>17809</v>
+        <v>17770</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -873,43 +873,67 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17804</v>
+        <v>17790</v>
       </c>
       <c r="D19" t="n">
-        <v>3141</v>
+        <v>3526</v>
       </c>
       <c r="E19" t="n">
-        <v>10344124</v>
+        <v>6849150</v>
       </c>
       <c r="F19" t="n">
-        <v>17811</v>
+        <v>17809</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>日期：2021/11/19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>17804</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3141</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10344124</v>
+      </c>
+      <c r="F20" t="n">
+        <v>17811</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>日期：2021/11/18</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>202201</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C21" t="n">
         <v>17813</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>2560</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E21" t="n">
         <v>45601280</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F21" t="n">
         <v>17813</v>
       </c>
     </row>
-    <row r="21"/>
+    <row r="22"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -922,7 +946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -949,17 +973,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -969,7 +993,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -979,17 +1003,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -999,47 +1023,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1049,250 +1073,260 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B37" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1307,7 +1341,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H21:H22"/>
@@ -1339,455 +1373,468 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C2" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C3" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C4" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C5" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C6" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C7" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C8" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C10" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C11" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C12" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C13" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C14" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C15" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C16" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C17" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C18" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C21" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C22" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C23" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C24" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C26" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C27" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C28" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C30" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C31" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C32" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C33" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C34" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C35" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C36" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B37" t="n">
         <v>24.64</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C37" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1802,7 +1849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1829,340 +1876,350 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B36" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2178,7 +2235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2272,1494 +2329,1540 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C2" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D2" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E2" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F2" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G2" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H2" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I2" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J2" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K2" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L2" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M2" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N2" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C3" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D3" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E3" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F3" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G3" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H3" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I3" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J3" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K3" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L3" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M3" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N3" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C4" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D4" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E4" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F4" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G4" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H4" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I4" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J4" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K4" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L4" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M4" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N4" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C5" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D5" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E5" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F5" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G5" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H5" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I5" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J5" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K5" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L5" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M5" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N5" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C6" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D6" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E6" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F6" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G6" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H6" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I6" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J6" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K6" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L6" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M6" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N6" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C7" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D7" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E7" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F7" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G7" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H7" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I7" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J7" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K7" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L7" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M7" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N7" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C8" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D8" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E8" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F8" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G8" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H8" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I8" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J8" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K8" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L8" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M8" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N8" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C9" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D9" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E9" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F9" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G9" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H9" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I9" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J9" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K9" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L9" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M9" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N9" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C10" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D10" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E10" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F10" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G10" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H10" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I10" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J10" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K10" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L10" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M10" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N10" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C11" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D11" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E11" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F11" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G11" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H11" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I11" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J11" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K11" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L11" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M11" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N11" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C12" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D12" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E12" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F12" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G12" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H12" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I12" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J12" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K12" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L12" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M12" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N12" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C13" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D13" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E13" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F13" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G13" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H13" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I13" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J13" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K13" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L13" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M13" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N13" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C14" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D14" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E14" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F14" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G14" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H14" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I14" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J14" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K14" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L14" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M14" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N14" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C15" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D15" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E15" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F15" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G15" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H15" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I15" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J15" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K15" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L15" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M15" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N15" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C16" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D16" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E16" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F16" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G16" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H16" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I16" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J16" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K16" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L16" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M16" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N16" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C17" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D17" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E17" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F17" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G17" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H17" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I17" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J17" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K17" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L17" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M17" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N17" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C18" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D18" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E18" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F18" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G18" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H18" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I18" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J18" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K18" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L18" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M18" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N18" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C19" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D19" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E19" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F19" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G19" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H19" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I19" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J19" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K19" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L19" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M19" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N19" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C20" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D20" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E20" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F20" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G20" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H20" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I20" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J20" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K20" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L20" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M20" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N20" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C21" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D21" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E21" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F21" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G21" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H21" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I21" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J21" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K21" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L21" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M21" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N21" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C22" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D22" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E22" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F22" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G22" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H22" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I22" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J22" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K22" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L22" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M22" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N22" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C23" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D23" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E23" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F23" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G23" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H23" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I23" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J23" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K23" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L23" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M23" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N23" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C24" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D24" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E24" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F24" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G24" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H24" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I24" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J24" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K24" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L24" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M24" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N24" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C25" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D25" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E25" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F25" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G25" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H25" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I25" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J25" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K25" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L25" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M25" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N25" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C26" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D26" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E26" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F26" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G26" t="n">
+        <v>40270</v>
       </c>
       <c r="H26" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I26" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J26" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K26" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L26" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M26" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N26" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C27" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D27" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E27" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H27" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I27" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J27" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K27" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L27" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M27" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N27" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C28" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D28" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E28" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H28" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I28" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J28" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K28" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L28" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M28" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N28" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C29" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D29" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E29" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H29" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I29" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J29" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K29" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L29" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M29" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N29" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C30" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E30" t="n">
+        <v>749</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J30" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M30" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B31" t="n">
         <v>45267</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C31" t="n">
         <v>49710</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D31" t="n">
         <v>-1089</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E31" t="n">
         <v>-2353</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F31" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G31" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H31" t="n">
         <v>-751</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I31" t="n">
         <v>-1660</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J31" t="n">
         <v>-21534</v>
       </c>
-      <c r="K30" t="n">
+      <c r="K31" t="n">
         <v>909</v>
       </c>
-      <c r="L30" t="n">
+      <c r="L31" t="n">
         <v>-338</v>
       </c>
-      <c r="M30" t="n">
+      <c r="M31" t="n">
         <v>-693</v>
       </c>
-      <c r="N30" t="n">
+      <c r="N31" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C31" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D31" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E31" t="n">
-        <v>793</v>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G31" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H31" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I31" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J31" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K31" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L31" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M31" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N31" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C32" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D32" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E32" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H32" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I32" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J32" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K32" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L32" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M32" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N32" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C33" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D33" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E33" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H33" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I33" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J33" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K33" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L33" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M33" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N33" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C34" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I34" t="n">
+        <v>557</v>
+      </c>
+      <c r="J34" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L34" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N34" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B35" t="n">
         <v>42514</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C35" t="n">
         <v>51801</v>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="F35" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G34" s="2" t="n">
+      <c r="G35" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J34" t="n">
+      <c r="J35" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/17 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,41 +465,65 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D2" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E2" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F2" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F3" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" t="n">
         <v>202202</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>17571</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>892</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E4" t="n">
         <v>15673332</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F4" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="4"/>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -512,7 +536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -539,17 +563,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -559,17 +583,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -579,7 +603,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -589,17 +613,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -609,47 +633,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -659,250 +683,260 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B39" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -917,7 +951,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -949,481 +983,494 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>-25.74</v>
       </c>
       <c r="C2" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C3" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C4" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C5" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C6" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C7" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C8" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C9" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C10" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C12" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C13" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C14" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C15" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C16" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C17" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C18" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C19" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C20" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C22" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C23" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C24" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C25" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C26" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C28" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C29" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C30" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C31" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C32" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C33" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C34" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C35" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C36" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C37" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C38" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B39" t="n">
         <v>24.64</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C39" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1438,7 +1485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1465,360 +1512,370 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B38" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1834,7 +1891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1928,1586 +1985,1632 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C2" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D2" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E2" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F2" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G2" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H2" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I2" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J2" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K2" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L2" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M2" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N2" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C3" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D3" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E3" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F3" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G3" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H3" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I3" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J3" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K3" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L3" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M3" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N3" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C4" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D4" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E4" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F4" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G4" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H4" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I4" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J4" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K4" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L4" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M4" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N4" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C5" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D5" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E5" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F5" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G5" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H5" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I5" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J5" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K5" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L5" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M5" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N5" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C6" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D6" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E6" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F6" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G6" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H6" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I6" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J6" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K6" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L6" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M6" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N6" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C7" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D7" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E7" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F7" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G7" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H7" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I7" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J7" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K7" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L7" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M7" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N7" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C8" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D8" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E8" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F8" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G8" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H8" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I8" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J8" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K8" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L8" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M8" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N8" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C9" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D9" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E9" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F9" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G9" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H9" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I9" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J9" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K9" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L9" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M9" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N9" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C10" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D10" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E10" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F10" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G10" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H10" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I10" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J10" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K10" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L10" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M10" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N10" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C11" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D11" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E11" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F11" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G11" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H11" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I11" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J11" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K11" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L11" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M11" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N11" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C12" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D12" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E12" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F12" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G12" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H12" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I12" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J12" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K12" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L12" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M12" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N12" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C13" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D13" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E13" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F13" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G13" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H13" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I13" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J13" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K13" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L13" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M13" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N13" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C14" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D14" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E14" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F14" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G14" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H14" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I14" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J14" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K14" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L14" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M14" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N14" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C15" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D15" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E15" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F15" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G15" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H15" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I15" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J15" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K15" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L15" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M15" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N15" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C16" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D16" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E16" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F16" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G16" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H16" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I16" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J16" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K16" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L16" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M16" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N16" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C17" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D17" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E17" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F17" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G17" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H17" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I17" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J17" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K17" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L17" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M17" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N17" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C18" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D18" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E18" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F18" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G18" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H18" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I18" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J18" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K18" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L18" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M18" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N18" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C19" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D19" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E19" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F19" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G19" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H19" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I19" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J19" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K19" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L19" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M19" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N19" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C20" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D20" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E20" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F20" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G20" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H20" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I20" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J20" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K20" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L20" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M20" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N20" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C21" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D21" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E21" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F21" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G21" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H21" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I21" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J21" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K21" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L21" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M21" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N21" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C22" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D22" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E22" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F22" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G22" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H22" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I22" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J22" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K22" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L22" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M22" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N22" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C23" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D23" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E23" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F23" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G23" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H23" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I23" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J23" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K23" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L23" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M23" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N23" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C24" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D24" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E24" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F24" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G24" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H24" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I24" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J24" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K24" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L24" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M24" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N24" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C25" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D25" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E25" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F25" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G25" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H25" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I25" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J25" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K25" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L25" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M25" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N25" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C26" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D26" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E26" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F26" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G26" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H26" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I26" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J26" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K26" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L26" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M26" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N26" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C27" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D27" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E27" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F27" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G27" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H27" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I27" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J27" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K27" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L27" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M27" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N27" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C28" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D28" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E28" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F28" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G28" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F28" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G28" t="n">
+        <v>40270</v>
       </c>
       <c r="H28" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I28" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J28" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K28" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L28" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M28" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N28" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C29" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D29" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E29" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H29" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I29" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J29" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K29" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L29" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M29" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N29" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C30" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D30" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E30" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H30" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I30" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J30" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K30" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L30" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M30" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N30" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C31" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D31" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E31" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H31" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I31" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J31" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K31" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L31" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M31" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N31" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C32" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E32" t="n">
+        <v>749</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M32" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N32" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B33" t="n">
         <v>45267</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C33" t="n">
         <v>49710</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D33" t="n">
         <v>-1089</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E33" t="n">
         <v>-2353</v>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F33" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G33" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H33" t="n">
         <v>-751</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I33" t="n">
         <v>-1660</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J33" t="n">
         <v>-21534</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K33" t="n">
         <v>909</v>
       </c>
-      <c r="L32" t="n">
+      <c r="L33" t="n">
         <v>-338</v>
       </c>
-      <c r="M32" t="n">
+      <c r="M33" t="n">
         <v>-693</v>
       </c>
-      <c r="N32" t="n">
+      <c r="N33" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C33" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D33" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E33" t="n">
-        <v>793</v>
-      </c>
-      <c r="F33" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H33" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I33" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J33" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K33" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L33" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M33" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N33" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C34" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D34" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E34" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H34" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I34" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J34" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K34" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L34" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M34" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N34" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C35" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D35" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E35" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H35" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I35" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J35" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K35" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L35" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M35" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N35" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C36" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I36" t="n">
+        <v>557</v>
+      </c>
+      <c r="J36" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K36" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L36" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M36" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N36" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B37" t="n">
         <v>42514</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C37" t="n">
         <v>51801</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F37" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G37" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J36" t="n">
+      <c r="J37" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/20 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D2" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E2" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F2" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,41 +489,65 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D3" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E3" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F3" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F4" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B5" t="n">
         <v>202202</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>17571</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>892</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E5" t="n">
         <v>15673332</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="5"/>
+    <row r="6"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -536,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -563,27 +587,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -593,17 +617,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -613,7 +637,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -623,17 +647,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -643,47 +667,47 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -693,250 +717,260 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B40" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -951,7 +985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -983,494 +1017,507 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C2" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>-25.74</v>
       </c>
       <c r="C3" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C4" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C5" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C6" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C7" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C8" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C9" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C10" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C11" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C13" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C14" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C15" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C16" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C17" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C18" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C19" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C20" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C21" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C22" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C24" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C25" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C26" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C27" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C29" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C30" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C31" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C32" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C33" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C34" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C35" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C36" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C37" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C38" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C39" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B40" t="n">
         <v>24.64</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C40" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1485,7 +1532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1512,370 +1559,380 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B39" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1891,7 +1948,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1985,1632 +2042,1678 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C2" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D2" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E2" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F2" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G2" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H2" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I2" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J2" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K2" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L2" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M2" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N2" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C3" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D3" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E3" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F3" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G3" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H3" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I3" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J3" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K3" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L3" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M3" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N3" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C4" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D4" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E4" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F4" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G4" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H4" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I4" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J4" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K4" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L4" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M4" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N4" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C5" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D5" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E5" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F5" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G5" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H5" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I5" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J5" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K5" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L5" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M5" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N5" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C6" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D6" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E6" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F6" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G6" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H6" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I6" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J6" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K6" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L6" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M6" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N6" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C7" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D7" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E7" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F7" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G7" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H7" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I7" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J7" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K7" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L7" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M7" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N7" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C8" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D8" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E8" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F8" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G8" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H8" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I8" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J8" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K8" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L8" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M8" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N8" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C9" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D9" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E9" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F9" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G9" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H9" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I9" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J9" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K9" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L9" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M9" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N9" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C10" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D10" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E10" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F10" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G10" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H10" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I10" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J10" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K10" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L10" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M10" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N10" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C11" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D11" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E11" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F11" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G11" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H11" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I11" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J11" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K11" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L11" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M11" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N11" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C12" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D12" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E12" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F12" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G12" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H12" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I12" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J12" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K12" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L12" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M12" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N12" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C13" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D13" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E13" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F13" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G13" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H13" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I13" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J13" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K13" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L13" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M13" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N13" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C14" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D14" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E14" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F14" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G14" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H14" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I14" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J14" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K14" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L14" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M14" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N14" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C15" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D15" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E15" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F15" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G15" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H15" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I15" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J15" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K15" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L15" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M15" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N15" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C16" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D16" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E16" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F16" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G16" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H16" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I16" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J16" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K16" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L16" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M16" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N16" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C17" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D17" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E17" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F17" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G17" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H17" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I17" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J17" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K17" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L17" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M17" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N17" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C18" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D18" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E18" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F18" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G18" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H18" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I18" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J18" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K18" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L18" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M18" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N18" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C19" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D19" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E19" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F19" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G19" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H19" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I19" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J19" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K19" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L19" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M19" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N19" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C20" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D20" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E20" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F20" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G20" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H20" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I20" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J20" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K20" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L20" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M20" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N20" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C21" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D21" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E21" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F21" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G21" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H21" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I21" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J21" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K21" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L21" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M21" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N21" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C22" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D22" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E22" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F22" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G22" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H22" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I22" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J22" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K22" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L22" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M22" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N22" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C23" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D23" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E23" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F23" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G23" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H23" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I23" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J23" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K23" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L23" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M23" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N23" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C24" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D24" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E24" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F24" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G24" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H24" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I24" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J24" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K24" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L24" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M24" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N24" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C25" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D25" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E25" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F25" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G25" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H25" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I25" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J25" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K25" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L25" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M25" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N25" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C26" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D26" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E26" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F26" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G26" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H26" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I26" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J26" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K26" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L26" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M26" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N26" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C27" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D27" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E27" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F27" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G27" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H27" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I27" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J27" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K27" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L27" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M27" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N27" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C28" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D28" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E28" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F28" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G28" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H28" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I28" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J28" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K28" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L28" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M28" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N28" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C29" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D29" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E29" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G29" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F29" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G29" t="n">
+        <v>40270</v>
       </c>
       <c r="H29" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I29" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J29" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K29" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L29" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M29" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N29" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C30" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D30" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E30" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H30" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I30" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J30" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K30" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L30" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M30" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N30" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C31" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D31" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E31" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H31" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I31" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J31" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K31" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L31" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M31" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N31" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C32" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D32" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E32" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H32" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I32" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J32" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K32" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L32" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M32" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N32" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C33" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E33" t="n">
+        <v>749</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J33" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M33" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
         <v>45267</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C34" t="n">
         <v>49710</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D34" t="n">
         <v>-1089</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E34" t="n">
         <v>-2353</v>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F34" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G33" s="2" t="n">
+      <c r="G34" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H34" t="n">
         <v>-751</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I34" t="n">
         <v>-1660</v>
       </c>
-      <c r="J33" t="n">
+      <c r="J34" t="n">
         <v>-21534</v>
       </c>
-      <c r="K33" t="n">
+      <c r="K34" t="n">
         <v>909</v>
       </c>
-      <c r="L33" t="n">
+      <c r="L34" t="n">
         <v>-338</v>
       </c>
-      <c r="M33" t="n">
+      <c r="M34" t="n">
         <v>-693</v>
       </c>
-      <c r="N33" t="n">
+      <c r="N34" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C34" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D34" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E34" t="n">
-        <v>793</v>
-      </c>
-      <c r="F34" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G34" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H34" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I34" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J34" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K34" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L34" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M34" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N34" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C35" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D35" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E35" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H35" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I35" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J35" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K35" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L35" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M35" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N35" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C36" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D36" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E36" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H36" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I36" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J36" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K36" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L36" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M36" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N36" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C37" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H37" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I37" t="n">
+        <v>557</v>
+      </c>
+      <c r="J37" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K37" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L37" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M37" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N37" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B38" t="n">
         <v>42514</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C38" t="n">
         <v>51801</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F38" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G38" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J37" t="n">
+      <c r="J38" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/21 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17549</v>
+        <v>17766</v>
       </c>
       <c r="D2" t="n">
-        <v>2109</v>
+        <v>2462</v>
       </c>
       <c r="E2" t="n">
-        <v>11845575</v>
+        <v>6271398</v>
       </c>
       <c r="F2" t="n">
-        <v>17614</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D3" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E3" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F3" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,41 +513,65 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D4" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E4" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F4" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F5" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B6" t="n">
         <v>202202</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>17571</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>892</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>15673332</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F6" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="6"/>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -560,7 +584,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -587,37 +611,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -627,17 +651,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -647,7 +671,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -657,17 +681,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -677,47 +701,47 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -727,250 +751,260 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B41" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -985,7 +1019,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1017,507 +1051,520 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-194.23</v>
+        <v>106.52</v>
       </c>
       <c r="C2" t="n">
-        <v>50.75</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C3" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>-25.74</v>
       </c>
       <c r="C4" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C5" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C6" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C7" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C8" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C9" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C10" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C11" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C12" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C14" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C15" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C16" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C17" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C18" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C19" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C20" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C21" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C22" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C24" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C25" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C26" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C27" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C28" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C30" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C31" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C32" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C33" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C34" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C35" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C36" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C37" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C38" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C39" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C40" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B41" t="n">
         <v>24.64</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C41" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1532,7 +1579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1559,380 +1606,390 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17720.87</v>
+        <v>17748.15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B40" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -1948,7 +2005,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2042,1678 +2099,1724 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/20</t>
+          <t>2021/12/21</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46944</v>
+        <v>47439</v>
       </c>
       <c r="C2" t="n">
-        <v>55396</v>
+        <v>55318</v>
       </c>
       <c r="D2" t="n">
-        <v>1101</v>
+        <v>495</v>
       </c>
       <c r="E2" t="n">
-        <v>1087</v>
+        <v>-78</v>
       </c>
       <c r="F2" t="n">
-        <v>21589</v>
+        <v>22106</v>
       </c>
       <c r="G2" t="n">
-        <v>48231</v>
+        <v>47519</v>
       </c>
       <c r="H2" t="n">
-        <v>-426</v>
+        <v>517</v>
       </c>
       <c r="I2" t="n">
-        <v>802</v>
+        <v>-712</v>
       </c>
       <c r="J2" t="n">
-        <v>-26642</v>
+        <v>-25413</v>
       </c>
       <c r="K2" t="n">
-        <v>-1228</v>
+        <v>1229</v>
       </c>
       <c r="L2" t="n">
-        <v>1527</v>
+        <v>-22</v>
       </c>
       <c r="M2" t="n">
-        <v>285</v>
+        <v>634</v>
       </c>
       <c r="N2" t="n">
-        <v>1242</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C3" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D3" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E3" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F3" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G3" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H3" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I3" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J3" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K3" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L3" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M3" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N3" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C4" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D4" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E4" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F4" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G4" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H4" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I4" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J4" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K4" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L4" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M4" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N4" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C5" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D5" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E5" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F5" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G5" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H5" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I5" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J5" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K5" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L5" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M5" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N5" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C6" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D6" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E6" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F6" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G6" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H6" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I6" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J6" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K6" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L6" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M6" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N6" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C7" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D7" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E7" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F7" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G7" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H7" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I7" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J7" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K7" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L7" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M7" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N7" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C8" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D8" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E8" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F8" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G8" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H8" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I8" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J8" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K8" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L8" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M8" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N8" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C9" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D9" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E9" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F9" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G9" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H9" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I9" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J9" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K9" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L9" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M9" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N9" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C10" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D10" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E10" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F10" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G10" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H10" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I10" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J10" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K10" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L10" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M10" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N10" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C11" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D11" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E11" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F11" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G11" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H11" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I11" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J11" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K11" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L11" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M11" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N11" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C12" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D12" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E12" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F12" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G12" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H12" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I12" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J12" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K12" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L12" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M12" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N12" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C13" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D13" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E13" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F13" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G13" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H13" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I13" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J13" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K13" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L13" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M13" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N13" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C14" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D14" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E14" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F14" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G14" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H14" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I14" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J14" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K14" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L14" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M14" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N14" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C15" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D15" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E15" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F15" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G15" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H15" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I15" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J15" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K15" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L15" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M15" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N15" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C16" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D16" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E16" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F16" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G16" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H16" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I16" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J16" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K16" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L16" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M16" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N16" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C17" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D17" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E17" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F17" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G17" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H17" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I17" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J17" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K17" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L17" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M17" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N17" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C18" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D18" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E18" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F18" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G18" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H18" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I18" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J18" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K18" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L18" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M18" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N18" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C19" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D19" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E19" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F19" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G19" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H19" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I19" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J19" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K19" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L19" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M19" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N19" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C20" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D20" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E20" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F20" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G20" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H20" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I20" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J20" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K20" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L20" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M20" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N20" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C21" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D21" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E21" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F21" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G21" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H21" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I21" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J21" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K21" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L21" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M21" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N21" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C22" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D22" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E22" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F22" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G22" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H22" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I22" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J22" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K22" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L22" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M22" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N22" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C23" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D23" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E23" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F23" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G23" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H23" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I23" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J23" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K23" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L23" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M23" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N23" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C24" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D24" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E24" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F24" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G24" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H24" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I24" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J24" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K24" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L24" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M24" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N24" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C25" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D25" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E25" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F25" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G25" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H25" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I25" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J25" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K25" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L25" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M25" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N25" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C26" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D26" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E26" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F26" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G26" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H26" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I26" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J26" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K26" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L26" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M26" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N26" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C27" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D27" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E27" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F27" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G27" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H27" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I27" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J27" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K27" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L27" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M27" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N27" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C28" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D28" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E28" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F28" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G28" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H28" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I28" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J28" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K28" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L28" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M28" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N28" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C29" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D29" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E29" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F29" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G29" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H29" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I29" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J29" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K29" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L29" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M29" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N29" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C30" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D30" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E30" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F30" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G30" t="n">
+        <v>40270</v>
       </c>
       <c r="H30" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I30" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J30" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K30" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L30" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M30" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N30" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C31" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D31" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E31" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H31" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I31" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J31" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K31" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L31" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M31" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N31" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C32" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D32" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E32" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H32" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I32" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J32" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K32" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L32" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M32" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N32" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C33" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D33" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E33" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H33" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I33" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J33" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K33" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L33" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M33" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N33" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C34" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E34" t="n">
+        <v>749</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J34" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N34" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B35" t="n">
         <v>45267</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C35" t="n">
         <v>49710</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D35" t="n">
         <v>-1089</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E35" t="n">
         <v>-2353</v>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="F35" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G34" s="2" t="n">
+      <c r="G35" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H35" t="n">
         <v>-751</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I35" t="n">
         <v>-1660</v>
       </c>
-      <c r="J34" t="n">
+      <c r="J35" t="n">
         <v>-21534</v>
       </c>
-      <c r="K34" t="n">
+      <c r="K35" t="n">
         <v>909</v>
       </c>
-      <c r="L34" t="n">
+      <c r="L35" t="n">
         <v>-338</v>
       </c>
-      <c r="M34" t="n">
+      <c r="M35" t="n">
         <v>-693</v>
       </c>
-      <c r="N34" t="n">
+      <c r="N35" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C35" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D35" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E35" t="n">
-        <v>793</v>
-      </c>
-      <c r="F35" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G35" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H35" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I35" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J35" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K35" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L35" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M35" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N35" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C36" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D36" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E36" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H36" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I36" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J36" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K36" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L36" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M36" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N36" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C37" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D37" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E37" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H37" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I37" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J37" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K37" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L37" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M37" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N37" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C38" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I38" t="n">
+        <v>557</v>
+      </c>
+      <c r="J38" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K38" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L38" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M38" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N38" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B39" t="n">
         <v>42514</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C39" t="n">
         <v>51801</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F39" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G38" s="2" t="n">
+      <c r="G39" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J38" t="n">
+      <c r="J39" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/22 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17766</v>
+        <v>17802</v>
       </c>
       <c r="D2" t="n">
-        <v>2462</v>
+        <v>2496</v>
       </c>
       <c r="E2" t="n">
-        <v>6271398</v>
+        <v>605268</v>
       </c>
       <c r="F2" t="n">
-        <v>17636</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17549</v>
+        <v>17766</v>
       </c>
       <c r="D3" t="n">
-        <v>2109</v>
+        <v>2462</v>
       </c>
       <c r="E3" t="n">
-        <v>11845575</v>
+        <v>6271398</v>
       </c>
       <c r="F3" t="n">
-        <v>17614</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D4" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E4" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F4" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,41 +537,65 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D5" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E5" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F5" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F6" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>202202</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C7" t="n">
         <v>17571</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>892</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E7" t="n">
         <v>15673332</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F7" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="7"/>
+    <row r="8"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -584,7 +608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -611,7 +635,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -621,37 +645,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -661,17 +685,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -681,7 +705,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -691,17 +715,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -711,47 +735,47 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -761,250 +785,260 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B42" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1019,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1051,520 +1085,533 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>106.52</v>
+        <v>17.7</v>
       </c>
       <c r="C2" t="n">
-        <v>13.64</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-194.23</v>
+        <v>106.52</v>
       </c>
       <c r="C3" t="n">
-        <v>50.75</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C4" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>-25.74</v>
       </c>
       <c r="C5" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C6" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C7" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C8" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C9" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C10" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C11" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C12" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C13" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C15" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C16" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C17" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C18" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C19" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C20" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C21" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C22" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C23" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C24" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C26" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C27" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C28" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C29" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C30" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C32" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C33" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C34" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C35" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C36" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C37" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C38" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C39" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C40" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C41" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B42" t="n">
         <v>24.64</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C42" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1579,7 +1626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1606,390 +1653,400 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17748.15</v>
+        <v>17835.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17720.87</v>
+        <v>17748.15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B41" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2005,7 +2062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2099,1724 +2156,1770 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/21</t>
+          <t>2021/12/22</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47439</v>
+        <v>46323</v>
       </c>
       <c r="C2" t="n">
-        <v>55318</v>
+        <v>53049</v>
       </c>
       <c r="D2" t="n">
-        <v>495</v>
+        <v>-1116</v>
       </c>
       <c r="E2" t="n">
-        <v>-78</v>
+        <v>-2269</v>
       </c>
       <c r="F2" t="n">
-        <v>22106</v>
+        <v>21197</v>
       </c>
       <c r="G2" t="n">
-        <v>47519</v>
+        <v>45391</v>
       </c>
       <c r="H2" t="n">
-        <v>517</v>
+        <v>-909</v>
       </c>
       <c r="I2" t="n">
-        <v>-712</v>
+        <v>-2128</v>
       </c>
       <c r="J2" t="n">
-        <v>-25413</v>
+        <v>-24194</v>
       </c>
       <c r="K2" t="n">
-        <v>1229</v>
+        <v>1219</v>
       </c>
       <c r="L2" t="n">
-        <v>-22</v>
+        <v>-207</v>
       </c>
       <c r="M2" t="n">
-        <v>634</v>
+        <v>-141</v>
       </c>
       <c r="N2" t="n">
-        <v>-656</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/20</t>
+          <t>2021/12/21</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46944</v>
+        <v>47439</v>
       </c>
       <c r="C3" t="n">
-        <v>55396</v>
+        <v>55318</v>
       </c>
       <c r="D3" t="n">
-        <v>1101</v>
+        <v>495</v>
       </c>
       <c r="E3" t="n">
-        <v>1087</v>
+        <v>-78</v>
       </c>
       <c r="F3" t="n">
-        <v>21589</v>
+        <v>22106</v>
       </c>
       <c r="G3" t="n">
-        <v>48231</v>
+        <v>47519</v>
       </c>
       <c r="H3" t="n">
-        <v>-426</v>
+        <v>517</v>
       </c>
       <c r="I3" t="n">
-        <v>802</v>
+        <v>-712</v>
       </c>
       <c r="J3" t="n">
-        <v>-26642</v>
+        <v>-25413</v>
       </c>
       <c r="K3" t="n">
-        <v>-1228</v>
+        <v>1229</v>
       </c>
       <c r="L3" t="n">
-        <v>1527</v>
+        <v>-22</v>
       </c>
       <c r="M3" t="n">
-        <v>285</v>
+        <v>634</v>
       </c>
       <c r="N3" t="n">
-        <v>1242</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C4" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D4" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E4" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F4" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G4" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H4" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I4" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J4" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K4" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L4" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M4" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N4" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C5" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D5" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E5" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F5" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G5" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H5" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I5" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J5" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K5" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L5" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M5" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N5" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C6" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D6" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E6" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F6" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G6" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H6" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I6" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J6" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K6" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L6" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M6" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N6" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C7" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D7" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E7" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F7" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G7" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H7" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I7" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J7" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K7" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L7" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M7" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N7" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C8" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D8" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E8" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F8" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G8" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H8" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I8" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J8" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K8" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L8" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M8" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N8" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C9" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D9" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E9" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F9" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G9" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H9" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I9" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J9" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K9" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L9" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M9" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N9" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C10" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D10" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E10" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F10" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G10" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H10" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I10" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J10" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K10" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L10" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M10" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N10" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C11" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D11" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E11" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F11" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G11" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H11" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I11" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J11" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K11" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L11" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M11" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N11" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C12" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D12" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E12" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F12" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G12" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H12" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I12" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J12" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K12" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L12" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M12" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N12" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C13" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D13" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E13" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F13" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G13" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H13" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I13" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J13" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K13" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L13" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M13" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N13" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C14" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D14" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E14" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F14" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G14" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H14" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I14" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J14" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K14" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L14" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M14" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N14" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C15" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D15" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E15" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F15" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G15" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H15" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I15" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J15" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K15" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L15" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M15" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N15" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C16" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D16" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E16" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F16" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G16" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H16" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I16" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J16" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K16" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L16" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M16" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N16" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C17" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D17" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E17" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F17" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G17" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H17" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I17" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J17" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K17" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L17" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M17" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N17" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C18" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D18" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E18" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F18" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G18" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H18" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I18" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J18" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K18" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L18" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M18" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N18" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C19" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D19" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E19" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F19" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G19" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H19" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I19" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J19" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K19" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L19" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M19" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N19" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C20" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D20" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E20" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F20" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G20" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H20" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I20" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J20" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K20" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L20" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M20" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N20" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C21" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D21" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E21" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F21" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G21" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H21" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I21" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J21" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K21" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L21" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M21" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N21" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C22" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D22" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E22" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F22" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G22" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H22" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I22" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J22" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K22" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L22" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M22" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N22" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C23" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D23" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E23" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F23" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G23" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H23" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I23" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J23" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K23" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L23" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M23" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N23" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C24" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D24" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E24" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F24" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G24" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H24" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I24" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J24" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K24" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L24" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M24" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N24" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C25" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D25" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E25" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F25" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G25" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H25" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I25" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J25" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K25" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L25" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M25" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N25" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C26" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D26" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E26" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F26" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G26" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H26" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I26" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J26" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K26" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L26" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M26" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N26" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C27" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D27" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E27" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F27" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G27" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H27" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I27" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J27" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K27" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L27" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M27" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N27" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C28" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D28" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E28" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F28" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G28" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H28" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I28" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J28" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K28" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L28" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M28" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N28" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C29" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D29" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E29" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F29" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G29" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H29" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I29" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J29" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K29" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L29" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M29" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N29" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C30" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D30" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E30" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F30" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G30" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H30" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I30" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J30" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K30" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L30" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M30" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N30" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C31" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D31" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E31" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G31" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F31" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G31" t="n">
+        <v>40270</v>
       </c>
       <c r="H31" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I31" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J31" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K31" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L31" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M31" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N31" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C32" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D32" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E32" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H32" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I32" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J32" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K32" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L32" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M32" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N32" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C33" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D33" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E33" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H33" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I33" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J33" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K33" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L33" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M33" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N33" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C34" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D34" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E34" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H34" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I34" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J34" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K34" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L34" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M34" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N34" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C35" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E35" t="n">
+        <v>749</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J35" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M35" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N35" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B36" t="n">
         <v>45267</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C36" t="n">
         <v>49710</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D36" t="n">
         <v>-1089</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E36" t="n">
         <v>-2353</v>
       </c>
-      <c r="F35" s="2" t="n">
+      <c r="F36" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G35" s="2" t="n">
+      <c r="G36" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H36" t="n">
         <v>-751</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I36" t="n">
         <v>-1660</v>
       </c>
-      <c r="J35" t="n">
+      <c r="J36" t="n">
         <v>-21534</v>
       </c>
-      <c r="K35" t="n">
+      <c r="K36" t="n">
         <v>909</v>
       </c>
-      <c r="L35" t="n">
+      <c r="L36" t="n">
         <v>-338</v>
       </c>
-      <c r="M35" t="n">
+      <c r="M36" t="n">
         <v>-693</v>
       </c>
-      <c r="N35" t="n">
+      <c r="N36" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C36" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D36" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E36" t="n">
-        <v>793</v>
-      </c>
-      <c r="F36" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G36" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H36" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I36" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J36" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K36" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M36" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N36" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C37" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D37" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E37" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H37" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I37" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J37" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K37" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L37" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M37" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N37" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C38" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D38" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E38" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H38" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I38" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J38" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K38" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L38" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M38" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N38" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C39" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I39" t="n">
+        <v>557</v>
+      </c>
+      <c r="J39" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K39" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L39" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M39" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N39" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B40" t="n">
         <v>42514</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C40" t="n">
         <v>51801</v>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="F40" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G39" s="2" t="n">
+      <c r="G40" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J39" t="n">
+      <c r="J40" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/23 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17802</v>
+        <v>17922</v>
       </c>
       <c r="D2" t="n">
-        <v>2496</v>
+        <v>2735</v>
       </c>
       <c r="E2" t="n">
-        <v>605268</v>
+        <v>4283358</v>
       </c>
       <c r="F2" t="n">
-        <v>17638</v>
+        <v>17663</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17766</v>
+        <v>17802</v>
       </c>
       <c r="D3" t="n">
-        <v>2462</v>
+        <v>2496</v>
       </c>
       <c r="E3" t="n">
-        <v>6271398</v>
+        <v>605268</v>
       </c>
       <c r="F3" t="n">
-        <v>17636</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17549</v>
+        <v>17766</v>
       </c>
       <c r="D4" t="n">
-        <v>2109</v>
+        <v>2462</v>
       </c>
       <c r="E4" t="n">
-        <v>11845575</v>
+        <v>6271398</v>
       </c>
       <c r="F4" t="n">
-        <v>17614</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D5" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E5" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F5" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,41 +561,65 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D6" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E6" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F6" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F7" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" t="n">
         <v>202202</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C8" t="n">
         <v>17571</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>892</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E8" t="n">
         <v>15673332</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F8" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="8"/>
+    <row r="9"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -608,7 +632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -635,17 +659,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.08</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -655,37 +679,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -695,17 +719,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -715,7 +739,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -725,17 +749,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -745,47 +769,47 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -795,250 +819,260 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B43" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1053,7 +1087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1085,533 +1119,546 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17.7</v>
+        <v>180.23</v>
       </c>
       <c r="C2" t="n">
-        <v>19.86</v>
+        <v>-60.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>106.52</v>
+        <v>17.7</v>
       </c>
       <c r="C3" t="n">
-        <v>13.64</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-194.23</v>
+        <v>106.52</v>
       </c>
       <c r="C4" t="n">
-        <v>50.75</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C5" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>-25.74</v>
       </c>
       <c r="C6" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C7" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C8" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C9" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C10" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C11" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C12" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C13" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C14" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C16" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C17" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C18" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C19" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C20" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C21" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C22" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C23" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C24" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C26" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C27" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C28" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C29" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C30" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C31" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C32" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C33" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C34" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C35" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C36" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C37" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C38" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C39" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C40" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C41" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C42" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B43" t="n">
         <v>24.64</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C43" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1626,7 +1673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1653,400 +1700,410 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17835.4</v>
+        <v>17931.41</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17748.15</v>
+        <v>17835.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17720.87</v>
+        <v>17748.15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B42" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2062,7 +2119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2156,1770 +2213,1816 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/22</t>
+          <t>2021/12/23</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46323</v>
+        <v>45936</v>
       </c>
       <c r="C2" t="n">
-        <v>53049</v>
+        <v>52465</v>
       </c>
       <c r="D2" t="n">
-        <v>-1116</v>
+        <v>-387</v>
       </c>
       <c r="E2" t="n">
-        <v>-2269</v>
+        <v>-584</v>
       </c>
       <c r="F2" t="n">
-        <v>21197</v>
+        <v>22282</v>
       </c>
       <c r="G2" t="n">
-        <v>45391</v>
+        <v>46148</v>
       </c>
       <c r="H2" t="n">
-        <v>-909</v>
+        <v>1085</v>
       </c>
       <c r="I2" t="n">
-        <v>-2128</v>
+        <v>757</v>
       </c>
       <c r="J2" t="n">
-        <v>-24194</v>
+        <v>-23866</v>
       </c>
       <c r="K2" t="n">
-        <v>1219</v>
+        <v>328</v>
       </c>
       <c r="L2" t="n">
-        <v>-207</v>
+        <v>-1472</v>
       </c>
       <c r="M2" t="n">
-        <v>-141</v>
+        <v>-1341</v>
       </c>
       <c r="N2" t="n">
-        <v>-66</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/21</t>
+          <t>2021/12/22</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47439</v>
+        <v>46323</v>
       </c>
       <c r="C3" t="n">
-        <v>55318</v>
+        <v>53049</v>
       </c>
       <c r="D3" t="n">
-        <v>495</v>
+        <v>-1116</v>
       </c>
       <c r="E3" t="n">
-        <v>-78</v>
+        <v>-2269</v>
       </c>
       <c r="F3" t="n">
-        <v>22106</v>
+        <v>21197</v>
       </c>
       <c r="G3" t="n">
-        <v>47519</v>
+        <v>45391</v>
       </c>
       <c r="H3" t="n">
-        <v>517</v>
+        <v>-909</v>
       </c>
       <c r="I3" t="n">
-        <v>-712</v>
+        <v>-2128</v>
       </c>
       <c r="J3" t="n">
-        <v>-25413</v>
+        <v>-24194</v>
       </c>
       <c r="K3" t="n">
-        <v>1229</v>
+        <v>1219</v>
       </c>
       <c r="L3" t="n">
-        <v>-22</v>
+        <v>-207</v>
       </c>
       <c r="M3" t="n">
-        <v>634</v>
+        <v>-141</v>
       </c>
       <c r="N3" t="n">
-        <v>-656</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/20</t>
+          <t>2021/12/21</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46944</v>
+        <v>47439</v>
       </c>
       <c r="C4" t="n">
-        <v>55396</v>
+        <v>55318</v>
       </c>
       <c r="D4" t="n">
-        <v>1101</v>
+        <v>495</v>
       </c>
       <c r="E4" t="n">
-        <v>1087</v>
+        <v>-78</v>
       </c>
       <c r="F4" t="n">
-        <v>21589</v>
+        <v>22106</v>
       </c>
       <c r="G4" t="n">
-        <v>48231</v>
+        <v>47519</v>
       </c>
       <c r="H4" t="n">
-        <v>-426</v>
+        <v>517</v>
       </c>
       <c r="I4" t="n">
-        <v>802</v>
+        <v>-712</v>
       </c>
       <c r="J4" t="n">
-        <v>-26642</v>
+        <v>-25413</v>
       </c>
       <c r="K4" t="n">
-        <v>-1228</v>
+        <v>1229</v>
       </c>
       <c r="L4" t="n">
-        <v>1527</v>
+        <v>-22</v>
       </c>
       <c r="M4" t="n">
-        <v>285</v>
+        <v>634</v>
       </c>
       <c r="N4" t="n">
-        <v>1242</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C5" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D5" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E5" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F5" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G5" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H5" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I5" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J5" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K5" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L5" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M5" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N5" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C6" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D6" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E6" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F6" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G6" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H6" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I6" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J6" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K6" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L6" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M6" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N6" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C7" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D7" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E7" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F7" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G7" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H7" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I7" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J7" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K7" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L7" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M7" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N7" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C8" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D8" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E8" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F8" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G8" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H8" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I8" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J8" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K8" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L8" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M8" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N8" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C9" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D9" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E9" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F9" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G9" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H9" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I9" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J9" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K9" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L9" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M9" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N9" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C10" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D10" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E10" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F10" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G10" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H10" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I10" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J10" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K10" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L10" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M10" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N10" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C11" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D11" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E11" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F11" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G11" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H11" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I11" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J11" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K11" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L11" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M11" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N11" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C12" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D12" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E12" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F12" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G12" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H12" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I12" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J12" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K12" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L12" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M12" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N12" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C13" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D13" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E13" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F13" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G13" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H13" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I13" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J13" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K13" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L13" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M13" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N13" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C14" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D14" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E14" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F14" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G14" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H14" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I14" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J14" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K14" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L14" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M14" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N14" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C15" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D15" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E15" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F15" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G15" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H15" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I15" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J15" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K15" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L15" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M15" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N15" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C16" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D16" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E16" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F16" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G16" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H16" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I16" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J16" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K16" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L16" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M16" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N16" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C17" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D17" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E17" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F17" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G17" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H17" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I17" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J17" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K17" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L17" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M17" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N17" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C18" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D18" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E18" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F18" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G18" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H18" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I18" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J18" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K18" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L18" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M18" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N18" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C19" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D19" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E19" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F19" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G19" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H19" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I19" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J19" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K19" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L19" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M19" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N19" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C20" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D20" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E20" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F20" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G20" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H20" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I20" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J20" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K20" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L20" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M20" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N20" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C21" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D21" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E21" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F21" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G21" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H21" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I21" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J21" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K21" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L21" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M21" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N21" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C22" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D22" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E22" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F22" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G22" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H22" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I22" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J22" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K22" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L22" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M22" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N22" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C23" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D23" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E23" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F23" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G23" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H23" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I23" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J23" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K23" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L23" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M23" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N23" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C24" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D24" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E24" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F24" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G24" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H24" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I24" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J24" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K24" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L24" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M24" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N24" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C25" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D25" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E25" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F25" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G25" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H25" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I25" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J25" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K25" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L25" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M25" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N25" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C26" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D26" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E26" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F26" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G26" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H26" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I26" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J26" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K26" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L26" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M26" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N26" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C27" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D27" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E27" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F27" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G27" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H27" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I27" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J27" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K27" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L27" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M27" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N27" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C28" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D28" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E28" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F28" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G28" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H28" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I28" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J28" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K28" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L28" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M28" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N28" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C29" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D29" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E29" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F29" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G29" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H29" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I29" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J29" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K29" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L29" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M29" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N29" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C30" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D30" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E30" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F30" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G30" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H30" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I30" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J30" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K30" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L30" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M30" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N30" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C31" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D31" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E31" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F31" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G31" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H31" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I31" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J31" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K31" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L31" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M31" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N31" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C32" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D32" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E32" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F32" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G32" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F32" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G32" t="n">
+        <v>40270</v>
       </c>
       <c r="H32" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I32" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J32" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K32" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L32" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M32" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N32" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C33" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D33" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E33" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H33" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I33" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J33" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K33" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L33" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M33" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N33" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C34" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D34" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E34" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H34" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I34" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J34" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K34" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L34" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M34" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N34" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C35" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D35" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E35" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H35" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I35" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J35" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K35" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L35" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M35" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N35" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C36" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E36" t="n">
+        <v>749</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J36" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K36" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M36" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N36" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B37" t="n">
         <v>45267</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C37" t="n">
         <v>49710</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D37" t="n">
         <v>-1089</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E37" t="n">
         <v>-2353</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F37" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G37" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H37" t="n">
         <v>-751</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I37" t="n">
         <v>-1660</v>
       </c>
-      <c r="J36" t="n">
+      <c r="J37" t="n">
         <v>-21534</v>
       </c>
-      <c r="K36" t="n">
+      <c r="K37" t="n">
         <v>909</v>
       </c>
-      <c r="L36" t="n">
+      <c r="L37" t="n">
         <v>-338</v>
       </c>
-      <c r="M36" t="n">
+      <c r="M37" t="n">
         <v>-693</v>
       </c>
-      <c r="N36" t="n">
+      <c r="N37" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C37" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D37" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E37" t="n">
-        <v>793</v>
-      </c>
-      <c r="F37" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G37" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H37" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I37" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J37" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K37" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L37" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M37" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N37" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C38" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D38" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E38" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H38" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I38" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J38" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K38" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L38" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M38" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N38" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C39" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D39" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E39" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H39" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I39" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J39" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K39" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L39" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M39" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N39" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C40" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H40" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I40" t="n">
+        <v>557</v>
+      </c>
+      <c r="J40" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K40" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L40" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M40" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N40" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B41" t="n">
         <v>42514</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C41" t="n">
         <v>51801</v>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="F41" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G40" s="2" t="n">
+      <c r="G41" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J40" t="n">
+      <c r="J41" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/24 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/23</t>
+          <t>日期：2021/12/24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17922</v>
+        <v>17925</v>
       </c>
       <c r="D2" t="n">
-        <v>2735</v>
+        <v>2905</v>
       </c>
       <c r="E2" t="n">
-        <v>4283358</v>
+        <v>3047250</v>
       </c>
       <c r="F2" t="n">
-        <v>17663</v>
+        <v>17678</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17802</v>
+        <v>17922</v>
       </c>
       <c r="D3" t="n">
-        <v>2496</v>
+        <v>2735</v>
       </c>
       <c r="E3" t="n">
-        <v>605268</v>
+        <v>4283358</v>
       </c>
       <c r="F3" t="n">
-        <v>17638</v>
+        <v>17663</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17766</v>
+        <v>17802</v>
       </c>
       <c r="D4" t="n">
-        <v>2462</v>
+        <v>2496</v>
       </c>
       <c r="E4" t="n">
-        <v>6271398</v>
+        <v>605268</v>
       </c>
       <c r="F4" t="n">
-        <v>17636</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17549</v>
+        <v>17766</v>
       </c>
       <c r="D5" t="n">
-        <v>2109</v>
+        <v>2462</v>
       </c>
       <c r="E5" t="n">
-        <v>11845575</v>
+        <v>6271398</v>
       </c>
       <c r="F5" t="n">
-        <v>17614</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D6" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E6" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F6" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,41 +585,65 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D7" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E7" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F7" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F8" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B9" t="n">
         <v>202202</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C9" t="n">
         <v>17571</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>892</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" t="n">
         <v>15673332</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F9" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="9"/>
+    <row r="10"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -632,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -659,27 +683,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/23</t>
+          <t>日期：2021/12/24</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -689,37 +713,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -729,17 +753,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -749,7 +773,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -759,17 +783,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -779,47 +803,47 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -829,250 +853,260 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B44" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1087,7 +1121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1119,546 +1153,559 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月23日</t>
+          <t>110年12月24日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>180.23</v>
+        <v>86.02</v>
       </c>
       <c r="C2" t="n">
-        <v>-60.4</v>
+        <v>-71.04000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17.7</v>
+        <v>180.23</v>
       </c>
       <c r="C3" t="n">
-        <v>19.86</v>
+        <v>-60.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>106.52</v>
+        <v>17.7</v>
       </c>
       <c r="C4" t="n">
-        <v>13.64</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-194.23</v>
+        <v>106.52</v>
       </c>
       <c r="C5" t="n">
-        <v>50.75</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C6" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>-25.74</v>
       </c>
       <c r="C7" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C8" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C9" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C10" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C11" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C12" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C13" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C14" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C15" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C16" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C17" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C18" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C19" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C20" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C21" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C22" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C23" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C24" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C25" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C26" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C28" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C29" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C30" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C31" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C32" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C33" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C34" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C35" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C36" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C37" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C38" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C39" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C40" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C41" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C42" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C43" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B44" t="n">
         <v>24.64</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C44" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1673,7 +1720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1700,410 +1747,420 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月23日</t>
+          <t>110年12月24日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17931.41</v>
+        <v>17996.55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17835.4</v>
+        <v>17931.41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17748.15</v>
+        <v>17835.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17720.87</v>
+        <v>17748.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B43" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2119,7 +2176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2213,1816 +2270,1862 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/23</t>
+          <t>2021/12/24</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45936</v>
+        <v>46586</v>
       </c>
       <c r="C2" t="n">
-        <v>52465</v>
+        <v>53749</v>
       </c>
       <c r="D2" t="n">
-        <v>-387</v>
+        <v>650</v>
       </c>
       <c r="E2" t="n">
-        <v>-584</v>
+        <v>1284</v>
       </c>
       <c r="F2" t="n">
-        <v>22282</v>
+        <v>23007</v>
       </c>
       <c r="G2" t="n">
-        <v>46148</v>
+        <v>47663</v>
       </c>
       <c r="H2" t="n">
-        <v>1085</v>
+        <v>725</v>
       </c>
       <c r="I2" t="n">
-        <v>757</v>
+        <v>1515</v>
       </c>
       <c r="J2" t="n">
-        <v>-23866</v>
+        <v>-24656</v>
       </c>
       <c r="K2" t="n">
-        <v>328</v>
+        <v>-790</v>
       </c>
       <c r="L2" t="n">
-        <v>-1472</v>
+        <v>-75</v>
       </c>
       <c r="M2" t="n">
-        <v>-1341</v>
+        <v>-231</v>
       </c>
       <c r="N2" t="n">
-        <v>-131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/22</t>
+          <t>2021/12/23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46323</v>
+        <v>45936</v>
       </c>
       <c r="C3" t="n">
-        <v>53049</v>
+        <v>52465</v>
       </c>
       <c r="D3" t="n">
-        <v>-1116</v>
+        <v>-387</v>
       </c>
       <c r="E3" t="n">
-        <v>-2269</v>
+        <v>-584</v>
       </c>
       <c r="F3" t="n">
-        <v>21197</v>
+        <v>22282</v>
       </c>
       <c r="G3" t="n">
-        <v>45391</v>
+        <v>46148</v>
       </c>
       <c r="H3" t="n">
-        <v>-909</v>
+        <v>1085</v>
       </c>
       <c r="I3" t="n">
-        <v>-2128</v>
+        <v>757</v>
       </c>
       <c r="J3" t="n">
-        <v>-24194</v>
+        <v>-23866</v>
       </c>
       <c r="K3" t="n">
-        <v>1219</v>
+        <v>328</v>
       </c>
       <c r="L3" t="n">
-        <v>-207</v>
+        <v>-1472</v>
       </c>
       <c r="M3" t="n">
-        <v>-141</v>
+        <v>-1341</v>
       </c>
       <c r="N3" t="n">
-        <v>-66</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/21</t>
+          <t>2021/12/22</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47439</v>
+        <v>46323</v>
       </c>
       <c r="C4" t="n">
-        <v>55318</v>
+        <v>53049</v>
       </c>
       <c r="D4" t="n">
-        <v>495</v>
+        <v>-1116</v>
       </c>
       <c r="E4" t="n">
-        <v>-78</v>
+        <v>-2269</v>
       </c>
       <c r="F4" t="n">
-        <v>22106</v>
+        <v>21197</v>
       </c>
       <c r="G4" t="n">
-        <v>47519</v>
+        <v>45391</v>
       </c>
       <c r="H4" t="n">
-        <v>517</v>
+        <v>-909</v>
       </c>
       <c r="I4" t="n">
-        <v>-712</v>
+        <v>-2128</v>
       </c>
       <c r="J4" t="n">
-        <v>-25413</v>
+        <v>-24194</v>
       </c>
       <c r="K4" t="n">
-        <v>1229</v>
+        <v>1219</v>
       </c>
       <c r="L4" t="n">
-        <v>-22</v>
+        <v>-207</v>
       </c>
       <c r="M4" t="n">
-        <v>634</v>
+        <v>-141</v>
       </c>
       <c r="N4" t="n">
-        <v>-656</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/20</t>
+          <t>2021/12/21</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46944</v>
+        <v>47439</v>
       </c>
       <c r="C5" t="n">
-        <v>55396</v>
+        <v>55318</v>
       </c>
       <c r="D5" t="n">
-        <v>1101</v>
+        <v>495</v>
       </c>
       <c r="E5" t="n">
-        <v>1087</v>
+        <v>-78</v>
       </c>
       <c r="F5" t="n">
-        <v>21589</v>
+        <v>22106</v>
       </c>
       <c r="G5" t="n">
-        <v>48231</v>
+        <v>47519</v>
       </c>
       <c r="H5" t="n">
-        <v>-426</v>
+        <v>517</v>
       </c>
       <c r="I5" t="n">
-        <v>802</v>
+        <v>-712</v>
       </c>
       <c r="J5" t="n">
-        <v>-26642</v>
+        <v>-25413</v>
       </c>
       <c r="K5" t="n">
-        <v>-1228</v>
+        <v>1229</v>
       </c>
       <c r="L5" t="n">
-        <v>1527</v>
+        <v>-22</v>
       </c>
       <c r="M5" t="n">
-        <v>285</v>
+        <v>634</v>
       </c>
       <c r="N5" t="n">
-        <v>1242</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C6" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D6" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E6" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F6" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G6" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H6" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I6" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J6" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K6" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L6" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M6" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N6" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C7" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D7" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E7" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F7" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G7" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H7" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I7" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J7" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K7" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L7" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M7" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N7" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C8" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D8" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E8" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F8" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G8" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H8" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I8" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J8" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K8" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L8" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M8" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N8" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C9" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D9" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E9" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F9" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G9" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H9" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I9" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J9" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K9" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L9" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M9" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N9" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C10" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D10" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E10" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F10" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G10" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H10" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I10" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J10" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K10" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L10" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M10" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N10" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C11" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D11" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E11" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F11" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G11" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H11" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I11" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J11" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K11" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L11" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M11" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N11" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C12" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D12" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E12" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F12" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G12" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H12" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I12" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J12" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K12" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L12" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M12" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N12" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C13" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D13" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E13" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F13" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G13" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H13" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I13" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J13" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K13" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L13" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M13" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N13" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C14" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D14" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E14" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F14" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G14" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H14" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I14" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J14" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K14" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L14" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M14" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N14" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C15" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D15" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E15" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F15" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G15" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H15" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I15" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J15" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K15" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L15" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M15" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N15" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C16" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D16" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E16" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F16" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G16" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H16" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I16" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J16" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K16" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L16" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M16" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N16" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C17" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D17" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E17" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F17" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G17" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H17" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I17" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J17" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K17" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L17" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M17" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N17" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C18" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D18" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E18" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F18" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G18" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H18" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I18" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J18" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K18" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L18" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M18" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N18" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C19" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D19" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E19" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F19" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G19" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H19" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I19" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J19" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K19" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L19" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M19" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N19" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C20" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D20" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E20" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F20" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G20" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H20" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I20" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J20" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K20" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L20" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M20" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N20" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C21" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D21" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E21" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F21" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G21" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H21" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I21" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J21" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K21" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L21" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M21" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N21" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C22" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D22" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E22" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F22" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G22" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H22" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I22" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J22" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K22" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L22" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M22" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N22" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C23" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D23" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E23" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F23" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G23" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H23" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I23" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J23" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K23" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L23" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M23" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N23" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C24" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D24" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E24" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F24" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G24" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H24" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I24" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J24" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K24" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L24" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M24" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N24" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C25" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D25" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E25" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F25" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G25" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H25" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I25" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J25" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K25" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L25" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M25" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N25" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C26" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D26" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E26" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F26" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G26" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H26" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I26" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J26" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K26" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L26" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M26" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N26" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C27" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D27" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E27" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F27" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G27" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H27" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I27" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J27" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K27" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L27" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M27" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N27" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C28" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D28" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E28" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F28" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G28" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H28" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I28" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J28" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K28" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L28" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M28" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N28" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C29" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D29" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E29" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F29" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G29" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H29" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I29" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J29" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K29" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L29" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M29" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N29" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C30" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D30" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E30" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F30" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G30" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H30" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I30" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J30" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K30" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L30" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M30" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N30" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C31" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D31" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E31" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F31" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G31" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H31" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I31" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J31" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K31" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L31" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M31" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N31" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C32" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D32" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E32" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F32" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G32" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H32" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I32" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J32" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K32" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L32" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M32" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N32" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C33" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D33" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E33" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F33" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F33" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G33" t="n">
+        <v>40270</v>
       </c>
       <c r="H33" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I33" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J33" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K33" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L33" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M33" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N33" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C34" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D34" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E34" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H34" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I34" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J34" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K34" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L34" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M34" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N34" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C35" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D35" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E35" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H35" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I35" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J35" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K35" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L35" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M35" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N35" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C36" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D36" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E36" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H36" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I36" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J36" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K36" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L36" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M36" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N36" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C37" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E37" t="n">
+        <v>749</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H37" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J37" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K37" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L37" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M37" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N37" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B38" t="n">
         <v>45267</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C38" t="n">
         <v>49710</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D38" t="n">
         <v>-1089</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E38" t="n">
         <v>-2353</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F38" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G38" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H37" t="n">
+      <c r="H38" t="n">
         <v>-751</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I38" t="n">
         <v>-1660</v>
       </c>
-      <c r="J37" t="n">
+      <c r="J38" t="n">
         <v>-21534</v>
       </c>
-      <c r="K37" t="n">
+      <c r="K38" t="n">
         <v>909</v>
       </c>
-      <c r="L37" t="n">
+      <c r="L38" t="n">
         <v>-338</v>
       </c>
-      <c r="M37" t="n">
+      <c r="M38" t="n">
         <v>-693</v>
       </c>
-      <c r="N37" t="n">
+      <c r="N38" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C38" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D38" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E38" t="n">
-        <v>793</v>
-      </c>
-      <c r="F38" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G38" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H38" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I38" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J38" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K38" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L38" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M38" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N38" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C39" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D39" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E39" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H39" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I39" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J39" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K39" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L39" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M39" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N39" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C40" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D40" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E40" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H40" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I40" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J40" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K40" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L40" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M40" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N40" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C41" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H41" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I41" t="n">
+        <v>557</v>
+      </c>
+      <c r="J41" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K41" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L41" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M41" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N41" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B42" t="n">
         <v>42514</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C42" t="n">
         <v>51801</v>
       </c>
-      <c r="F41" s="2" t="n">
+      <c r="F42" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G41" s="2" t="n">
+      <c r="G42" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J41" t="n">
+      <c r="J42" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/27 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/24</t>
+          <t>日期：2021/12/27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17925</v>
+        <v>18036</v>
       </c>
       <c r="D2" t="n">
-        <v>2905</v>
+        <v>3054</v>
       </c>
       <c r="E2" t="n">
-        <v>3047250</v>
+        <v>2687364</v>
       </c>
       <c r="F2" t="n">
-        <v>17678</v>
+        <v>17695</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/23</t>
+          <t>日期：2021/12/24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17922</v>
+        <v>17925</v>
       </c>
       <c r="D3" t="n">
-        <v>2735</v>
+        <v>2905</v>
       </c>
       <c r="E3" t="n">
-        <v>4283358</v>
+        <v>3047250</v>
       </c>
       <c r="F3" t="n">
-        <v>17663</v>
+        <v>17678</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17802</v>
+        <v>17922</v>
       </c>
       <c r="D4" t="n">
-        <v>2496</v>
+        <v>2735</v>
       </c>
       <c r="E4" t="n">
-        <v>605268</v>
+        <v>4283358</v>
       </c>
       <c r="F4" t="n">
-        <v>17638</v>
+        <v>17663</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17766</v>
+        <v>17802</v>
       </c>
       <c r="D5" t="n">
-        <v>2462</v>
+        <v>2496</v>
       </c>
       <c r="E5" t="n">
-        <v>6271398</v>
+        <v>605268</v>
       </c>
       <c r="F5" t="n">
-        <v>17636</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17549</v>
+        <v>17766</v>
       </c>
       <c r="D6" t="n">
-        <v>2109</v>
+        <v>2462</v>
       </c>
       <c r="E6" t="n">
-        <v>11845575</v>
+        <v>6271398</v>
       </c>
       <c r="F6" t="n">
-        <v>17614</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D7" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E7" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F7" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,41 +609,65 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D8" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E8" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F8" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F9" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>202202</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>17571</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>892</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>15673332</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="10"/>
+    <row r="11"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -656,7 +680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -683,37 +707,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/24</t>
+          <t>日期：2021/12/27</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.04</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/23</t>
+          <t>日期：2021/12/24</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.08</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -723,37 +747,37 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -763,17 +787,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -783,7 +807,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -793,17 +817,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -813,47 +837,47 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -863,250 +887,260 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B45" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1121,7 +1155,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1153,559 +1187,572 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月24日</t>
+          <t>110年12月27日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>86.02</v>
+        <v>111.66</v>
       </c>
       <c r="C2" t="n">
-        <v>-71.04000000000001</v>
+        <v>-24.36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月23日</t>
+          <t>110年12月24日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>180.23</v>
+        <v>86.02</v>
       </c>
       <c r="C3" t="n">
-        <v>-60.4</v>
+        <v>-71.04000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.7</v>
+        <v>180.23</v>
       </c>
       <c r="C4" t="n">
-        <v>19.86</v>
+        <v>-60.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>106.52</v>
+        <v>17.7</v>
       </c>
       <c r="C5" t="n">
-        <v>13.64</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-194.23</v>
+        <v>106.52</v>
       </c>
       <c r="C6" t="n">
-        <v>50.75</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C7" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>-25.74</v>
       </c>
       <c r="C8" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C9" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C10" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C11" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C12" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C13" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C14" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C15" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C16" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C17" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C18" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C19" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C20" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C21" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C22" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C23" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C24" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C25" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C26" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C29" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C30" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C31" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C32" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C33" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C34" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C35" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C36" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C37" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C38" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C39" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C40" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C41" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C42" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C43" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C44" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B45" t="n">
         <v>24.64</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C45" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1720,7 +1767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1747,420 +1794,430 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月24日</t>
+          <t>110年12月27日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17996.55</v>
+        <v>18053.58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月23日</t>
+          <t>110年12月24日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17931.41</v>
+        <v>17996.55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17835.4</v>
+        <v>17931.41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17748.15</v>
+        <v>17835.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17720.87</v>
+        <v>17748.15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B44" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2176,7 +2233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2270,1862 +2327,1908 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/24</t>
+          <t>2021/12/27</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46586</v>
+        <v>47184</v>
       </c>
       <c r="C2" t="n">
-        <v>53749</v>
+        <v>54192</v>
       </c>
       <c r="D2" t="n">
-        <v>650</v>
+        <v>598</v>
       </c>
       <c r="E2" t="n">
-        <v>1284</v>
+        <v>443</v>
       </c>
       <c r="F2" t="n">
-        <v>23007</v>
+        <v>25438</v>
       </c>
       <c r="G2" t="n">
-        <v>47663</v>
+        <v>48898</v>
       </c>
       <c r="H2" t="n">
-        <v>725</v>
+        <v>2431</v>
       </c>
       <c r="I2" t="n">
-        <v>1515</v>
+        <v>1235</v>
       </c>
       <c r="J2" t="n">
-        <v>-24656</v>
+        <v>-23460</v>
       </c>
       <c r="K2" t="n">
-        <v>-790</v>
+        <v>1196</v>
       </c>
       <c r="L2" t="n">
-        <v>-75</v>
+        <v>-1833</v>
       </c>
       <c r="M2" t="n">
-        <v>-231</v>
+        <v>-792</v>
       </c>
       <c r="N2" t="n">
-        <v>156</v>
+        <v>-1041</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/23</t>
+          <t>2021/12/24</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45936</v>
+        <v>46586</v>
       </c>
       <c r="C3" t="n">
-        <v>52465</v>
+        <v>53749</v>
       </c>
       <c r="D3" t="n">
-        <v>-387</v>
+        <v>650</v>
       </c>
       <c r="E3" t="n">
-        <v>-584</v>
+        <v>1284</v>
       </c>
       <c r="F3" t="n">
-        <v>22282</v>
+        <v>23007</v>
       </c>
       <c r="G3" t="n">
-        <v>46148</v>
+        <v>47663</v>
       </c>
       <c r="H3" t="n">
-        <v>1085</v>
+        <v>725</v>
       </c>
       <c r="I3" t="n">
-        <v>757</v>
+        <v>1515</v>
       </c>
       <c r="J3" t="n">
-        <v>-23866</v>
+        <v>-24656</v>
       </c>
       <c r="K3" t="n">
-        <v>328</v>
+        <v>-790</v>
       </c>
       <c r="L3" t="n">
-        <v>-1472</v>
+        <v>-75</v>
       </c>
       <c r="M3" t="n">
-        <v>-1341</v>
+        <v>-231</v>
       </c>
       <c r="N3" t="n">
-        <v>-131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/22</t>
+          <t>2021/12/23</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46323</v>
+        <v>45936</v>
       </c>
       <c r="C4" t="n">
-        <v>53049</v>
+        <v>52465</v>
       </c>
       <c r="D4" t="n">
-        <v>-1116</v>
+        <v>-387</v>
       </c>
       <c r="E4" t="n">
-        <v>-2269</v>
+        <v>-584</v>
       </c>
       <c r="F4" t="n">
-        <v>21197</v>
+        <v>22282</v>
       </c>
       <c r="G4" t="n">
-        <v>45391</v>
+        <v>46148</v>
       </c>
       <c r="H4" t="n">
-        <v>-909</v>
+        <v>1085</v>
       </c>
       <c r="I4" t="n">
-        <v>-2128</v>
+        <v>757</v>
       </c>
       <c r="J4" t="n">
-        <v>-24194</v>
+        <v>-23866</v>
       </c>
       <c r="K4" t="n">
-        <v>1219</v>
+        <v>328</v>
       </c>
       <c r="L4" t="n">
-        <v>-207</v>
+        <v>-1472</v>
       </c>
       <c r="M4" t="n">
-        <v>-141</v>
+        <v>-1341</v>
       </c>
       <c r="N4" t="n">
-        <v>-66</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/21</t>
+          <t>2021/12/22</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47439</v>
+        <v>46323</v>
       </c>
       <c r="C5" t="n">
-        <v>55318</v>
+        <v>53049</v>
       </c>
       <c r="D5" t="n">
-        <v>495</v>
+        <v>-1116</v>
       </c>
       <c r="E5" t="n">
-        <v>-78</v>
+        <v>-2269</v>
       </c>
       <c r="F5" t="n">
-        <v>22106</v>
+        <v>21197</v>
       </c>
       <c r="G5" t="n">
-        <v>47519</v>
+        <v>45391</v>
       </c>
       <c r="H5" t="n">
-        <v>517</v>
+        <v>-909</v>
       </c>
       <c r="I5" t="n">
-        <v>-712</v>
+        <v>-2128</v>
       </c>
       <c r="J5" t="n">
-        <v>-25413</v>
+        <v>-24194</v>
       </c>
       <c r="K5" t="n">
-        <v>1229</v>
+        <v>1219</v>
       </c>
       <c r="L5" t="n">
-        <v>-22</v>
+        <v>-207</v>
       </c>
       <c r="M5" t="n">
-        <v>634</v>
+        <v>-141</v>
       </c>
       <c r="N5" t="n">
-        <v>-656</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/20</t>
+          <t>2021/12/21</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46944</v>
+        <v>47439</v>
       </c>
       <c r="C6" t="n">
-        <v>55396</v>
+        <v>55318</v>
       </c>
       <c r="D6" t="n">
-        <v>1101</v>
+        <v>495</v>
       </c>
       <c r="E6" t="n">
-        <v>1087</v>
+        <v>-78</v>
       </c>
       <c r="F6" t="n">
-        <v>21589</v>
+        <v>22106</v>
       </c>
       <c r="G6" t="n">
-        <v>48231</v>
+        <v>47519</v>
       </c>
       <c r="H6" t="n">
-        <v>-426</v>
+        <v>517</v>
       </c>
       <c r="I6" t="n">
-        <v>802</v>
+        <v>-712</v>
       </c>
       <c r="J6" t="n">
-        <v>-26642</v>
+        <v>-25413</v>
       </c>
       <c r="K6" t="n">
-        <v>-1228</v>
+        <v>1229</v>
       </c>
       <c r="L6" t="n">
-        <v>1527</v>
+        <v>-22</v>
       </c>
       <c r="M6" t="n">
-        <v>285</v>
+        <v>634</v>
       </c>
       <c r="N6" t="n">
-        <v>1242</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C7" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D7" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E7" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F7" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G7" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H7" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I7" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J7" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K7" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L7" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M7" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N7" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C8" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D8" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E8" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F8" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G8" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H8" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I8" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J8" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K8" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L8" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M8" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N8" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C9" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D9" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E9" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F9" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G9" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H9" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I9" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J9" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K9" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L9" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M9" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N9" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C10" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D10" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E10" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F10" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G10" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H10" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I10" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J10" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K10" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L10" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M10" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N10" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C11" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D11" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E11" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F11" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G11" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H11" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I11" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J11" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K11" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L11" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M11" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N11" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C12" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D12" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E12" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F12" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G12" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H12" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I12" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J12" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K12" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L12" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M12" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N12" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C13" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D13" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E13" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F13" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G13" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H13" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I13" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J13" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K13" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L13" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M13" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N13" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C14" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D14" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E14" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F14" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G14" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H14" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I14" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J14" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K14" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L14" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M14" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N14" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C15" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D15" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E15" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F15" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G15" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H15" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I15" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J15" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K15" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L15" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M15" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N15" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C16" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D16" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E16" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F16" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G16" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H16" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I16" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J16" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K16" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L16" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M16" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N16" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C17" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D17" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E17" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F17" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G17" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H17" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I17" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J17" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K17" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L17" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M17" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N17" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C18" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D18" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E18" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F18" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G18" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H18" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I18" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J18" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K18" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L18" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M18" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N18" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C19" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D19" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E19" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F19" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G19" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H19" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I19" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J19" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K19" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L19" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M19" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N19" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C20" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D20" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E20" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F20" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G20" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H20" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I20" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J20" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K20" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L20" t="n">
-        <v>-337</v>
+        <v>-963</v>
       </c>
       <c r="M20" t="n">
-        <v>297</v>
+        <v>-1679</v>
       </c>
       <c r="N20" t="n">
-        <v>-634</v>
+        <v>716</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/29</t>
+          <t>2021/11/30</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>50934</v>
+        <v>49123</v>
       </c>
       <c r="C21" t="n">
-        <v>53204</v>
+        <v>55341</v>
       </c>
       <c r="D21" t="n">
-        <v>1297</v>
+        <v>-1811</v>
       </c>
       <c r="E21" t="n">
-        <v>2045</v>
+        <v>2137</v>
       </c>
       <c r="F21" t="n">
-        <v>27290</v>
+        <v>25816</v>
       </c>
       <c r="G21" t="n">
-        <v>45770</v>
+        <v>47610</v>
       </c>
       <c r="H21" t="n">
-        <v>1807</v>
+        <v>-1474</v>
       </c>
       <c r="I21" t="n">
-        <v>244</v>
+        <v>1840</v>
       </c>
       <c r="J21" t="n">
-        <v>-18480</v>
+        <v>-21794</v>
       </c>
       <c r="K21" t="n">
-        <v>1563</v>
+        <v>-3314</v>
       </c>
       <c r="L21" t="n">
-        <v>-510</v>
+        <v>-337</v>
       </c>
       <c r="M21" t="n">
-        <v>1801</v>
+        <v>297</v>
       </c>
       <c r="N21" t="n">
-        <v>-2311</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2021/11/26</t>
+          <t>2021/11/29</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>49637</v>
+        <v>50934</v>
       </c>
       <c r="C22" t="n">
-        <v>51159</v>
+        <v>53204</v>
       </c>
       <c r="D22" t="n">
-        <v>2800</v>
+        <v>1297</v>
       </c>
       <c r="E22" t="n">
-        <v>-1019</v>
+        <v>2045</v>
       </c>
       <c r="F22" t="n">
-        <v>25483</v>
+        <v>27290</v>
       </c>
       <c r="G22" t="n">
-        <v>45526</v>
+        <v>45770</v>
       </c>
       <c r="H22" t="n">
-        <v>-1108</v>
+        <v>1807</v>
       </c>
       <c r="I22" t="n">
-        <v>-30</v>
+        <v>244</v>
       </c>
       <c r="J22" t="n">
-        <v>-20043</v>
+        <v>-18480</v>
       </c>
       <c r="K22" t="n">
-        <v>-1078</v>
+        <v>1563</v>
       </c>
       <c r="L22" t="n">
-        <v>3908</v>
+        <v>-510</v>
       </c>
       <c r="M22" t="n">
-        <v>-989</v>
+        <v>1801</v>
       </c>
       <c r="N22" t="n">
-        <v>4897</v>
+        <v>-2311</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2021/11/24</t>
+          <t>2021/11/26</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>46837</v>
+        <v>49637</v>
       </c>
       <c r="C23" t="n">
-        <v>52178</v>
+        <v>51159</v>
       </c>
       <c r="D23" t="n">
-        <v>387</v>
+        <v>2800</v>
       </c>
       <c r="E23" t="n">
-        <v>578</v>
+        <v>-1019</v>
       </c>
       <c r="F23" t="n">
-        <v>26591</v>
+        <v>25483</v>
       </c>
       <c r="G23" t="n">
-        <v>45556</v>
+        <v>45526</v>
       </c>
       <c r="H23" t="n">
-        <v>1200</v>
+        <v>-1108</v>
       </c>
       <c r="I23" t="n">
-        <v>1458</v>
+        <v>-30</v>
       </c>
       <c r="J23" t="n">
-        <v>-18965</v>
+        <v>-20043</v>
       </c>
       <c r="K23" t="n">
-        <v>-258</v>
+        <v>-1078</v>
       </c>
       <c r="L23" t="n">
-        <v>-813</v>
+        <v>3908</v>
       </c>
       <c r="M23" t="n">
-        <v>-880</v>
+        <v>-989</v>
       </c>
       <c r="N23" t="n">
-        <v>67</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2021/11/23</t>
+          <t>2021/11/24</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46450</v>
+        <v>46837</v>
       </c>
       <c r="C24" t="n">
-        <v>51600</v>
+        <v>52178</v>
       </c>
       <c r="D24" t="n">
-        <v>31</v>
+        <v>387</v>
       </c>
       <c r="E24" t="n">
-        <v>284</v>
+        <v>578</v>
       </c>
       <c r="F24" t="n">
-        <v>25391</v>
+        <v>26591</v>
       </c>
       <c r="G24" t="n">
-        <v>44098</v>
+        <v>45556</v>
       </c>
       <c r="H24" t="n">
-        <v>-728</v>
+        <v>1200</v>
       </c>
       <c r="I24" t="n">
-        <v>-677</v>
+        <v>1458</v>
       </c>
       <c r="J24" t="n">
-        <v>-18707</v>
+        <v>-18965</v>
       </c>
       <c r="K24" t="n">
-        <v>-51</v>
+        <v>-258</v>
       </c>
       <c r="L24" t="n">
-        <v>759</v>
+        <v>-813</v>
       </c>
       <c r="M24" t="n">
-        <v>961</v>
+        <v>-880</v>
       </c>
       <c r="N24" t="n">
-        <v>-202</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2021/11/22</t>
+          <t>2021/11/23</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>46419</v>
+        <v>46450</v>
       </c>
       <c r="C25" t="n">
-        <v>51316</v>
+        <v>51600</v>
       </c>
       <c r="D25" t="n">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="E25" t="n">
-        <v>2092</v>
+        <v>284</v>
       </c>
       <c r="F25" t="n">
-        <v>26119</v>
+        <v>25391</v>
       </c>
       <c r="G25" t="n">
-        <v>44775</v>
+        <v>44098</v>
       </c>
       <c r="H25" t="n">
-        <v>3188</v>
+        <v>-728</v>
       </c>
       <c r="I25" t="n">
-        <v>2077</v>
+        <v>-677</v>
       </c>
       <c r="J25" t="n">
-        <v>-18656</v>
+        <v>-18707</v>
       </c>
       <c r="K25" t="n">
-        <v>1111</v>
+        <v>-51</v>
       </c>
       <c r="L25" t="n">
-        <v>-2156</v>
+        <v>759</v>
       </c>
       <c r="M25" t="n">
-        <v>15</v>
+        <v>961</v>
       </c>
       <c r="N25" t="n">
-        <v>-2171</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2021/11/19</t>
+          <t>2021/11/22</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>45387</v>
+        <v>46419</v>
       </c>
       <c r="C26" t="n">
-        <v>49224</v>
+        <v>51316</v>
       </c>
       <c r="D26" t="n">
-        <v>679</v>
+        <v>1032</v>
       </c>
       <c r="E26" t="n">
-        <v>723</v>
+        <v>2092</v>
       </c>
       <c r="F26" t="n">
-        <v>22931</v>
+        <v>26119</v>
       </c>
       <c r="G26" t="n">
-        <v>42698</v>
+        <v>44775</v>
       </c>
       <c r="H26" t="n">
-        <v>-1244</v>
+        <v>3188</v>
       </c>
       <c r="I26" t="n">
-        <v>583</v>
+        <v>2077</v>
       </c>
       <c r="J26" t="n">
-        <v>-19767</v>
+        <v>-18656</v>
       </c>
       <c r="K26" t="n">
-        <v>-1827</v>
+        <v>1111</v>
       </c>
       <c r="L26" t="n">
-        <v>1923</v>
+        <v>-2156</v>
       </c>
       <c r="M26" t="n">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="N26" t="n">
-        <v>1783</v>
+        <v>-2171</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2021/11/18</t>
+          <t>2021/11/19</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>44708</v>
+        <v>45387</v>
       </c>
       <c r="C27" t="n">
-        <v>48501</v>
+        <v>49224</v>
       </c>
       <c r="D27" t="n">
-        <v>74</v>
+        <v>679</v>
       </c>
       <c r="E27" t="n">
-        <v>2209</v>
+        <v>723</v>
       </c>
       <c r="F27" t="n">
-        <v>24175</v>
+        <v>22931</v>
       </c>
       <c r="G27" t="n">
-        <v>42115</v>
+        <v>42698</v>
       </c>
       <c r="H27" t="n">
-        <v>1245</v>
+        <v>-1244</v>
       </c>
       <c r="I27" t="n">
-        <v>3635</v>
+        <v>583</v>
       </c>
       <c r="J27" t="n">
-        <v>-17940</v>
+        <v>-19767</v>
       </c>
       <c r="K27" t="n">
-        <v>-2390</v>
+        <v>-1827</v>
       </c>
       <c r="L27" t="n">
-        <v>-1171</v>
+        <v>1923</v>
       </c>
       <c r="M27" t="n">
-        <v>-1426</v>
+        <v>140</v>
       </c>
       <c r="N27" t="n">
-        <v>255</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2021/11/17</t>
+          <t>2021/11/18</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>44634</v>
+        <v>44708</v>
       </c>
       <c r="C28" t="n">
-        <v>46292</v>
+        <v>48501</v>
       </c>
       <c r="D28" t="n">
-        <v>-4902</v>
+        <v>74</v>
       </c>
       <c r="E28" t="n">
-        <v>-2263</v>
+        <v>2209</v>
       </c>
       <c r="F28" t="n">
-        <v>22930</v>
+        <v>24175</v>
       </c>
       <c r="G28" t="n">
-        <v>38480</v>
+        <v>42115</v>
       </c>
       <c r="H28" t="n">
-        <v>-6746</v>
+        <v>1245</v>
       </c>
       <c r="I28" t="n">
-        <v>-6259</v>
+        <v>3635</v>
       </c>
       <c r="J28" t="n">
-        <v>-15550</v>
+        <v>-17940</v>
       </c>
       <c r="K28" t="n">
-        <v>-487</v>
+        <v>-2390</v>
       </c>
       <c r="L28" t="n">
-        <v>1844</v>
+        <v>-1171</v>
       </c>
       <c r="M28" t="n">
-        <v>3996</v>
+        <v>-1426</v>
       </c>
       <c r="N28" t="n">
-        <v>-2152</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2021/11/16</t>
+          <t>2021/11/17</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>49536</v>
+        <v>44634</v>
       </c>
       <c r="C29" t="n">
-        <v>48555</v>
+        <v>46292</v>
       </c>
       <c r="D29" t="n">
-        <v>296</v>
+        <v>-4902</v>
       </c>
       <c r="E29" t="n">
-        <v>-900</v>
+        <v>-2263</v>
       </c>
       <c r="F29" t="n">
-        <v>29676</v>
+        <v>22930</v>
       </c>
       <c r="G29" t="n">
-        <v>44739</v>
+        <v>38480</v>
       </c>
       <c r="H29" t="n">
-        <v>222</v>
+        <v>-6746</v>
       </c>
       <c r="I29" t="n">
-        <v>-294</v>
+        <v>-6259</v>
       </c>
       <c r="J29" t="n">
-        <v>-15063</v>
+        <v>-15550</v>
       </c>
       <c r="K29" t="n">
-        <v>516</v>
+        <v>-487</v>
       </c>
       <c r="L29" t="n">
-        <v>74</v>
+        <v>1844</v>
       </c>
       <c r="M29" t="n">
-        <v>-606</v>
+        <v>3996</v>
       </c>
       <c r="N29" t="n">
-        <v>680</v>
+        <v>-2152</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2021/11/15</t>
+          <t>2021/11/16</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>49240</v>
+        <v>49536</v>
       </c>
       <c r="C30" t="n">
-        <v>49455</v>
+        <v>48555</v>
       </c>
       <c r="D30" t="n">
-        <v>1205</v>
+        <v>296</v>
       </c>
       <c r="E30" t="n">
-        <v>494</v>
+        <v>-900</v>
       </c>
       <c r="F30" t="n">
-        <v>29454</v>
+        <v>29676</v>
       </c>
       <c r="G30" t="n">
-        <v>45033</v>
+        <v>44739</v>
       </c>
       <c r="H30" t="n">
-        <v>3755</v>
+        <v>222</v>
       </c>
       <c r="I30" t="n">
-        <v>2363</v>
+        <v>-294</v>
       </c>
       <c r="J30" t="n">
-        <v>-15579</v>
+        <v>-15063</v>
       </c>
       <c r="K30" t="n">
-        <v>1392</v>
+        <v>516</v>
       </c>
       <c r="L30" t="n">
-        <v>-2550</v>
+        <v>74</v>
       </c>
       <c r="M30" t="n">
-        <v>-1869</v>
+        <v>-606</v>
       </c>
       <c r="N30" t="n">
-        <v>-681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2021/11/12</t>
+          <t>2021/11/15</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>48035</v>
+        <v>49240</v>
       </c>
       <c r="C31" t="n">
-        <v>48961</v>
+        <v>49455</v>
       </c>
       <c r="D31" t="n">
-        <v>272</v>
+        <v>1205</v>
       </c>
       <c r="E31" t="n">
-        <v>1326</v>
+        <v>494</v>
       </c>
       <c r="F31" t="n">
-        <v>25699</v>
+        <v>29454</v>
       </c>
       <c r="G31" t="n">
-        <v>42670</v>
+        <v>45033</v>
       </c>
       <c r="H31" t="n">
-        <v>2351</v>
+        <v>3755</v>
       </c>
       <c r="I31" t="n">
-        <v>1332</v>
+        <v>2363</v>
       </c>
       <c r="J31" t="n">
-        <v>-16971</v>
+        <v>-15579</v>
       </c>
       <c r="K31" t="n">
-        <v>1019</v>
+        <v>1392</v>
       </c>
       <c r="L31" t="n">
-        <v>-2079</v>
+        <v>-2550</v>
       </c>
       <c r="M31" t="n">
-        <v>-6</v>
+        <v>-1869</v>
       </c>
       <c r="N31" t="n">
-        <v>-2073</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2021/11/11</t>
+          <t>2021/11/12</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>47763</v>
+        <v>48035</v>
       </c>
       <c r="C32" t="n">
-        <v>47635</v>
+        <v>48961</v>
       </c>
       <c r="D32" t="n">
-        <v>-1095</v>
+        <v>272</v>
       </c>
       <c r="E32" t="n">
-        <v>-135</v>
+        <v>1326</v>
       </c>
       <c r="F32" t="n">
-        <v>23348</v>
+        <v>25699</v>
       </c>
       <c r="G32" t="n">
-        <v>41338</v>
+        <v>42670</v>
       </c>
       <c r="H32" t="n">
-        <v>-409</v>
+        <v>2351</v>
       </c>
       <c r="I32" t="n">
-        <v>1068</v>
+        <v>1332</v>
       </c>
       <c r="J32" t="n">
-        <v>-17990</v>
+        <v>-16971</v>
       </c>
       <c r="K32" t="n">
-        <v>-1477</v>
+        <v>1019</v>
       </c>
       <c r="L32" t="n">
-        <v>-686</v>
+        <v>-2079</v>
       </c>
       <c r="M32" t="n">
-        <v>-1203</v>
+        <v>-6</v>
       </c>
       <c r="N32" t="n">
-        <v>517</v>
+        <v>-2073</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2021/11/10</t>
+          <t>2021/11/11</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>48858</v>
+        <v>47763</v>
       </c>
       <c r="C33" t="n">
-        <v>47770</v>
+        <v>47635</v>
       </c>
       <c r="D33" t="n">
-        <v>474</v>
+        <v>-1095</v>
       </c>
       <c r="E33" t="n">
-        <v>-737</v>
+        <v>-135</v>
       </c>
       <c r="F33" t="n">
-        <v>23757</v>
+        <v>23348</v>
       </c>
       <c r="G33" t="n">
-        <v>40270</v>
+        <v>41338</v>
       </c>
       <c r="H33" t="n">
-        <v>-2027</v>
+        <v>-409</v>
       </c>
       <c r="I33" t="n">
-        <v>904</v>
+        <v>1068</v>
       </c>
       <c r="J33" t="n">
-        <v>-16513</v>
+        <v>-17990</v>
       </c>
       <c r="K33" t="n">
-        <v>-2931</v>
+        <v>-1477</v>
       </c>
       <c r="L33" t="n">
-        <v>2501</v>
+        <v>-686</v>
       </c>
       <c r="M33" t="n">
-        <v>-1641</v>
+        <v>-1203</v>
       </c>
       <c r="N33" t="n">
-        <v>4142</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2021/11/09</t>
+          <t>2021/11/10</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>48384</v>
+        <v>48858</v>
       </c>
       <c r="C34" t="n">
-        <v>48507</v>
+        <v>47770</v>
       </c>
       <c r="D34" t="n">
-        <v>1314</v>
+        <v>474</v>
       </c>
       <c r="E34" t="n">
-        <v>-472</v>
-      </c>
-      <c r="F34" s="2" t="n">
-        <v>25784</v>
-      </c>
-      <c r="G34" s="2" t="n">
-        <v>39366</v>
+        <v>-737</v>
+      </c>
+      <c r="F34" t="n">
+        <v>23757</v>
+      </c>
+      <c r="G34" t="n">
+        <v>40270</v>
       </c>
       <c r="H34" t="n">
-        <v>896</v>
+        <v>-2027</v>
       </c>
       <c r="I34" t="n">
-        <v>-2977</v>
+        <v>904</v>
       </c>
       <c r="J34" t="n">
-        <v>-13582</v>
+        <v>-16513</v>
       </c>
       <c r="K34" t="n">
-        <v>3873</v>
+        <v>-2931</v>
       </c>
       <c r="L34" t="n">
-        <v>418</v>
+        <v>2501</v>
       </c>
       <c r="M34" t="n">
-        <v>2505</v>
+        <v>-1641</v>
       </c>
       <c r="N34" t="n">
-        <v>-2087</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2021/11/08</t>
+          <t>2021/11/09</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>47070</v>
+        <v>48384</v>
       </c>
       <c r="C35" t="n">
-        <v>48979</v>
+        <v>48507</v>
       </c>
       <c r="D35" t="n">
-        <v>1594</v>
+        <v>1314</v>
       </c>
       <c r="E35" t="n">
-        <v>-1512</v>
+        <v>-472</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>24888</v>
+        <v>25784</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>42343</v>
+        <v>39366</v>
       </c>
       <c r="H35" t="n">
-        <v>2148</v>
+        <v>896</v>
       </c>
       <c r="I35" t="n">
-        <v>-1793</v>
+        <v>-2977</v>
       </c>
       <c r="J35" t="n">
-        <v>-17455</v>
+        <v>-13582</v>
       </c>
       <c r="K35" t="n">
-        <v>3941</v>
+        <v>3873</v>
       </c>
       <c r="L35" t="n">
-        <v>-554</v>
+        <v>418</v>
       </c>
       <c r="M35" t="n">
-        <v>281</v>
+        <v>2505</v>
       </c>
       <c r="N35" t="n">
-        <v>-835</v>
+        <v>-2087</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2021/11/05</t>
+          <t>2021/11/08</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>45476</v>
+        <v>47070</v>
       </c>
       <c r="C36" t="n">
-        <v>50491</v>
+        <v>48979</v>
       </c>
       <c r="D36" t="n">
-        <v>-1055</v>
+        <v>1594</v>
       </c>
       <c r="E36" t="n">
-        <v>32</v>
+        <v>-1512</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>22740</v>
+        <v>24888</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>44136</v>
+        <v>42343</v>
       </c>
       <c r="H36" t="n">
-        <v>1964</v>
+        <v>2148</v>
       </c>
       <c r="I36" t="n">
-        <v>263</v>
+        <v>-1793</v>
       </c>
       <c r="J36" t="n">
-        <v>-21396</v>
+        <v>-17455</v>
       </c>
       <c r="K36" t="n">
-        <v>1701</v>
+        <v>3941</v>
       </c>
       <c r="L36" t="n">
-        <v>-3019</v>
+        <v>-554</v>
       </c>
       <c r="M36" t="n">
-        <v>-231</v>
+        <v>281</v>
       </c>
       <c r="N36" t="n">
-        <v>-2788</v>
+        <v>-835</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2021/11/04</t>
+          <t>2021/11/05</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>46531</v>
+        <v>45476</v>
       </c>
       <c r="C37" t="n">
-        <v>50459</v>
+        <v>50491</v>
       </c>
       <c r="D37" t="n">
-        <v>1264</v>
+        <v>-1055</v>
       </c>
       <c r="E37" t="n">
-        <v>749</v>
+        <v>32</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>20776</v>
+        <v>22740</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>43873</v>
+        <v>44136</v>
       </c>
       <c r="H37" t="n">
-        <v>-14</v>
+        <v>1964</v>
       </c>
       <c r="I37" t="n">
-        <v>1549</v>
+        <v>263</v>
       </c>
       <c r="J37" t="n">
-        <v>-23097</v>
+        <v>-21396</v>
       </c>
       <c r="K37" t="n">
-        <v>-1563</v>
+        <v>1701</v>
       </c>
       <c r="L37" t="n">
-        <v>1278</v>
+        <v>-3019</v>
       </c>
       <c r="M37" t="n">
-        <v>-800</v>
+        <v>-231</v>
       </c>
       <c r="N37" t="n">
-        <v>2078</v>
+        <v>-2788</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>2021/11/04</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>46531</v>
+      </c>
+      <c r="C38" t="n">
+        <v>50459</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1264</v>
+      </c>
+      <c r="E38" t="n">
+        <v>749</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>20776</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>43873</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-14</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1549</v>
+      </c>
+      <c r="J38" t="n">
+        <v>-23097</v>
+      </c>
+      <c r="K38" t="n">
+        <v>-1563</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1278</v>
+      </c>
+      <c r="M38" t="n">
+        <v>-800</v>
+      </c>
+      <c r="N38" t="n">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>2021/11/03</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B39" t="n">
         <v>45267</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C39" t="n">
         <v>49710</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D39" t="n">
         <v>-1089</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E39" t="n">
         <v>-2353</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F39" s="2" t="n">
         <v>20790</v>
       </c>
-      <c r="G38" s="2" t="n">
+      <c r="G39" s="2" t="n">
         <v>42324</v>
       </c>
-      <c r="H38" t="n">
+      <c r="H39" t="n">
         <v>-751</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I39" t="n">
         <v>-1660</v>
       </c>
-      <c r="J38" t="n">
+      <c r="J39" t="n">
         <v>-21534</v>
       </c>
-      <c r="K38" t="n">
+      <c r="K39" t="n">
         <v>909</v>
       </c>
-      <c r="L38" t="n">
+      <c r="L39" t="n">
         <v>-338</v>
       </c>
-      <c r="M38" t="n">
+      <c r="M39" t="n">
         <v>-693</v>
       </c>
-      <c r="N38" t="n">
+      <c r="N39" t="n">
         <v>355</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>2021/11/02</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>46356</v>
-      </c>
-      <c r="C39" t="n">
-        <v>52063</v>
-      </c>
-      <c r="D39" t="n">
-        <v>2402</v>
-      </c>
-      <c r="E39" t="n">
-        <v>793</v>
-      </c>
-      <c r="F39" s="2" t="n">
-        <v>21541</v>
-      </c>
-      <c r="G39" s="2" t="n">
-        <v>43984</v>
-      </c>
-      <c r="H39" t="n">
-        <v>1314</v>
-      </c>
-      <c r="I39" t="n">
-        <v>1673</v>
-      </c>
-      <c r="J39" t="n">
-        <v>-22443</v>
-      </c>
-      <c r="K39" t="n">
-        <v>-359</v>
-      </c>
-      <c r="L39" t="n">
-        <v>1088</v>
-      </c>
-      <c r="M39" t="n">
-        <v>-880</v>
-      </c>
-      <c r="N39" t="n">
-        <v>1968</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>2021/11/01</t>
+          <t>2021/11/02</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>43954</v>
+        <v>46356</v>
       </c>
       <c r="C40" t="n">
-        <v>51270</v>
+        <v>52063</v>
       </c>
       <c r="D40" t="n">
-        <v>-476</v>
+        <v>2402</v>
       </c>
       <c r="E40" t="n">
-        <v>-357</v>
+        <v>793</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>20227</v>
+        <v>21541</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>42311</v>
+        <v>43984</v>
       </c>
       <c r="H40" t="n">
-        <v>1165</v>
+        <v>1314</v>
       </c>
       <c r="I40" t="n">
-        <v>-593</v>
+        <v>1673</v>
       </c>
       <c r="J40" t="n">
-        <v>-22084</v>
+        <v>-22443</v>
       </c>
       <c r="K40" t="n">
-        <v>1758</v>
+        <v>-359</v>
       </c>
       <c r="L40" t="n">
-        <v>-1641</v>
+        <v>1088</v>
       </c>
       <c r="M40" t="n">
-        <v>236</v>
+        <v>-880</v>
       </c>
       <c r="N40" t="n">
-        <v>-1877</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>2021/10/29</t>
+          <t>2021/11/01</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>44430</v>
+        <v>43954</v>
       </c>
       <c r="C41" t="n">
-        <v>51627</v>
+        <v>51270</v>
       </c>
       <c r="D41" t="n">
-        <v>1916</v>
+        <v>-476</v>
       </c>
       <c r="E41" t="n">
-        <v>-174</v>
+        <v>-357</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>19062</v>
+        <v>20227</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>42904</v>
+        <v>42311</v>
       </c>
       <c r="H41" t="n">
-        <v>-871</v>
+        <v>1165</v>
       </c>
       <c r="I41" t="n">
-        <v>557</v>
+        <v>-593</v>
       </c>
       <c r="J41" t="n">
-        <v>-23842</v>
+        <v>-22084</v>
       </c>
       <c r="K41" t="n">
-        <v>-1428</v>
+        <v>1758</v>
       </c>
       <c r="L41" t="n">
-        <v>2787</v>
+        <v>-1641</v>
       </c>
       <c r="M41" t="n">
-        <v>-731</v>
+        <v>236</v>
       </c>
       <c r="N41" t="n">
-        <v>3518</v>
+        <v>-1877</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
+          <t>2021/10/29</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C42" t="n">
+        <v>51627</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1916</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-174</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>19062</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>42904</v>
+      </c>
+      <c r="H42" t="n">
+        <v>-871</v>
+      </c>
+      <c r="I42" t="n">
+        <v>557</v>
+      </c>
+      <c r="J42" t="n">
+        <v>-23842</v>
+      </c>
+      <c r="K42" t="n">
+        <v>-1428</v>
+      </c>
+      <c r="L42" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M42" t="n">
+        <v>-731</v>
+      </c>
+      <c r="N42" t="n">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
           <t>2021/10/28</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B43" t="n">
         <v>42514</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C43" t="n">
         <v>51801</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F43" s="2" t="n">
         <v>19933</v>
       </c>
-      <c r="G42" s="2" t="n">
+      <c r="G43" s="2" t="n">
         <v>42347</v>
       </c>
-      <c r="J42" t="n">
+      <c r="J43" t="n">
         <v>-22414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021/12/28 - everyday data updated
</commit_message>
<xml_diff>
--- a/everyday_ver2.xlsx
+++ b/everyday_ver2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/27</t>
+          <t>日期：2021/12/28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>18036</v>
+        <v>18175</v>
       </c>
       <c r="D2" t="n">
-        <v>3054</v>
+        <v>3307</v>
       </c>
       <c r="E2" t="n">
-        <v>2687364</v>
+        <v>4598275</v>
       </c>
       <c r="F2" t="n">
-        <v>17695</v>
+        <v>17732</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/24</t>
+          <t>日期：2021/12/27</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,22 +489,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17925</v>
+        <v>18036</v>
       </c>
       <c r="D3" t="n">
-        <v>2905</v>
+        <v>3054</v>
       </c>
       <c r="E3" t="n">
-        <v>3047250</v>
+        <v>2687364</v>
       </c>
       <c r="F3" t="n">
-        <v>17678</v>
+        <v>17695</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/23</t>
+          <t>日期：2021/12/24</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -513,22 +513,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17922</v>
+        <v>17925</v>
       </c>
       <c r="D4" t="n">
-        <v>2735</v>
+        <v>2905</v>
       </c>
       <c r="E4" t="n">
-        <v>4283358</v>
+        <v>3047250</v>
       </c>
       <c r="F4" t="n">
-        <v>17663</v>
+        <v>17678</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -537,22 +537,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17802</v>
+        <v>17922</v>
       </c>
       <c r="D5" t="n">
-        <v>2496</v>
+        <v>2735</v>
       </c>
       <c r="E5" t="n">
-        <v>605268</v>
+        <v>4283358</v>
       </c>
       <c r="F5" t="n">
-        <v>17638</v>
+        <v>17663</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,22 +561,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17766</v>
+        <v>17802</v>
       </c>
       <c r="D6" t="n">
-        <v>2462</v>
+        <v>2496</v>
       </c>
       <c r="E6" t="n">
-        <v>6271398</v>
+        <v>605268</v>
       </c>
       <c r="F6" t="n">
-        <v>17636</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17549</v>
+        <v>17766</v>
       </c>
       <c r="D7" t="n">
-        <v>2109</v>
+        <v>2462</v>
       </c>
       <c r="E7" t="n">
-        <v>11845575</v>
+        <v>6271398</v>
       </c>
       <c r="F7" t="n">
-        <v>17614</v>
+        <v>17636</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -609,22 +609,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17759</v>
+        <v>17549</v>
       </c>
       <c r="D8" t="n">
-        <v>1434</v>
+        <v>2109</v>
       </c>
       <c r="E8" t="n">
-        <v>5487531</v>
+        <v>11845575</v>
       </c>
       <c r="F8" t="n">
-        <v>17645</v>
+        <v>17614</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,41 +633,65 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17778</v>
+        <v>17759</v>
       </c>
       <c r="D9" t="n">
-        <v>1125</v>
+        <v>1434</v>
       </c>
       <c r="E9" t="n">
-        <v>4142274</v>
+        <v>5487531</v>
       </c>
       <c r="F9" t="n">
-        <v>17613</v>
+        <v>17645</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>日期：2021/12/16</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>202202</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>17778</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4142274</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17613</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>日期：2021/12/15</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B11" t="n">
         <v>202202</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C11" t="n">
         <v>17571</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>892</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E11" t="n">
         <v>15673332</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F11" t="n">
         <v>17571</v>
       </c>
     </row>
-    <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -680,7 +704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -707,47 +731,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>日期：2021/12/27</t>
+          <t>日期：2021/12/28</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>日期：2021/12/24</t>
+          <t>日期：2021/12/27</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.04</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>日期：2021/12/23</t>
+          <t>日期：2021/12/24</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>日期：2021/12/22</t>
+          <t>日期：2021/12/23</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>日期：2021/12/21</t>
+          <t>日期：2021/12/22</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -757,37 +781,37 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>日期：2021/12/20</t>
+          <t>日期：2021/12/21</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>日期：2021/12/17</t>
+          <t>日期：2021/12/20</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>日期：2021/12/16</t>
+          <t>日期：2021/12/17</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>日期：2021/12/15</t>
+          <t>日期：2021/12/16</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -797,17 +821,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>日期：2021/12/14</t>
+          <t>日期：2021/12/15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>日期：2021/12/13</t>
+          <t>日期：2021/12/14</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -817,7 +841,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>日期：2021/12/10</t>
+          <t>日期：2021/12/13</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -827,17 +851,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>日期：2021/12/09</t>
+          <t>日期：2021/12/10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>日期：2021/12/08</t>
+          <t>日期：2021/12/09</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -847,47 +871,47 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>日期：2021/12/07</t>
+          <t>日期：2021/12/08</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.09</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>日期：2021/12/06</t>
+          <t>日期：2021/12/07</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>日期：2021/12/03</t>
+          <t>日期：2021/12/06</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>日期：2021/12/02</t>
+          <t>日期：2021/12/03</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>日期：2021/12/01</t>
+          <t>日期：2021/12/02</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -897,250 +921,260 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>日期：2021/11/30</t>
+          <t>日期：2021/12/01</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>日期：2021/11/29</t>
+          <t>日期：2021/11/30</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>日期：2021/11/26</t>
+          <t>日期：2021/11/29</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>日期：2021/11/25</t>
+          <t>日期：2021/11/26</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>日期：2021/11/24</t>
+          <t>日期：2021/11/25</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>日期：2021/11/23</t>
+          <t>日期：2021/11/24</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>日期：2021/11/22</t>
+          <t>日期：2021/11/23</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>日期：2021/11/19</t>
+          <t>日期：2021/11/22</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>日期：2021/11/18</t>
+          <t>日期：2021/11/19</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>日期：2021/11/17</t>
+          <t>日期：2021/11/18</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>日期：2021/11/16</t>
+          <t>日期：2021/11/17</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.05</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>日期：2021/11/15</t>
+          <t>日期：2021/11/16</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>日期：2021/11/12</t>
+          <t>日期：2021/11/15</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>日期：2021/11/11</t>
+          <t>日期：2021/11/12</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>日期：2021/11/10</t>
+          <t>日期：2021/11/11</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>日期：2021/11/09</t>
+          <t>日期：2021/11/10</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>日期：2021/11/08</t>
+          <t>日期：2021/11/09</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.11</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>日期：2021/11/05</t>
+          <t>日期：2021/11/08</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.06</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>日期：2021/11/04</t>
+          <t>日期：2021/11/05</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.1</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>日期：2021/11/03</t>
+          <t>日期：2021/11/04</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>日期：2021/11/02</t>
+          <t>日期：2021/11/03</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>日期：2021/11/01</t>
+          <t>日期：2021/11/02</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>日期：2021/10/29</t>
+          <t>日期：2021/11/01</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>日期：2021/10/28</t>
+          <t>日期：2021/10/29</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>日期：2021/10/28</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>日期：2021/10/27</t>
         </is>
       </c>
-      <c r="B45" t="n">
+      <c r="B46" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -1155,7 +1189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -1187,572 +1221,585 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月27日</t>
+          <t>110年12月28日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>111.66</v>
+        <v>215.55</v>
       </c>
       <c r="C2" t="n">
-        <v>-24.36</v>
+        <v>-67.68000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月24日</t>
+          <t>110年12月27日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>86.02</v>
+        <v>111.66</v>
       </c>
       <c r="C3" t="n">
-        <v>-71.04000000000001</v>
+        <v>-24.36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月23日</t>
+          <t>110年12月24日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>180.23</v>
+        <v>86.02</v>
       </c>
       <c r="C4" t="n">
-        <v>-60.4</v>
+        <v>-71.04000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.7</v>
+        <v>180.23</v>
       </c>
       <c r="C5" t="n">
-        <v>19.86</v>
+        <v>-60.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>106.52</v>
+        <v>17.7</v>
       </c>
       <c r="C6" t="n">
-        <v>13.64</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-194.23</v>
+        <v>106.52</v>
       </c>
       <c r="C7" t="n">
-        <v>50.75</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-25.74</v>
+        <v>-194.23</v>
       </c>
       <c r="C8" t="n">
-        <v>52.59</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>-25.74</v>
       </c>
       <c r="C9" t="n">
-        <v>151.38</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-61.8</v>
+        <v>-25.74</v>
       </c>
       <c r="C10" t="n">
-        <v>122.53</v>
+        <v>151.38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-156</v>
+        <v>-61.8</v>
       </c>
       <c r="C11" t="n">
-        <v>-12.23</v>
+        <v>122.53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-90.95</v>
+        <v>-156</v>
       </c>
       <c r="C12" t="n">
-        <v>32.29</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-32.7</v>
+        <v>-90.95</v>
       </c>
       <c r="C13" t="n">
-        <v>-55.16</v>
+        <v>32.29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>61.47</v>
+        <v>-32.7</v>
       </c>
       <c r="C14" t="n">
-        <v>20.23</v>
+        <v>-55.16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>169.47</v>
+        <v>61.47</v>
       </c>
       <c r="C15" t="n">
-        <v>-133.97</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.62</v>
+        <v>169.47</v>
       </c>
       <c r="C16" t="n">
-        <v>106.09</v>
+        <v>-133.97</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-78.54000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="C17" t="n">
-        <v>69.61</v>
+        <v>106.09</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>75.7</v>
+        <v>-78.54000000000001</v>
       </c>
       <c r="C18" t="n">
-        <v>-103.44</v>
+        <v>69.61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>126.33</v>
+        <v>75.7</v>
       </c>
       <c r="C19" t="n">
-        <v>12.56</v>
+        <v>-103.44</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>84.34</v>
+        <v>126.33</v>
       </c>
       <c r="C20" t="n">
-        <v>73.89</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-166.84</v>
+        <v>84.34</v>
       </c>
       <c r="C21" t="n">
-        <v>266.51</v>
+        <v>73.89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>60.65</v>
+        <v>-166.84</v>
       </c>
       <c r="C22" t="n">
-        <v>-101.95</v>
+        <v>266.51</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-309.63</v>
+        <v>60.65</v>
       </c>
       <c r="C23" t="n">
-        <v>24.83</v>
+        <v>-101.95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-82.64</v>
+        <v>-309.63</v>
       </c>
       <c r="C24" t="n">
-        <v>94.31</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6.82</v>
+        <v>-82.64</v>
       </c>
       <c r="C25" t="n">
-        <v>-30.42</v>
+        <v>94.31</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-128.1</v>
+        <v>6.82</v>
       </c>
       <c r="C26" t="n">
-        <v>-9.32</v>
+        <v>-30.42</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>9.619999999999999</v>
+        <v>-128.1</v>
       </c>
       <c r="C27" t="n">
-        <v>-24.39</v>
+        <v>-9.32</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>80.34999999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>-103.41</v>
+        <v>-24.39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>101.7</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>-24.37</v>
+        <v>-103.41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-2.27</v>
+        <v>101.7</v>
       </c>
       <c r="C30" t="n">
-        <v>73.18000000000001</v>
+        <v>-24.37</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>76.95</v>
+        <v>-2.27</v>
       </c>
       <c r="C31" t="n">
-        <v>-18.29</v>
+        <v>73.18000000000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>54.36</v>
+        <v>76.95</v>
       </c>
       <c r="C32" t="n">
-        <v>61.98</v>
+        <v>-18.29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>79.23999999999999</v>
+        <v>54.36</v>
       </c>
       <c r="C33" t="n">
-        <v>-13.63</v>
+        <v>61.98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-70.66</v>
+        <v>79.23999999999999</v>
       </c>
       <c r="C34" t="n">
-        <v>-36.47</v>
+        <v>-13.63</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.29</v>
+        <v>-70.66</v>
       </c>
       <c r="C35" t="n">
-        <v>18</v>
+        <v>-36.47</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>196.05</v>
+        <v>0.29</v>
       </c>
       <c r="C36" t="n">
-        <v>-69.98999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>67.51000000000001</v>
+        <v>196.05</v>
       </c>
       <c r="C37" t="n">
-        <v>50.89</v>
+        <v>-69.98999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>265.52</v>
+        <v>67.51000000000001</v>
       </c>
       <c r="C38" t="n">
-        <v>-47.48</v>
+        <v>50.89</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-74.23999999999999</v>
+        <v>265.52</v>
       </c>
       <c r="C39" t="n">
-        <v>30.94</v>
+        <v>-47.48</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>38.92</v>
+        <v>-74.23999999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>17.27</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>19.71</v>
+        <v>38.92</v>
       </c>
       <c r="C41" t="n">
-        <v>-21.98</v>
+        <v>17.27</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-31.96</v>
+        <v>19.71</v>
       </c>
       <c r="C42" t="n">
-        <v>112.79</v>
+        <v>-21.98</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-115.21</v>
+        <v>-31.96</v>
       </c>
       <c r="C43" t="n">
-        <v>60.99</v>
+        <v>112.79</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>110年10月28日</t>
+          <t>110年10月29日</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-73.59</v>
+        <v>-115.21</v>
       </c>
       <c r="C44" t="n">
-        <v>40.67</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>110年10月28日</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>-73.59</v>
+      </c>
+      <c r="C45" t="n">
+        <v>40.67</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>110年10月27日</t>
         </is>
       </c>
-      <c r="B45" t="n">
+      <c r="B46" t="n">
         <v>24.64</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C46" t="n">
         <v>15.57</v>
       </c>
     </row>
@@ -1767,7 +1814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1794,430 +1841,440 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>110年12月27日</t>
+          <t>110年12月28日</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18053.58</v>
+        <v>18164.34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110年12月24日</t>
+          <t>110年12月27日</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17996.55</v>
+        <v>18053.58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>110年12月23日</t>
+          <t>110年12月24日</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17931.41</v>
+        <v>17996.55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>110年12月22日</t>
+          <t>110年12月23日</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17835.4</v>
+        <v>17931.41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>110年12月21日</t>
+          <t>110年12月22日</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17748.15</v>
+        <v>17835.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110年12月20日</t>
+          <t>110年12月21日</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17720.87</v>
+        <v>17748.15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>110年12月17日</t>
+          <t>110年12月20日</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17782.21</v>
+        <v>17720.87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>110年12月16日</t>
+          <t>110年12月17日</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17765.63</v>
+        <v>17782.21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110年12月15日</t>
+          <t>110年12月16日</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17625.43</v>
+        <v>17765.63</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110年12月14日</t>
+          <t>110年12月15日</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17635.97</v>
+        <v>17625.43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110年12月13日</t>
+          <t>110年12月14日</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17864.87</v>
+        <v>17635.97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110年12月10日</t>
+          <t>110年12月13日</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17832.17</v>
+        <v>17864.87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110年12月09日</t>
+          <t>110年12月10日</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17876.02</v>
+        <v>17832.17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110年12月08日</t>
+          <t>110年12月09日</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17913.87</v>
+        <v>17876.02</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>110年12月07日</t>
+          <t>110年12月08日</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17697.98</v>
+        <v>17913.87</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110年12月06日</t>
+          <t>110年12月07日</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17675.07</v>
+        <v>17697.98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110年12月03日</t>
+          <t>110年12月06日</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17728.92</v>
+        <v>17675.07</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110年12月02日</t>
+          <t>110年12月03日</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17670.86</v>
+        <v>17728.92</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110年12月01日</t>
+          <t>110年12月02日</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17487.19</v>
+        <v>17670.86</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>110年11月30日</t>
+          <t>110年12月01日</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17473.4</v>
+        <v>17487.19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>110年11月29日</t>
+          <t>110年11月30日</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17305.94</v>
+        <v>17473.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110年11月26日</t>
+          <t>110年11月29日</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>17451.48</v>
+        <v>17305.94</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>110年11月25日</t>
+          <t>110年11月26日</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17659.83</v>
+        <v>17451.48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>110年11月24日</t>
+          <t>110年11月25日</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>17656.76</v>
+        <v>17659.83</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110年11月23日</t>
+          <t>110年11月24日</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17711.53</v>
+        <v>17656.76</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110年11月22日</t>
+          <t>110年11月23日</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17822.48</v>
+        <v>17711.53</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110年11月19日</t>
+          <t>110年11月22日</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>17869.31</v>
+        <v>17822.48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110年11月18日</t>
+          <t>110年11月19日</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17804.99</v>
+        <v>17869.31</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>110年11月17日</t>
+          <t>110年11月18日</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>17728.81</v>
+        <v>17804.99</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110年11月16日</t>
+          <t>110年11月17日</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>17672.38</v>
+        <v>17728.81</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110年11月15日</t>
+          <t>110年11月16日</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>17639.87</v>
+        <v>17672.38</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>110年11月12日</t>
+          <t>110年11月15日</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17531.84</v>
+        <v>17639.87</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>110年11月11日</t>
+          <t>110年11月12日</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17464.79</v>
+        <v>17531.84</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110年11月10日</t>
+          <t>110年11月11日</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17541.18</v>
+        <v>17464.79</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>110年11月09日</t>
+          <t>110年11月10日</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17542.65</v>
+        <v>17541.18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110年11月08日</t>
+          <t>110年11月09日</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>17348.15</v>
+        <v>17542.65</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110年11月05日</t>
+          <t>110年11月08日</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>17202.29</v>
+        <v>17348.15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>110年11月04日</t>
+          <t>110年11月05日</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>17156.65</v>
+        <v>17202.29</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>110年11月03日</t>
+          <t>110年11月04日</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>17116.74</v>
+        <v>17156.65</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>110年11月02日</t>
+          <t>110年11月03日</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>17133.93</v>
+        <v>17116.74</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>110年11月01日</t>
+          <t>110年11月02日</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>17080.39</v>
+        <v>17133.93</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>110年10月29日</t>
+          <t>110年11月01日</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>16983.35</v>
+        <v>17080.39</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>110年10月29日</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>16983.35</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>110年10月28日</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B45" t="n">
         <v>17054.47</v>
       </c>
     </row>
@@ -2233,7 +2290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2327,1908 +2384,1954 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/12/27</t>
+          <t>2021/12/28</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47184</v>
+        <v>47833</v>
       </c>
       <c r="C2" t="n">
-        <v>54192</v>
+        <v>55260</v>
       </c>
       <c r="D2" t="n">
-        <v>598</v>
+        <v>649</v>
       </c>
       <c r="E2" t="n">
-        <v>443</v>
+        <v>1068</v>
       </c>
       <c r="F2" t="n">
-        <v>25438</v>
+        <v>27786</v>
       </c>
       <c r="G2" t="n">
-        <v>48898</v>
+        <v>50379</v>
       </c>
       <c r="H2" t="n">
-        <v>2431</v>
+        <v>2348</v>
       </c>
       <c r="I2" t="n">
-        <v>1235</v>
+        <v>1481</v>
       </c>
       <c r="J2" t="n">
-        <v>-23460</v>
+        <v>-22593</v>
       </c>
       <c r="K2" t="n">
-        <v>1196</v>
+        <v>867</v>
       </c>
       <c r="L2" t="n">
-        <v>-1833</v>
+        <v>-1699</v>
       </c>
       <c r="M2" t="n">
-        <v>-792</v>
+        <v>-413</v>
       </c>
       <c r="N2" t="n">
-        <v>-1041</v>
+        <v>-1286</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/12/24</t>
+          <t>2021/12/27</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46586</v>
+        <v>47184</v>
       </c>
       <c r="C3" t="n">
-        <v>53749</v>
+        <v>54192</v>
       </c>
       <c r="D3" t="n">
-        <v>650</v>
+        <v>598</v>
       </c>
       <c r="E3" t="n">
-        <v>1284</v>
+        <v>443</v>
       </c>
       <c r="F3" t="n">
-        <v>23007</v>
+        <v>25438</v>
       </c>
       <c r="G3" t="n">
-        <v>47663</v>
+        <v>48898</v>
       </c>
       <c r="H3" t="n">
-        <v>725</v>
+        <v>2431</v>
       </c>
       <c r="I3" t="n">
-        <v>1515</v>
+        <v>1235</v>
       </c>
       <c r="J3" t="n">
-        <v>-24656</v>
+        <v>-23460</v>
       </c>
       <c r="K3" t="n">
-        <v>-790</v>
+        <v>1196</v>
       </c>
       <c r="L3" t="n">
-        <v>-75</v>
+        <v>-1833</v>
       </c>
       <c r="M3" t="n">
-        <v>-231</v>
+        <v>-792</v>
       </c>
       <c r="N3" t="n">
-        <v>156</v>
+        <v>-1041</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/12/23</t>
+          <t>2021/12/24</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45936</v>
+        <v>46586</v>
       </c>
       <c r="C4" t="n">
-        <v>52465</v>
+        <v>53749</v>
       </c>
       <c r="D4" t="n">
-        <v>-387</v>
+        <v>650</v>
       </c>
       <c r="E4" t="n">
-        <v>-584</v>
+        <v>1284</v>
       </c>
       <c r="F4" t="n">
-        <v>22282</v>
+        <v>23007</v>
       </c>
       <c r="G4" t="n">
-        <v>46148</v>
+        <v>47663</v>
       </c>
       <c r="H4" t="n">
-        <v>1085</v>
+        <v>725</v>
       </c>
       <c r="I4" t="n">
-        <v>757</v>
+        <v>1515</v>
       </c>
       <c r="J4" t="n">
-        <v>-23866</v>
+        <v>-24656</v>
       </c>
       <c r="K4" t="n">
-        <v>328</v>
+        <v>-790</v>
       </c>
       <c r="L4" t="n">
-        <v>-1472</v>
+        <v>-75</v>
       </c>
       <c r="M4" t="n">
-        <v>-1341</v>
+        <v>-231</v>
       </c>
       <c r="N4" t="n">
-        <v>-131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/12/22</t>
+          <t>2021/12/23</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>46323</v>
+        <v>45936</v>
       </c>
       <c r="C5" t="n">
-        <v>53049</v>
+        <v>52465</v>
       </c>
       <c r="D5" t="n">
-        <v>-1116</v>
+        <v>-387</v>
       </c>
       <c r="E5" t="n">
-        <v>-2269</v>
+        <v>-584</v>
       </c>
       <c r="F5" t="n">
-        <v>21197</v>
+        <v>22282</v>
       </c>
       <c r="G5" t="n">
-        <v>45391</v>
+        <v>46148</v>
       </c>
       <c r="H5" t="n">
-        <v>-909</v>
+        <v>1085</v>
       </c>
       <c r="I5" t="n">
-        <v>-2128</v>
+        <v>757</v>
       </c>
       <c r="J5" t="n">
-        <v>-24194</v>
+        <v>-23866</v>
       </c>
       <c r="K5" t="n">
-        <v>1219</v>
+        <v>328</v>
       </c>
       <c r="L5" t="n">
-        <v>-207</v>
+        <v>-1472</v>
       </c>
       <c r="M5" t="n">
-        <v>-141</v>
+        <v>-1341</v>
       </c>
       <c r="N5" t="n">
-        <v>-66</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/12/21</t>
+          <t>2021/12/22</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>47439</v>
+        <v>46323</v>
       </c>
       <c r="C6" t="n">
-        <v>55318</v>
+        <v>53049</v>
       </c>
       <c r="D6" t="n">
-        <v>495</v>
+        <v>-1116</v>
       </c>
       <c r="E6" t="n">
-        <v>-78</v>
+        <v>-2269</v>
       </c>
       <c r="F6" t="n">
-        <v>22106</v>
+        <v>21197</v>
       </c>
       <c r="G6" t="n">
-        <v>47519</v>
+        <v>45391</v>
       </c>
       <c r="H6" t="n">
-        <v>517</v>
+        <v>-909</v>
       </c>
       <c r="I6" t="n">
-        <v>-712</v>
+        <v>-2128</v>
       </c>
       <c r="J6" t="n">
-        <v>-25413</v>
+        <v>-24194</v>
       </c>
       <c r="K6" t="n">
-        <v>1229</v>
+        <v>1219</v>
       </c>
       <c r="L6" t="n">
-        <v>-22</v>
+        <v>-207</v>
       </c>
       <c r="M6" t="n">
-        <v>634</v>
+        <v>-141</v>
       </c>
       <c r="N6" t="n">
-        <v>-656</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/12/20</t>
+          <t>2021/12/21</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46944</v>
+        <v>47439</v>
       </c>
       <c r="C7" t="n">
-        <v>55396</v>
+        <v>55318</v>
       </c>
       <c r="D7" t="n">
-        <v>1101</v>
+        <v>495</v>
       </c>
       <c r="E7" t="n">
-        <v>1087</v>
+        <v>-78</v>
       </c>
       <c r="F7" t="n">
-        <v>21589</v>
+        <v>22106</v>
       </c>
       <c r="G7" t="n">
-        <v>48231</v>
+        <v>47519</v>
       </c>
       <c r="H7" t="n">
-        <v>-426</v>
+        <v>517</v>
       </c>
       <c r="I7" t="n">
-        <v>802</v>
+        <v>-712</v>
       </c>
       <c r="J7" t="n">
-        <v>-26642</v>
+        <v>-25413</v>
       </c>
       <c r="K7" t="n">
-        <v>-1228</v>
+        <v>1229</v>
       </c>
       <c r="L7" t="n">
-        <v>1527</v>
+        <v>-22</v>
       </c>
       <c r="M7" t="n">
-        <v>285</v>
+        <v>634</v>
       </c>
       <c r="N7" t="n">
-        <v>1242</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/12/17</t>
+          <t>2021/12/20</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>45843</v>
+        <v>46944</v>
       </c>
       <c r="C8" t="n">
-        <v>54309</v>
+        <v>55396</v>
       </c>
       <c r="D8" t="n">
-        <v>-630</v>
+        <v>1101</v>
       </c>
       <c r="E8" t="n">
-        <v>-27</v>
+        <v>1087</v>
       </c>
       <c r="F8" t="n">
-        <v>22015</v>
+        <v>21589</v>
       </c>
       <c r="G8" t="n">
-        <v>47429</v>
+        <v>48231</v>
       </c>
       <c r="H8" t="n">
-        <v>812</v>
+        <v>-426</v>
       </c>
       <c r="I8" t="n">
-        <v>-304</v>
+        <v>802</v>
       </c>
       <c r="J8" t="n">
-        <v>-25414</v>
+        <v>-26642</v>
       </c>
       <c r="K8" t="n">
-        <v>1116</v>
+        <v>-1228</v>
       </c>
       <c r="L8" t="n">
-        <v>-1442</v>
+        <v>1527</v>
       </c>
       <c r="M8" t="n">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="N8" t="n">
-        <v>-1719</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/12/16</t>
+          <t>2021/12/17</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46473</v>
+        <v>45843</v>
       </c>
       <c r="C9" t="n">
-        <v>54336</v>
+        <v>54309</v>
       </c>
       <c r="D9" t="n">
-        <v>-51</v>
+        <v>-630</v>
       </c>
       <c r="E9" t="n">
-        <v>381</v>
+        <v>-27</v>
       </c>
       <c r="F9" t="n">
-        <v>21203</v>
+        <v>22015</v>
       </c>
       <c r="G9" t="n">
-        <v>47733</v>
+        <v>47429</v>
       </c>
       <c r="H9" t="n">
-        <v>313</v>
+        <v>812</v>
       </c>
       <c r="I9" t="n">
-        <v>1055</v>
+        <v>-304</v>
       </c>
       <c r="J9" t="n">
-        <v>-26530</v>
+        <v>-25414</v>
       </c>
       <c r="K9" t="n">
-        <v>-742</v>
+        <v>1116</v>
       </c>
       <c r="L9" t="n">
-        <v>-364</v>
+        <v>-1442</v>
       </c>
       <c r="M9" t="n">
-        <v>-674</v>
+        <v>277</v>
       </c>
       <c r="N9" t="n">
-        <v>310</v>
+        <v>-1719</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/12/15</t>
+          <t>2021/12/16</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46524</v>
+        <v>46473</v>
       </c>
       <c r="C10" t="n">
-        <v>53955</v>
+        <v>54336</v>
       </c>
       <c r="D10" t="n">
-        <v>-5237</v>
+        <v>-51</v>
       </c>
       <c r="E10" t="n">
-        <v>-5329</v>
+        <v>381</v>
       </c>
       <c r="F10" t="n">
-        <v>20890</v>
+        <v>21203</v>
       </c>
       <c r="G10" t="n">
-        <v>46678</v>
+        <v>47733</v>
       </c>
       <c r="H10" t="n">
-        <v>-5128</v>
+        <v>313</v>
       </c>
       <c r="I10" t="n">
-        <v>-5868</v>
+        <v>1055</v>
       </c>
       <c r="J10" t="n">
-        <v>-25788</v>
+        <v>-26530</v>
       </c>
       <c r="K10" t="n">
-        <v>740</v>
+        <v>-742</v>
       </c>
       <c r="L10" t="n">
-        <v>-109</v>
+        <v>-364</v>
       </c>
       <c r="M10" t="n">
-        <v>539</v>
+        <v>-674</v>
       </c>
       <c r="N10" t="n">
-        <v>-648</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/12/14</t>
+          <t>2021/12/15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>51761</v>
+        <v>46524</v>
       </c>
       <c r="C11" t="n">
-        <v>59284</v>
+        <v>53955</v>
       </c>
       <c r="D11" t="n">
-        <v>800</v>
+        <v>-5237</v>
       </c>
       <c r="E11" t="n">
-        <v>1430</v>
+        <v>-5329</v>
       </c>
       <c r="F11" t="n">
-        <v>26018</v>
+        <v>20890</v>
       </c>
       <c r="G11" t="n">
-        <v>52546</v>
+        <v>46678</v>
       </c>
       <c r="H11" t="n">
-        <v>-995</v>
+        <v>-5128</v>
       </c>
       <c r="I11" t="n">
-        <v>-217</v>
+        <v>-5868</v>
       </c>
       <c r="J11" t="n">
-        <v>-26528</v>
+        <v>-25788</v>
       </c>
       <c r="K11" t="n">
-        <v>-778</v>
+        <v>740</v>
       </c>
       <c r="L11" t="n">
-        <v>1795</v>
+        <v>-109</v>
       </c>
       <c r="M11" t="n">
-        <v>1647</v>
+        <v>539</v>
       </c>
       <c r="N11" t="n">
-        <v>148</v>
+        <v>-648</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/12/13</t>
+          <t>2021/12/14</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50961</v>
+        <v>51761</v>
       </c>
       <c r="C12" t="n">
-        <v>57854</v>
+        <v>59284</v>
       </c>
       <c r="D12" t="n">
-        <v>2566</v>
+        <v>800</v>
       </c>
       <c r="E12" t="n">
-        <v>713</v>
+        <v>1430</v>
       </c>
       <c r="F12" t="n">
-        <v>27013</v>
+        <v>26018</v>
       </c>
       <c r="G12" t="n">
-        <v>52763</v>
+        <v>52546</v>
       </c>
       <c r="H12" t="n">
-        <v>2505</v>
+        <v>-995</v>
       </c>
       <c r="I12" t="n">
-        <v>1839</v>
+        <v>-217</v>
       </c>
       <c r="J12" t="n">
-        <v>-25750</v>
+        <v>-26528</v>
       </c>
       <c r="K12" t="n">
-        <v>666</v>
+        <v>-778</v>
       </c>
       <c r="L12" t="n">
-        <v>61</v>
+        <v>1795</v>
       </c>
       <c r="M12" t="n">
-        <v>-1126</v>
+        <v>1647</v>
       </c>
       <c r="N12" t="n">
-        <v>1187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2021/12/10</t>
+          <t>2021/12/13</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48395</v>
+        <v>50961</v>
       </c>
       <c r="C13" t="n">
-        <v>57141</v>
+        <v>57854</v>
       </c>
       <c r="D13" t="n">
-        <v>944</v>
+        <v>2566</v>
       </c>
       <c r="E13" t="n">
-        <v>879</v>
+        <v>713</v>
       </c>
       <c r="F13" t="n">
-        <v>24508</v>
+        <v>27013</v>
       </c>
       <c r="G13" t="n">
-        <v>50924</v>
+        <v>52763</v>
       </c>
       <c r="H13" t="n">
-        <v>-1296</v>
+        <v>2505</v>
       </c>
       <c r="I13" t="n">
-        <v>520</v>
+        <v>1839</v>
       </c>
       <c r="J13" t="n">
-        <v>-26416</v>
+        <v>-25750</v>
       </c>
       <c r="K13" t="n">
-        <v>-1816</v>
+        <v>666</v>
       </c>
       <c r="L13" t="n">
-        <v>2240</v>
+        <v>61</v>
       </c>
       <c r="M13" t="n">
-        <v>359</v>
+        <v>-1126</v>
       </c>
       <c r="N13" t="n">
-        <v>1881</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021/12/09</t>
+          <t>2021/12/10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>47451</v>
+        <v>48395</v>
       </c>
       <c r="C14" t="n">
-        <v>56262</v>
+        <v>57141</v>
       </c>
       <c r="D14" t="n">
-        <v>-545</v>
+        <v>944</v>
       </c>
       <c r="E14" t="n">
-        <v>789</v>
+        <v>879</v>
       </c>
       <c r="F14" t="n">
-        <v>25804</v>
+        <v>24508</v>
       </c>
       <c r="G14" t="n">
-        <v>50404</v>
+        <v>50924</v>
       </c>
       <c r="H14" t="n">
-        <v>803</v>
+        <v>-1296</v>
       </c>
       <c r="I14" t="n">
-        <v>-11</v>
+        <v>520</v>
       </c>
       <c r="J14" t="n">
-        <v>-24600</v>
+        <v>-26416</v>
       </c>
       <c r="K14" t="n">
-        <v>814</v>
+        <v>-1816</v>
       </c>
       <c r="L14" t="n">
-        <v>-1348</v>
+        <v>2240</v>
       </c>
       <c r="M14" t="n">
-        <v>800</v>
+        <v>359</v>
       </c>
       <c r="N14" t="n">
-        <v>-2148</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2021/12/08</t>
+          <t>2021/12/09</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>47996</v>
+        <v>47451</v>
       </c>
       <c r="C15" t="n">
-        <v>55473</v>
+        <v>56262</v>
       </c>
       <c r="D15" t="n">
-        <v>-2741</v>
+        <v>-545</v>
       </c>
       <c r="E15" t="n">
-        <v>-3078</v>
+        <v>789</v>
       </c>
       <c r="F15" t="n">
-        <v>25001</v>
+        <v>25804</v>
       </c>
       <c r="G15" t="n">
-        <v>50415</v>
+        <v>50404</v>
       </c>
       <c r="H15" t="n">
-        <v>-349</v>
+        <v>803</v>
       </c>
       <c r="I15" t="n">
-        <v>-1153</v>
+        <v>-11</v>
       </c>
       <c r="J15" t="n">
-        <v>-25414</v>
+        <v>-24600</v>
       </c>
       <c r="K15" t="n">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="L15" t="n">
-        <v>-2392</v>
+        <v>-1348</v>
       </c>
       <c r="M15" t="n">
-        <v>-1925</v>
+        <v>800</v>
       </c>
       <c r="N15" t="n">
-        <v>-467</v>
+        <v>-2148</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2021/12/07</t>
+          <t>2021/12/08</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>50737</v>
+        <v>47996</v>
       </c>
       <c r="C16" t="n">
-        <v>58551</v>
+        <v>55473</v>
       </c>
       <c r="D16" t="n">
-        <v>181</v>
+        <v>-2741</v>
       </c>
       <c r="E16" t="n">
-        <v>1400</v>
+        <v>-3078</v>
       </c>
       <c r="F16" t="n">
-        <v>25350</v>
+        <v>25001</v>
       </c>
       <c r="G16" t="n">
-        <v>51568</v>
+        <v>50415</v>
       </c>
       <c r="H16" t="n">
-        <v>-1527</v>
+        <v>-349</v>
       </c>
       <c r="I16" t="n">
-        <v>661</v>
+        <v>-1153</v>
       </c>
       <c r="J16" t="n">
-        <v>-26218</v>
+        <v>-25414</v>
       </c>
       <c r="K16" t="n">
-        <v>-2188</v>
+        <v>804</v>
       </c>
       <c r="L16" t="n">
-        <v>1708</v>
+        <v>-2392</v>
       </c>
       <c r="M16" t="n">
-        <v>739</v>
+        <v>-1925</v>
       </c>
       <c r="N16" t="n">
-        <v>969</v>
+        <v>-467</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2021/12/06</t>
+          <t>2021/12/07</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>50556</v>
+        <v>50737</v>
       </c>
       <c r="C17" t="n">
-        <v>57151</v>
+        <v>58551</v>
       </c>
       <c r="D17" t="n">
-        <v>1269</v>
+        <v>181</v>
       </c>
       <c r="E17" t="n">
-        <v>3572</v>
+        <v>1400</v>
       </c>
       <c r="F17" t="n">
-        <v>26877</v>
+        <v>25350</v>
       </c>
       <c r="G17" t="n">
-        <v>50907</v>
+        <v>51568</v>
       </c>
       <c r="H17" t="n">
-        <v>1219</v>
+        <v>-1527</v>
       </c>
       <c r="I17" t="n">
-        <v>3082</v>
+        <v>661</v>
       </c>
       <c r="J17" t="n">
-        <v>-24030</v>
+        <v>-26218</v>
       </c>
       <c r="K17" t="n">
-        <v>-1863</v>
+        <v>-2188</v>
       </c>
       <c r="L17" t="n">
-        <v>50</v>
+        <v>1708</v>
       </c>
       <c r="M17" t="n">
-        <v>490</v>
+        <v>739</v>
       </c>
       <c r="N17" t="n">
-        <v>-440</v>
+        <v>969</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2021/12/03</t>
+          <t>2021/12/06</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49287</v>
+        <v>50556</v>
       </c>
       <c r="C18" t="n">
-        <v>53579</v>
+        <v>57151</v>
       </c>
       <c r="D18" t="n">
-        <v>500</v>
+        <v>1269</v>
       </c>
       <c r="E18" t="n">
-        <v>899</v>
+        <v>3572</v>
       </c>
       <c r="F18" t="n">
-        <v>25658</v>
+        <v>26877</v>
       </c>
       <c r="G18" t="n">
-        <v>47825</v>
+        <v>50907</v>
       </c>
       <c r="H18" t="n">
-        <v>-96</v>
+        <v>1219</v>
       </c>
       <c r="I18" t="n">
-        <v>213</v>
+        <v>3082</v>
       </c>
       <c r="J18" t="n">
-        <v>-22167</v>
+        <v>-24030</v>
       </c>
       <c r="K18" t="n">
-        <v>-309</v>
+        <v>-1863</v>
       </c>
       <c r="L18" t="n">
-        <v>596</v>
+        <v>50</v>
       </c>
       <c r="M18" t="n">
-        <v>686</v>
+        <v>490</v>
       </c>
       <c r="N18" t="n">
-        <v>-90</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2021/12/02</t>
+          <t>2021/12/03</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>48787</v>
+        <v>49287</v>
       </c>
       <c r="C19" t="n">
-        <v>52680</v>
+        <v>53579</v>
       </c>
       <c r="D19" t="n">
-        <v>-624</v>
+        <v>500</v>
       </c>
       <c r="E19" t="n">
-        <v>-2013</v>
+        <v>899</v>
       </c>
       <c r="F19" t="n">
-        <v>25754</v>
+        <v>25658</v>
       </c>
       <c r="G19" t="n">
-        <v>47612</v>
+        <v>47825</v>
       </c>
       <c r="H19" t="n">
-        <v>-1313</v>
+        <v>-96</v>
       </c>
       <c r="I19" t="n">
-        <v>-1029</v>
+        <v>213</v>
       </c>
       <c r="J19" t="n">
-        <v>-21858</v>
+        <v>-22167</v>
       </c>
       <c r="K19" t="n">
-        <v>-284</v>
+        <v>-309</v>
       </c>
       <c r="L19" t="n">
-        <v>689</v>
+        <v>596</v>
       </c>
       <c r="M19" t="n">
-        <v>-984</v>
+        <v>686</v>
       </c>
       <c r="N19" t="n">
-        <v>1673</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2021/12/01</t>
+          <t>2021/12/02</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>49411</v>
+        <v>48787</v>
       </c>
       <c r="C20" t="n">
-        <v>54693</v>
+        <v>52680</v>
       </c>
       <c r="D20" t="n">
-        <v>288</v>
+        <v>-624</v>
       </c>
       <c r="E20" t="n">
-        <v>-648</v>
+        <v>-2013</v>
       </c>
       <c r="F20" t="n">
-        <v>27067</v>
+        <v>25754</v>
       </c>
       <c r="G20" t="n">
-        <v>48641</v>
+        <v>47612</v>
       </c>
       <c r="H20" t="n">
-        <v>1251</v>
+        <v>-1313</v>
       </c>
       <c r="I20" t="n">
-        <v>1031</v>
+        <v>-1029</v>
       </c>
       <c r="J20" t="n">
-        <v>-21574</v>
+        <v>-21858</v>
       </c>
       <c r="K20" t="n">
-        <v>220</v>
+        <v>-284</v>
       </c>
       <c r="L20" t="n">
-        <v>-963</v>
+        <v>689</v>
       </c>
       <c r="M20" t="n">
-        <v>-1679</v>
+        <v>-984</v>
       </c>
       <c r="N20" t="n">
-        <v>716</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2021/11/30</t>
+          <t>2021/12/01</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>49123</v>
+        <v>49411</v>
       </c>
       <c r="C21" t="n">
-        <v>55341</v>
+        <v>54693</v>
       </c>
       <c r="D21" t="n">
-        <v>-1811</v>
+        <v>288</v>
       </c>
       <c r="E21" t="n">
-        <v>2137</v>
+        <v>-648</v>
       </c>
       <c r="F21" t="n">
-        <v>25816</v>
+        <v>27067</v>
       </c>
       <c r="G21" t="n">
-        <v>47610</v>
+        <v>48641</v>
       </c>
       <c r="H21" t="n">
-        <v>-1474</v>
+        <v>1251</v>
       </c>
       <c r="I21" t="n">
-        <v>1840</v>
+        <v>1031</v>
       </c>
       <c r="J21" t="n">
-        <v>-21794</v>
+        <v>-21574</v>
       </c>
       <c r="K21" t="n">
-        <v>-3314</v>
+        <v>220</v>
       </c>
       <c r="L21" t="n">
-        <v>-337</v>